<commit_message>
Fixed that Belanger typo
Sorry, Josee
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-ptfc-orl-041716.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-ptfc-orl-041716.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5292" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5292" uniqueCount="181">
   <si>
     <t>event</t>
   </si>
@@ -519,9 +519,6 @@
     <t>switch</t>
   </si>
   <si>
-    <t xml:space="preserve"> Belanger</t>
-  </si>
-  <si>
     <t>45+1</t>
   </si>
   <si>
@@ -786,8 +783,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -907,7 +906,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -927,6 +926,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -946,6 +946,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1278,7 +1279,7 @@
   <dimension ref="A1:T1539"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1965,7 +1966,7 @@
         <v>21</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>104</v>
@@ -1986,7 +1987,7 @@
         <v>21</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M13" s="9" t="s">
         <v>107</v>
@@ -2013,7 +2014,7 @@
         <v>21</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>108</v>
@@ -2034,7 +2035,7 @@
         <v>21</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M14" s="9" t="s">
         <v>111</v>
@@ -2059,7 +2060,7 @@
         <v>21</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>107</v>
@@ -2080,7 +2081,7 @@
         <v>21</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>114</v>
@@ -2195,7 +2196,7 @@
         <v>121</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>97</v>
@@ -2210,7 +2211,7 @@
         <v>121</v>
       </c>
       <c r="L18" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M18" s="13" t="s">
         <v>122</v>
@@ -2533,7 +2534,7 @@
         <v>121</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>136</v>
@@ -2548,7 +2549,7 @@
         <v>121</v>
       </c>
       <c r="L27" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M27" s="17"/>
       <c r="N27" s="3"/>
@@ -2569,7 +2570,7 @@
         <v>121</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>137</v>
@@ -2584,7 +2585,7 @@
         <v>121</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M28" s="17"/>
       <c r="N28" s="3"/>
@@ -2605,7 +2606,7 @@
         <v>121</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>138</v>
@@ -2620,7 +2621,7 @@
         <v>121</v>
       </c>
       <c r="L29" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
@@ -2831,7 +2832,7 @@
         <v>121</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F36" s="27" t="s">
         <v>118</v>
@@ -3737,7 +3738,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M63" s="27" t="s">
         <v>90</v>
@@ -3763,7 +3764,7 @@
         <v>121</v>
       </c>
       <c r="E64" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F64" s="27" t="s">
         <v>68</v>
@@ -3831,7 +3832,7 @@
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F66" s="27" t="s">
         <v>68</v>
@@ -3897,7 +3898,7 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F68" s="27" t="s">
         <v>75</v>
@@ -3963,7 +3964,7 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F70" s="27" t="s">
         <v>68</v>
@@ -4386,7 +4387,7 @@
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F83" s="27" t="s">
         <v>81</v>
@@ -4508,7 +4509,7 @@
         <v>121</v>
       </c>
       <c r="L86" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M86" s="27" t="s">
         <v>107</v>
@@ -4907,7 +4908,7 @@
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F98" s="27" t="s">
         <v>68</v>
@@ -5773,7 +5774,7 @@
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F124" s="27" t="s">
         <v>68</v>
@@ -7091,7 +7092,7 @@
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F164" s="27" t="s">
         <v>68</v>
@@ -7592,7 +7593,7 @@
         <v>121</v>
       </c>
       <c r="L178" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M178" s="27" t="s">
         <v>71</v>
@@ -7627,7 +7628,7 @@
       <c r="J179" s="1"/>
       <c r="K179" s="1"/>
       <c r="L179" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M179" s="27" t="s">
         <v>84</v>
@@ -8114,7 +8115,7 @@
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
       <c r="E193" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F193" s="27" t="s">
         <v>81</v>
@@ -9527,7 +9528,7 @@
       <c r="J235" s="1"/>
       <c r="K235" s="1"/>
       <c r="L235" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M235" s="27" t="s">
         <v>103</v>
@@ -11723,7 +11724,7 @@
       <c r="C302" s="1"/>
       <c r="D302" s="1"/>
       <c r="E302" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F302" s="27" t="s">
         <v>68</v>
@@ -13337,7 +13338,7 @@
       <c r="C350" s="1"/>
       <c r="D350" s="1"/>
       <c r="E350" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F350" s="27" t="s">
         <v>68</v>
@@ -14192,7 +14193,7 @@
       <c r="C375" s="1"/>
       <c r="D375" s="1"/>
       <c r="E375" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F375" s="27" t="s">
         <v>81</v>
@@ -14681,7 +14682,7 @@
         <v>121</v>
       </c>
       <c r="E390" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F390" s="27" t="s">
         <v>118</v>
@@ -14712,7 +14713,7 @@
       <c r="C391" s="1"/>
       <c r="D391" s="1"/>
       <c r="E391" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F391" s="27" t="s">
         <v>81</v>
@@ -14890,7 +14891,7 @@
         <v>121</v>
       </c>
       <c r="L396" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M396" s="27" t="s">
         <v>78</v>
@@ -15595,7 +15596,7 @@
       <c r="J417" s="1"/>
       <c r="K417" s="1"/>
       <c r="L417" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M417" s="27" t="s">
         <v>78</v>
@@ -16052,7 +16053,7 @@
       <c r="C431" s="1"/>
       <c r="D431" s="1"/>
       <c r="E431" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F431" s="27" t="s">
         <v>87</v>
@@ -16083,7 +16084,7 @@
       <c r="C432" s="1"/>
       <c r="D432" s="1"/>
       <c r="E432" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F432" s="27" t="s">
         <v>68</v>
@@ -16168,7 +16169,7 @@
         <v>121</v>
       </c>
       <c r="L434" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M434" s="27" t="s">
         <v>90</v>
@@ -16223,7 +16224,7 @@
         <v>121</v>
       </c>
       <c r="E436" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F436" s="27" t="s">
         <v>68</v>
@@ -16431,7 +16432,7 @@
         <v>121</v>
       </c>
       <c r="E442" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F442" s="27" t="s">
         <v>118</v>
@@ -16462,7 +16463,7 @@
       <c r="C443" s="1"/>
       <c r="D443" s="1"/>
       <c r="E443" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F443" s="27" t="s">
         <v>68</v>
@@ -17844,7 +17845,7 @@
       <c r="J484" s="1"/>
       <c r="K484" s="1"/>
       <c r="L484" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M484" s="27" t="s">
         <v>71</v>
@@ -18320,7 +18321,7 @@
         <v>121</v>
       </c>
       <c r="E499" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F499" s="27" t="s">
         <v>68</v>
@@ -19928,7 +19929,7 @@
       <c r="C547" s="1"/>
       <c r="D547" s="1"/>
       <c r="E547" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F547" s="27" t="s">
         <v>68</v>
@@ -19990,7 +19991,7 @@
       <c r="C549" s="1"/>
       <c r="D549" s="1"/>
       <c r="E549" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F549" s="27" t="s">
         <v>68</v>
@@ -20494,7 +20495,7 @@
       <c r="J564" s="1"/>
       <c r="K564" s="1"/>
       <c r="L564" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M564" s="27" t="s">
         <v>111</v>
@@ -20560,7 +20561,7 @@
       <c r="J566" s="1"/>
       <c r="K566" s="1"/>
       <c r="L566" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M566" s="27" t="s">
         <v>84</v>
@@ -21583,7 +21584,7 @@
       <c r="C596" s="1"/>
       <c r="D596" s="1"/>
       <c r="E596" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F596" s="27" t="s">
         <v>75</v>
@@ -22815,7 +22816,7 @@
       <c r="C632" s="1"/>
       <c r="D632" s="1"/>
       <c r="E632" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F632" s="27" t="s">
         <v>68</v>
@@ -22881,7 +22882,7 @@
       <c r="C634" s="1"/>
       <c r="D634" s="1"/>
       <c r="E634" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F634" s="27" t="s">
         <v>104</v>
@@ -22916,7 +22917,7 @@
       <c r="C635" s="1"/>
       <c r="D635" s="1"/>
       <c r="E635" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F635" s="27" t="s">
         <v>118</v>
@@ -23130,7 +23131,7 @@
       <c r="C641" s="1"/>
       <c r="D641" s="1"/>
       <c r="E641" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F641" s="27" t="s">
         <v>81</v>
@@ -23196,7 +23197,7 @@
       <c r="C643" s="1"/>
       <c r="D643" s="1"/>
       <c r="E643" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F643" s="27" t="s">
         <v>87</v>
@@ -23227,7 +23228,7 @@
       <c r="C644" s="1"/>
       <c r="D644" s="1"/>
       <c r="E644" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F644" s="27" t="s">
         <v>68</v>
@@ -23460,7 +23461,7 @@
       <c r="J650" s="1"/>
       <c r="K650" s="1"/>
       <c r="L650" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M650" s="27" t="s">
         <v>90</v>
@@ -23486,7 +23487,7 @@
         <v>121</v>
       </c>
       <c r="E651" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F651" s="27" t="s">
         <v>75</v>
@@ -23954,7 +23955,7 @@
       <c r="C665" s="1"/>
       <c r="D665" s="1"/>
       <c r="E665" s="26" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F665" s="27" t="s">
         <v>162</v>
@@ -24362,7 +24363,7 @@
       <c r="C677" s="1"/>
       <c r="D677" s="1"/>
       <c r="E677" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F677" s="27" t="s">
         <v>87</v>
@@ -24393,7 +24394,7 @@
       <c r="C678" s="1"/>
       <c r="D678" s="1"/>
       <c r="E678" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F678" s="27" t="s">
         <v>87</v>
@@ -24424,7 +24425,7 @@
       <c r="C679" s="1"/>
       <c r="D679" s="1"/>
       <c r="E679" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F679" s="27" t="s">
         <v>104</v>
@@ -26664,7 +26665,7 @@
       <c r="C745" s="1"/>
       <c r="D745" s="1"/>
       <c r="E745" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F745" s="27" t="s">
         <v>68</v>
@@ -26842,7 +26843,7 @@
       <c r="J750" s="1"/>
       <c r="K750" s="1"/>
       <c r="L750" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M750" s="27" t="s">
         <v>111</v>
@@ -27724,7 +27725,7 @@
         <v>121</v>
       </c>
       <c r="L776" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M776" s="27" t="s">
         <v>90</v>
@@ -27750,7 +27751,7 @@
         <v>121</v>
       </c>
       <c r="E777" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F777" s="27" t="s">
         <v>68</v>
@@ -27857,7 +27858,7 @@
       <c r="C780" s="1"/>
       <c r="D780" s="1"/>
       <c r="E780" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F780" s="27" t="s">
         <v>75</v>
@@ -27919,7 +27920,7 @@
       <c r="C782" s="1"/>
       <c r="D782" s="1"/>
       <c r="E782" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F782" s="27" t="s">
         <v>93</v>
@@ -27954,7 +27955,7 @@
       <c r="C783" s="1"/>
       <c r="D783" s="1"/>
       <c r="E783" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F783" s="27" t="s">
         <v>87</v>
@@ -27985,7 +27986,7 @@
       <c r="C784" s="1"/>
       <c r="D784" s="1"/>
       <c r="E784" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F784" s="27" t="s">
         <v>68</v>
@@ -28689,7 +28690,7 @@
         <v>745</v>
       </c>
       <c r="B805" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C805" s="26"/>
       <c r="D805" s="26"/>
@@ -28718,7 +28719,7 @@
         <v>746</v>
       </c>
       <c r="B806" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C806" s="26"/>
       <c r="D806" s="26"/>
@@ -28747,7 +28748,7 @@
         <v>747</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C807" s="1"/>
       <c r="D807" s="26" t="s">
@@ -28782,7 +28783,7 @@
         <v>748</v>
       </c>
       <c r="B808" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C808" s="1"/>
       <c r="D808" s="1"/>
@@ -28819,7 +28820,7 @@
         <v>749</v>
       </c>
       <c r="B809" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C809" s="1"/>
       <c r="D809" s="26" t="s">
@@ -28852,7 +28853,7 @@
         <v>750</v>
       </c>
       <c r="B810" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C810" s="1"/>
       <c r="D810" s="1"/>
@@ -28883,7 +28884,7 @@
         <v>751</v>
       </c>
       <c r="B811" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C811" s="1"/>
       <c r="D811" s="1"/>
@@ -28918,7 +28919,7 @@
         <v>752</v>
       </c>
       <c r="B812" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C812" s="1"/>
       <c r="D812" s="1"/>
@@ -28949,7 +28950,7 @@
         <v>753</v>
       </c>
       <c r="B813" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C813" s="1"/>
       <c r="D813" s="1"/>
@@ -28980,7 +28981,7 @@
         <v>754</v>
       </c>
       <c r="B814" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C814" s="1"/>
       <c r="D814" s="1"/>
@@ -29015,7 +29016,7 @@
         <v>755</v>
       </c>
       <c r="B815" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C815" s="1"/>
       <c r="D815" s="26" t="s">
@@ -29052,7 +29053,7 @@
         <v>756</v>
       </c>
       <c r="B816" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C816" s="1"/>
       <c r="D816" s="1"/>
@@ -29083,7 +29084,7 @@
         <v>757</v>
       </c>
       <c r="B817" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C817" s="1"/>
       <c r="D817" s="1"/>
@@ -29512,7 +29513,7 @@
       </c>
       <c r="C830" s="29"/>
       <c r="D830" s="29"/>
-      <c r="E830" s="29" t="s">
+      <c r="E830" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F830" s="30" t="s">
@@ -29593,7 +29594,7 @@
       </c>
       <c r="J832" s="29"/>
       <c r="K832" s="29"/>
-      <c r="L832" s="29" t="s">
+      <c r="L832" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M832" s="30" t="s">
@@ -29684,7 +29685,7 @@
       <c r="C835" s="29"/>
       <c r="D835" s="29"/>
       <c r="E835" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F835" s="30" t="s">
         <v>87</v>
@@ -29715,7 +29716,7 @@
       <c r="C836" s="29"/>
       <c r="D836" s="29"/>
       <c r="E836" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F836" s="30" t="s">
         <v>68</v>
@@ -29777,7 +29778,7 @@
       <c r="C838" s="29"/>
       <c r="D838" s="29"/>
       <c r="E838" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F838" s="30" t="s">
         <v>75</v>
@@ -29839,7 +29840,7 @@
       <c r="C840" s="29"/>
       <c r="D840" s="29"/>
       <c r="E840" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F840" s="30" t="s">
         <v>87</v>
@@ -29874,7 +29875,7 @@
       <c r="C841" s="29"/>
       <c r="D841" s="29"/>
       <c r="E841" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F841" s="30" t="s">
         <v>81</v>
@@ -29975,7 +29976,7 @@
       <c r="C844" s="29"/>
       <c r="D844" s="29"/>
       <c r="E844" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F844" s="30" t="s">
         <v>68</v>
@@ -30411,7 +30412,7 @@
       <c r="J857" s="29"/>
       <c r="K857" s="29"/>
       <c r="L857" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M857" s="30" t="s">
         <v>111</v>
@@ -30477,7 +30478,7 @@
       <c r="J859" s="29"/>
       <c r="K859" s="29"/>
       <c r="L859" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M859" s="30" t="s">
         <v>71</v>
@@ -30602,7 +30603,7 @@
       <c r="C863" s="29"/>
       <c r="D863" s="29"/>
       <c r="E863" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F863" s="30" t="s">
         <v>68</v>
@@ -30685,7 +30686,7 @@
       <c r="J865" s="29"/>
       <c r="K865" s="29"/>
       <c r="L865" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M865" s="30" t="s">
         <v>90</v>
@@ -30738,7 +30739,7 @@
       <c r="C867" s="29"/>
       <c r="D867" s="29"/>
       <c r="E867" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F867" s="30" t="s">
         <v>81</v>
@@ -31316,7 +31317,7 @@
       </c>
       <c r="C884" s="29"/>
       <c r="D884" s="29"/>
-      <c r="E884" s="29" t="s">
+      <c r="E884" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F884" s="30" t="s">
@@ -31382,7 +31383,7 @@
       </c>
       <c r="C886" s="29"/>
       <c r="D886" s="29"/>
-      <c r="E886" s="29" t="s">
+      <c r="E886" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F886" s="30" t="s">
@@ -31413,7 +31414,7 @@
       </c>
       <c r="C887" s="29"/>
       <c r="D887" s="29"/>
-      <c r="E887" s="29" t="s">
+      <c r="E887" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F887" s="30" t="s">
@@ -31449,7 +31450,7 @@
       <c r="C888" s="29"/>
       <c r="D888" s="29"/>
       <c r="E888" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F888" s="30" t="s">
         <v>68</v>
@@ -31814,7 +31815,7 @@
       </c>
       <c r="J899" s="29"/>
       <c r="K899" s="29"/>
-      <c r="L899" s="29" t="s">
+      <c r="L899" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M899" s="30" t="s">
@@ -32038,7 +32039,7 @@
       </c>
       <c r="C906" s="29"/>
       <c r="D906" s="29"/>
-      <c r="E906" s="29" t="s">
+      <c r="E906" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F906" s="30" t="s">
@@ -32469,7 +32470,7 @@
       </c>
       <c r="C919" s="29"/>
       <c r="D919" s="29"/>
-      <c r="E919" s="29" t="s">
+      <c r="E919" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F919" s="30" t="s">
@@ -32802,7 +32803,7 @@
       <c r="I929" s="30"/>
       <c r="J929" s="29"/>
       <c r="K929" s="29"/>
-      <c r="L929" s="29" t="s">
+      <c r="L929" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M929" s="30" t="s">
@@ -33262,7 +33263,7 @@
       <c r="C943" s="29"/>
       <c r="D943" s="29"/>
       <c r="E943" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F943" s="30" t="s">
         <v>75</v>
@@ -33493,7 +33494,7 @@
       <c r="C950" s="29"/>
       <c r="D950" s="29"/>
       <c r="E950" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F950" s="30" t="s">
         <v>68</v>
@@ -33627,7 +33628,7 @@
       <c r="C954" s="29"/>
       <c r="D954" s="29"/>
       <c r="E954" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F954" s="30" t="s">
         <v>118</v>
@@ -33658,7 +33659,7 @@
       <c r="C955" s="29"/>
       <c r="D955" s="29"/>
       <c r="E955" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F955" s="30" t="s">
         <v>68</v>
@@ -34027,7 +34028,7 @@
       <c r="I966" s="30"/>
       <c r="J966" s="29"/>
       <c r="K966" s="29"/>
-      <c r="L966" s="29" t="s">
+      <c r="L966" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M966" s="30" t="s">
@@ -34051,7 +34052,7 @@
       </c>
       <c r="C967" s="29"/>
       <c r="D967" s="29"/>
-      <c r="E967" s="29" t="s">
+      <c r="E967" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F967" s="30" t="s">
@@ -34082,7 +34083,7 @@
       </c>
       <c r="C968" s="29"/>
       <c r="D968" s="29"/>
-      <c r="E968" s="29" t="s">
+      <c r="E968" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F968" s="30" t="s">
@@ -34223,7 +34224,7 @@
       <c r="C972" s="29"/>
       <c r="D972" s="29"/>
       <c r="E972" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F972" s="30" t="s">
         <v>118</v>
@@ -34254,7 +34255,7 @@
       <c r="C973" s="29"/>
       <c r="D973" s="29"/>
       <c r="E973" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F973" s="30" t="s">
         <v>68</v>
@@ -34423,7 +34424,7 @@
       <c r="C978" s="29"/>
       <c r="D978" s="29"/>
       <c r="E978" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F978" s="30" t="s">
         <v>81</v>
@@ -34485,7 +34486,7 @@
       <c r="C980" s="29"/>
       <c r="D980" s="29"/>
       <c r="E980" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F980" s="30" t="s">
         <v>68</v>
@@ -34612,7 +34613,7 @@
       </c>
       <c r="C984" s="29"/>
       <c r="D984" s="29"/>
-      <c r="E984" s="29" t="s">
+      <c r="E984" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F984" s="30" t="s">
@@ -34973,7 +34974,7 @@
       </c>
       <c r="C995" s="29"/>
       <c r="D995" s="29"/>
-      <c r="E995" s="29" t="s">
+      <c r="E995" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F995" s="30" t="s">
@@ -35369,7 +35370,7 @@
       </c>
       <c r="C1007" s="29"/>
       <c r="D1007" s="29"/>
-      <c r="E1007" s="29" t="s">
+      <c r="E1007" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1007" s="30" t="s">
@@ -35405,7 +35406,7 @@
       <c r="C1008" s="29"/>
       <c r="D1008" s="29"/>
       <c r="E1008" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1008" s="30" t="s">
         <v>68</v>
@@ -35647,7 +35648,7 @@
       <c r="J1015" s="29"/>
       <c r="K1015" s="29"/>
       <c r="L1015" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1015" s="30" t="s">
         <v>78</v>
@@ -35682,7 +35683,7 @@
       <c r="J1016" s="29"/>
       <c r="K1016" s="29"/>
       <c r="L1016" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1016" s="30" t="s">
         <v>71</v>
@@ -35894,7 +35895,7 @@
       <c r="J1022" s="29"/>
       <c r="K1022" s="29"/>
       <c r="L1022" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1022" s="30" t="s">
         <v>84</v>
@@ -36685,7 +36686,7 @@
       <c r="C1046" s="29"/>
       <c r="D1046" s="29"/>
       <c r="E1046" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1046" s="30" t="s">
         <v>130</v>
@@ -36749,7 +36750,7 @@
       <c r="C1048" s="29"/>
       <c r="D1048" s="29"/>
       <c r="E1048" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1048" s="30" t="s">
         <v>68</v>
@@ -37254,7 +37255,7 @@
       <c r="I1063" s="30"/>
       <c r="J1063" s="29"/>
       <c r="K1063" s="29"/>
-      <c r="L1063" s="29" t="s">
+      <c r="L1063" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1063" s="30" t="s">
@@ -37378,7 +37379,7 @@
       <c r="C1067" s="29"/>
       <c r="D1067" s="29"/>
       <c r="E1067" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1067" s="30" t="s">
         <v>130</v>
@@ -37584,7 +37585,7 @@
       </c>
       <c r="J1073" s="29"/>
       <c r="K1073" s="29"/>
-      <c r="L1073" s="29" t="s">
+      <c r="L1073" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1073" s="30" t="s">
@@ -37749,7 +37750,7 @@
       </c>
       <c r="J1078" s="29"/>
       <c r="K1078" s="29"/>
-      <c r="L1078" s="29" t="s">
+      <c r="L1078" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1078" s="30" t="s">
@@ -37822,7 +37823,7 @@
       <c r="J1080" s="29"/>
       <c r="K1080" s="29"/>
       <c r="L1080" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1080" s="30" t="s">
         <v>71</v>
@@ -38121,7 +38122,7 @@
       <c r="J1089" s="29"/>
       <c r="K1089" s="29"/>
       <c r="L1089" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1089" s="30" t="s">
         <v>71</v>
@@ -38415,7 +38416,7 @@
       <c r="C1098" s="29"/>
       <c r="D1098" s="29"/>
       <c r="E1098" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1098" s="30" t="s">
         <v>68</v>
@@ -38720,7 +38721,7 @@
       <c r="C1107" s="29"/>
       <c r="D1107" s="29"/>
       <c r="E1107" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1107" s="30" t="s">
         <v>107</v>
@@ -38898,7 +38899,7 @@
       <c r="J1112" s="29"/>
       <c r="K1112" s="29"/>
       <c r="L1112" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1112" s="30" t="s">
         <v>111</v>
@@ -38922,7 +38923,7 @@
       <c r="C1113" s="29"/>
       <c r="D1113" s="29"/>
       <c r="E1113" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1113" s="30" t="s">
         <v>118</v>
@@ -38957,7 +38958,7 @@
       <c r="C1114" s="29"/>
       <c r="D1114" s="29"/>
       <c r="E1114" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1114" s="30" t="s">
         <v>81</v>
@@ -39089,7 +39090,7 @@
       <c r="C1118" s="29"/>
       <c r="D1118" s="29"/>
       <c r="E1118" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1118" s="30" t="s">
         <v>68</v>
@@ -39253,7 +39254,7 @@
       </c>
       <c r="C1123" s="29"/>
       <c r="D1123" s="29"/>
-      <c r="E1123" s="29" t="s">
+      <c r="E1123" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1123" s="30" t="s">
@@ -39363,7 +39364,7 @@
       <c r="I1126" s="30"/>
       <c r="J1126" s="29"/>
       <c r="K1126" s="29"/>
-      <c r="L1126" s="29" t="s">
+      <c r="L1126" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1126" s="30" t="s">
@@ -39388,7 +39389,7 @@
       <c r="C1127" s="29"/>
       <c r="D1127" s="29"/>
       <c r="E1127" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1127" s="30" t="s">
         <v>118</v>
@@ -39419,7 +39420,7 @@
       <c r="C1128" s="29"/>
       <c r="D1128" s="29"/>
       <c r="E1128" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1128" s="30" t="s">
         <v>68</v>
@@ -39823,7 +39824,7 @@
       <c r="C1140" s="29"/>
       <c r="D1140" s="29"/>
       <c r="E1140" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1140" s="30" t="s">
         <v>68</v>
@@ -39949,7 +39950,7 @@
       <c r="C1144" s="29"/>
       <c r="D1144" s="29"/>
       <c r="E1144" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1144" s="30" t="s">
         <v>107</v>
@@ -39983,7 +39984,7 @@
       </c>
       <c r="C1145" s="29"/>
       <c r="D1145" s="29"/>
-      <c r="E1145" s="29" t="s">
+      <c r="E1145" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1145" s="30" t="s">
@@ -40018,7 +40019,7 @@
       </c>
       <c r="C1146" s="29"/>
       <c r="D1146" s="29"/>
-      <c r="E1146" s="29" t="s">
+      <c r="E1146" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1146" s="30" t="s">
@@ -40049,7 +40050,7 @@
       </c>
       <c r="C1147" s="29"/>
       <c r="D1147" s="29"/>
-      <c r="E1147" s="29" t="s">
+      <c r="E1147" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1147" s="30" t="s">
@@ -40221,7 +40222,7 @@
       <c r="C1152" s="29"/>
       <c r="D1152" s="29"/>
       <c r="E1152" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1152" s="30" t="s">
         <v>75</v>
@@ -40464,7 +40465,7 @@
       <c r="I1159" s="30"/>
       <c r="J1159" s="29"/>
       <c r="K1159" s="29"/>
-      <c r="L1159" s="29" t="s">
+      <c r="L1159" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1159" s="30" t="s">
@@ -40654,7 +40655,7 @@
       <c r="C1165" s="29"/>
       <c r="D1165" s="29"/>
       <c r="E1165" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1165" s="30" t="s">
         <v>81</v>
@@ -40751,7 +40752,7 @@
       <c r="C1168" s="29"/>
       <c r="D1168" s="29"/>
       <c r="E1168" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1168" s="30" t="s">
         <v>68</v>
@@ -41118,7 +41119,7 @@
       <c r="C1179" s="29"/>
       <c r="D1179" s="29"/>
       <c r="E1179" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1179" s="30" t="s">
         <v>118</v>
@@ -41153,7 +41154,7 @@
       <c r="C1180" s="29"/>
       <c r="D1180" s="29"/>
       <c r="E1180" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1180" s="30" t="s">
         <v>68</v>
@@ -41218,7 +41219,7 @@
       </c>
       <c r="C1182" s="29"/>
       <c r="D1182" s="29"/>
-      <c r="E1182" s="29" t="s">
+      <c r="E1182" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1182" s="30" t="s">
@@ -41253,7 +41254,7 @@
       </c>
       <c r="C1183" s="29"/>
       <c r="D1183" s="29"/>
-      <c r="E1183" s="29" t="s">
+      <c r="E1183" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1183" s="30" t="s">
@@ -41526,7 +41527,7 @@
       <c r="C1191" s="29"/>
       <c r="D1191" s="29"/>
       <c r="E1191" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1191" s="30" t="s">
         <v>81</v>
@@ -41753,7 +41754,7 @@
       <c r="C1198" s="29"/>
       <c r="D1198" s="29"/>
       <c r="E1198" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1198" s="30" t="s">
         <v>118</v>
@@ -41784,7 +41785,7 @@
       <c r="C1199" s="29"/>
       <c r="D1199" s="29"/>
       <c r="E1199" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1199" s="30" t="s">
         <v>68</v>
@@ -41977,7 +41978,7 @@
         <v>141</v>
       </c>
       <c r="F1205" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G1205" s="30" t="s">
         <v>51</v>
@@ -42092,7 +42093,7 @@
       <c r="J1208" s="29"/>
       <c r="K1208" s="29"/>
       <c r="L1208" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1208" s="30" t="s">
         <v>78</v>
@@ -42127,7 +42128,7 @@
       <c r="J1209" s="29"/>
       <c r="K1209" s="29"/>
       <c r="L1209" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1209" s="30" t="s">
         <v>78</v>
@@ -42655,7 +42656,7 @@
       <c r="J1225" s="29"/>
       <c r="K1225" s="29"/>
       <c r="L1225" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1225" s="30" t="s">
         <v>71</v>
@@ -42690,7 +42691,7 @@
       <c r="J1226" s="29"/>
       <c r="K1226" s="29"/>
       <c r="L1226" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1226" s="30" t="s">
         <v>71</v>
@@ -42912,7 +42913,7 @@
       <c r="C1233" s="29"/>
       <c r="D1233" s="29"/>
       <c r="E1233" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1233" s="30" t="s">
         <v>130</v>
@@ -42976,7 +42977,7 @@
       <c r="C1235" s="29"/>
       <c r="D1235" s="29"/>
       <c r="E1235" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1235" s="30" t="s">
         <v>111</v>
@@ -42987,7 +42988,7 @@
       <c r="J1235" s="29"/>
       <c r="K1235" s="29"/>
       <c r="L1235" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1235" s="30" t="s">
         <v>107</v>
@@ -43011,7 +43012,7 @@
       <c r="C1236" s="29"/>
       <c r="D1236" s="29"/>
       <c r="E1236" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1236" s="30" t="s">
         <v>118</v>
@@ -43042,7 +43043,7 @@
       <c r="C1237" s="29"/>
       <c r="D1237" s="29"/>
       <c r="E1237" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1237" s="30" t="s">
         <v>68</v>
@@ -43178,7 +43179,7 @@
       <c r="C1241" s="29"/>
       <c r="D1241" s="29"/>
       <c r="E1241" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1241" s="30" t="s">
         <v>111</v>
@@ -43349,7 +43350,7 @@
       <c r="C1246" s="29"/>
       <c r="D1246" s="29"/>
       <c r="E1246" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1246" s="30" t="s">
         <v>75</v>
@@ -43393,7 +43394,7 @@
       <c r="J1247" s="29"/>
       <c r="K1247" s="29"/>
       <c r="L1247" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1247" s="30" t="s">
         <v>71</v>
@@ -43459,7 +43460,7 @@
       <c r="J1249" s="29"/>
       <c r="K1249" s="29"/>
       <c r="L1249" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1249" s="30" t="s">
         <v>71</v>
@@ -43521,7 +43522,7 @@
       <c r="J1251" s="29"/>
       <c r="K1251" s="29"/>
       <c r="L1251" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1251" s="30" t="s">
         <v>84</v>
@@ -43791,7 +43792,7 @@
       <c r="J1259" s="29"/>
       <c r="K1259" s="29"/>
       <c r="L1259" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1259" s="30" t="s">
         <v>90</v>
@@ -43844,7 +43845,7 @@
       <c r="C1261" s="29"/>
       <c r="D1261" s="29"/>
       <c r="E1261" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1261" s="30" t="s">
         <v>68</v>
@@ -43855,7 +43856,7 @@
       <c r="J1261" s="29"/>
       <c r="K1261" s="29"/>
       <c r="L1261" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1261" s="30" t="s">
         <v>71</v>
@@ -43890,7 +43891,7 @@
       <c r="J1262" s="29"/>
       <c r="K1262" s="29"/>
       <c r="L1262" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1262" s="30" t="s">
         <v>71</v>
@@ -43925,7 +43926,7 @@
       <c r="J1263" s="29"/>
       <c r="K1263" s="29"/>
       <c r="L1263" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1263" s="30" t="s">
         <v>71</v>
@@ -43960,7 +43961,7 @@
       <c r="J1264" s="29"/>
       <c r="K1264" s="29"/>
       <c r="L1264" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1264" s="30" t="s">
         <v>78</v>
@@ -44018,7 +44019,7 @@
       </c>
       <c r="C1266" s="29"/>
       <c r="D1266" s="29"/>
-      <c r="E1266" s="29" t="s">
+      <c r="E1266" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1266" s="30" t="s">
@@ -44221,7 +44222,7 @@
       <c r="C1272" s="29"/>
       <c r="D1272" s="29"/>
       <c r="E1272" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1272" s="30" t="s">
         <v>118</v>
@@ -44252,7 +44253,7 @@
       <c r="C1273" s="29"/>
       <c r="D1273" s="29"/>
       <c r="E1273" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1273" s="30" t="s">
         <v>68</v>
@@ -44320,7 +44321,7 @@
       <c r="C1275" s="29"/>
       <c r="D1275" s="29"/>
       <c r="E1275" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1275" s="30" t="s">
         <v>87</v>
@@ -44351,7 +44352,7 @@
       <c r="C1276" s="29"/>
       <c r="D1276" s="29"/>
       <c r="E1276" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1276" s="30" t="s">
         <v>68</v>
@@ -44434,7 +44435,7 @@
       <c r="J1278" s="29"/>
       <c r="K1278" s="29"/>
       <c r="L1278" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1278" s="30"/>
       <c r="N1278" s="30"/>
@@ -44458,7 +44459,7 @@
       <c r="C1279" s="29"/>
       <c r="D1279" s="29"/>
       <c r="E1279" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1279" s="30" t="s">
         <v>75</v>
@@ -44729,7 +44730,7 @@
       <c r="J1287" s="29"/>
       <c r="K1287" s="29"/>
       <c r="L1287" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1287" s="30" t="s">
         <v>71</v>
@@ -44764,7 +44765,7 @@
       <c r="J1288" s="29"/>
       <c r="K1288" s="29"/>
       <c r="L1288" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1288" s="30" t="s">
         <v>71</v>
@@ -45151,7 +45152,7 @@
       <c r="C1300" s="29"/>
       <c r="D1300" s="29"/>
       <c r="E1300" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1300" s="30" t="s">
         <v>118</v>
@@ -45182,7 +45183,7 @@
       <c r="C1301" s="29"/>
       <c r="D1301" s="29"/>
       <c r="E1301" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1301" s="30" t="s">
         <v>103</v>
@@ -45275,7 +45276,7 @@
       <c r="C1304" s="29"/>
       <c r="D1304" s="29"/>
       <c r="E1304" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1304" s="30" t="s">
         <v>100</v>
@@ -45286,7 +45287,7 @@
       <c r="J1304" s="29"/>
       <c r="K1304" s="29"/>
       <c r="L1304" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1304" s="30" t="s">
         <v>35</v>
@@ -45352,7 +45353,7 @@
       <c r="J1306" s="29"/>
       <c r="K1306" s="29"/>
       <c r="L1306" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1306" s="30" t="s">
         <v>71</v>
@@ -45422,7 +45423,7 @@
       <c r="J1308" s="29"/>
       <c r="K1308" s="29"/>
       <c r="L1308" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1308" s="30" t="s">
         <v>71</v>
@@ -45477,7 +45478,7 @@
       <c r="C1310" s="29"/>
       <c r="D1310" s="29"/>
       <c r="E1310" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1310" s="30" t="s">
         <v>68</v>
@@ -45488,7 +45489,7 @@
       <c r="J1310" s="29"/>
       <c r="K1310" s="29"/>
       <c r="L1310" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1310" s="30" t="s">
         <v>71</v>
@@ -45543,7 +45544,7 @@
       <c r="C1312" s="29"/>
       <c r="D1312" s="29"/>
       <c r="E1312" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1312" s="30" t="s">
         <v>68</v>
@@ -45591,7 +45592,7 @@
       <c r="J1313" s="29"/>
       <c r="K1313" s="29"/>
       <c r="L1313" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1313" s="30" t="s">
         <v>71</v>
@@ -45879,7 +45880,7 @@
       <c r="I1322" s="30"/>
       <c r="J1322" s="29"/>
       <c r="K1322" s="29"/>
-      <c r="L1322" s="29" t="s">
+      <c r="L1322" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1322" s="30" t="s">
@@ -45903,7 +45904,7 @@
       </c>
       <c r="C1323" s="29"/>
       <c r="D1323" s="29"/>
-      <c r="E1323" s="29" t="s">
+      <c r="E1323" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1323" s="30" t="s">
@@ -45938,7 +45939,7 @@
       </c>
       <c r="C1324" s="29"/>
       <c r="D1324" s="29"/>
-      <c r="E1324" s="29" t="s">
+      <c r="E1324" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1324" s="30" t="s">
@@ -46015,7 +46016,7 @@
       <c r="I1326" s="30"/>
       <c r="J1326" s="29"/>
       <c r="K1326" s="29"/>
-      <c r="L1326" s="29" t="s">
+      <c r="L1326" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1326" s="30" t="s">
@@ -46083,7 +46084,7 @@
       </c>
       <c r="J1328" s="29"/>
       <c r="K1328" s="29"/>
-      <c r="L1328" s="29" t="s">
+      <c r="L1328" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1328" s="30" t="s">
@@ -46119,7 +46120,7 @@
       <c r="J1329" s="29"/>
       <c r="K1329" s="29"/>
       <c r="L1329" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1329" s="30" t="s">
         <v>111</v>
@@ -46207,7 +46208,7 @@
       <c r="C1332" s="29"/>
       <c r="D1332" s="29"/>
       <c r="E1332" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1332" s="30" t="s">
         <v>107</v>
@@ -46345,7 +46346,7 @@
       <c r="C1336" s="29"/>
       <c r="D1336" s="29"/>
       <c r="E1336" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1336" s="30" t="s">
         <v>75</v>
@@ -46477,7 +46478,7 @@
       <c r="C1340" s="29"/>
       <c r="D1340" s="29"/>
       <c r="E1340" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1340" s="30" t="s">
         <v>108</v>
@@ -46673,7 +46674,7 @@
       <c r="C1346" s="29"/>
       <c r="D1346" s="29"/>
       <c r="E1346" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1346" s="30"/>
       <c r="G1346" s="30"/>
@@ -46741,7 +46742,7 @@
       <c r="C1348" s="29"/>
       <c r="D1348" s="29"/>
       <c r="E1348" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1348" s="30" t="s">
         <v>68</v>
@@ -46813,7 +46814,7 @@
       <c r="C1350" s="29"/>
       <c r="D1350" s="29"/>
       <c r="E1350" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1350" s="30" t="s">
         <v>118</v>
@@ -46848,7 +46849,7 @@
       <c r="C1351" s="29"/>
       <c r="D1351" s="29"/>
       <c r="E1351" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1351" s="30" t="s">
         <v>104</v>
@@ -46894,7 +46895,7 @@
       <c r="J1352" s="29"/>
       <c r="K1352" s="29"/>
       <c r="L1352" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1352" s="30" t="s">
         <v>71</v>
@@ -46929,7 +46930,7 @@
       <c r="J1353" s="29"/>
       <c r="K1353" s="29"/>
       <c r="L1353" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1353" s="30" t="s">
         <v>71</v>
@@ -47539,7 +47540,7 @@
       <c r="J1371" s="29"/>
       <c r="K1371" s="29"/>
       <c r="L1371" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1371" s="30" t="s">
         <v>71</v>
@@ -47570,7 +47571,7 @@
       <c r="J1372" s="29"/>
       <c r="K1372" s="29"/>
       <c r="L1372" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1372" s="30" t="s">
         <v>84</v>
@@ -47691,7 +47692,7 @@
       <c r="C1376" s="29"/>
       <c r="D1376" s="29"/>
       <c r="E1376" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1376" s="30" t="s">
         <v>81</v>
@@ -47763,7 +47764,7 @@
       <c r="C1378" s="29"/>
       <c r="D1378" s="29"/>
       <c r="E1378" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1378" s="30" t="s">
         <v>75</v>
@@ -47969,7 +47970,7 @@
       <c r="C1384" s="29"/>
       <c r="D1384" s="29"/>
       <c r="E1384" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1384" s="30" t="s">
         <v>68</v>
@@ -48314,7 +48315,7 @@
       <c r="J1394" s="29"/>
       <c r="K1394" s="29"/>
       <c r="L1394" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1394" s="30" t="s">
         <v>84</v>
@@ -48668,7 +48669,7 @@
       <c r="I1405" s="30"/>
       <c r="J1405" s="29"/>
       <c r="K1405" s="29"/>
-      <c r="L1405" s="29" t="s">
+      <c r="L1405" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1405" s="30" t="s">
@@ -48774,7 +48775,7 @@
       <c r="J1408" s="29"/>
       <c r="K1408" s="29"/>
       <c r="L1408" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1408" s="30" t="s">
         <v>35</v>
@@ -48798,7 +48799,7 @@
       <c r="C1409" s="29"/>
       <c r="D1409" s="29"/>
       <c r="E1409" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1409" s="30" t="s">
         <v>75</v>
@@ -48811,7 +48812,7 @@
       <c r="J1409" s="29"/>
       <c r="K1409" s="29"/>
       <c r="L1409" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1409" s="30" t="s">
         <v>84</v>
@@ -48835,7 +48836,7 @@
       <c r="C1410" s="29"/>
       <c r="D1410" s="29"/>
       <c r="E1410" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1410" s="30" t="s">
         <v>118</v>
@@ -48870,7 +48871,7 @@
       <c r="C1411" s="29"/>
       <c r="D1411" s="29"/>
       <c r="E1411" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1411" s="30" t="s">
         <v>68</v>
@@ -49146,7 +49147,7 @@
       <c r="C1419" s="29"/>
       <c r="D1419" s="29"/>
       <c r="E1419" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1419" s="30" t="s">
         <v>68</v>
@@ -49247,7 +49248,7 @@
       <c r="C1422" s="29"/>
       <c r="D1422" s="29"/>
       <c r="E1422" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1422" s="30" t="s">
         <v>68</v>
@@ -49296,7 +49297,7 @@
       </c>
       <c r="J1423" s="29"/>
       <c r="K1423" s="29"/>
-      <c r="L1423" s="29" t="s">
+      <c r="L1423" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1423" s="30" t="s">
@@ -49397,7 +49398,7 @@
       </c>
       <c r="J1426" s="29"/>
       <c r="K1426" s="29"/>
-      <c r="L1426" s="29" t="s">
+      <c r="L1426" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1426" s="30" t="s">
@@ -49562,7 +49563,7 @@
       <c r="C1431" s="29"/>
       <c r="D1431" s="29"/>
       <c r="E1431" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1431" s="30" t="s">
         <v>68</v>
@@ -49641,7 +49642,7 @@
       <c r="J1433" s="29"/>
       <c r="K1433" s="29"/>
       <c r="L1433" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1433" s="30" t="s">
         <v>71</v>
@@ -49883,7 +49884,7 @@
       <c r="I1440" s="30"/>
       <c r="J1440" s="29"/>
       <c r="K1440" s="29"/>
-      <c r="L1440" s="29" t="s">
+      <c r="L1440" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1440" s="30" t="s">
@@ -49915,7 +49916,7 @@
       <c r="J1441" s="29"/>
       <c r="K1441" s="29"/>
       <c r="L1441" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1441" s="30" t="s">
         <v>84</v>
@@ -50035,7 +50036,7 @@
       </c>
       <c r="C1445" s="29"/>
       <c r="D1445" s="29"/>
-      <c r="E1445" s="29" t="s">
+      <c r="E1445" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1445" s="30" t="s">
@@ -50135,7 +50136,7 @@
       <c r="C1448" s="29"/>
       <c r="D1448" s="29"/>
       <c r="E1448" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F1448" s="30" t="s">
         <v>130</v>
@@ -50166,7 +50167,7 @@
       <c r="C1449" s="29"/>
       <c r="D1449" s="29"/>
       <c r="E1449" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1449" s="30" t="s">
         <v>75</v>
@@ -50228,7 +50229,7 @@
       <c r="C1451" s="29"/>
       <c r="D1451" s="29"/>
       <c r="E1451" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1451" s="30" t="s">
         <v>111</v>
@@ -50328,7 +50329,7 @@
       </c>
       <c r="C1454" s="29"/>
       <c r="D1454" s="29"/>
-      <c r="E1454" s="29" t="s">
+      <c r="E1454" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1454" s="30" t="s">
@@ -50342,7 +50343,7 @@
       <c r="J1454" s="29"/>
       <c r="K1454" s="29"/>
       <c r="L1454" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1454" s="30" t="s">
         <v>71</v>
@@ -50366,7 +50367,7 @@
       <c r="C1455" s="29"/>
       <c r="D1455" s="29"/>
       <c r="E1455" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F1455" s="30" t="s">
         <v>75</v>
@@ -50535,7 +50536,7 @@
       <c r="C1460" s="29"/>
       <c r="D1460" s="29"/>
       <c r="E1460" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1460" s="30" t="s">
         <v>68</v>
@@ -50603,7 +50604,7 @@
       <c r="C1462" s="29"/>
       <c r="D1462" s="29"/>
       <c r="E1462" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1462" s="30" t="s">
         <v>50</v>
@@ -50715,7 +50716,7 @@
       <c r="J1465" s="29"/>
       <c r="K1465" s="29"/>
       <c r="L1465" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1465" s="30" t="s">
         <v>107</v>
@@ -50739,7 +50740,7 @@
       <c r="C1466" s="29"/>
       <c r="D1466" s="29"/>
       <c r="E1466" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1466" s="30" t="s">
         <v>118</v>
@@ -50770,7 +50771,7 @@
       <c r="C1467" s="29"/>
       <c r="D1467" s="29"/>
       <c r="E1467" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1467" s="30" t="s">
         <v>68</v>
@@ -50873,7 +50874,7 @@
       <c r="C1470" s="29"/>
       <c r="D1470" s="29"/>
       <c r="E1470" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1470" s="30" t="s">
         <v>68</v>
@@ -50939,7 +50940,7 @@
       <c r="C1472" s="29"/>
       <c r="D1472" s="29"/>
       <c r="E1472" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1472" s="30" t="s">
         <v>68</v>
@@ -51073,7 +51074,7 @@
       <c r="C1476" s="29"/>
       <c r="D1476" s="29"/>
       <c r="E1476" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F1476" s="30" t="s">
         <v>130</v>
@@ -51150,7 +51151,7 @@
       <c r="J1478" s="29"/>
       <c r="K1478" s="29"/>
       <c r="L1478" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1478" s="30" t="s">
         <v>84</v>
@@ -51174,7 +51175,7 @@
       <c r="C1479" s="29"/>
       <c r="D1479" s="29"/>
       <c r="E1479" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1479" s="30" t="s">
         <v>118</v>
@@ -51209,7 +51210,7 @@
       <c r="C1480" s="29"/>
       <c r="D1480" s="29"/>
       <c r="E1480" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1480" s="30" t="s">
         <v>68</v>
@@ -51244,7 +51245,7 @@
       <c r="C1481" s="29"/>
       <c r="D1481" s="29"/>
       <c r="E1481" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F1481" s="30" t="s">
         <v>75</v>
@@ -51279,7 +51280,7 @@
       <c r="C1482" s="29"/>
       <c r="D1482" s="29"/>
       <c r="E1482" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F1482" s="30" t="s">
         <v>68</v>
@@ -51355,7 +51356,7 @@
       <c r="I1484" s="30"/>
       <c r="J1484" s="29"/>
       <c r="K1484" s="29"/>
-      <c r="L1484" s="29" t="s">
+      <c r="L1484" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1484" s="30" t="s">
@@ -51380,7 +51381,7 @@
       <c r="C1485" s="29"/>
       <c r="D1485" s="29"/>
       <c r="E1485" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1485" s="30" t="s">
         <v>118</v>
@@ -51411,7 +51412,7 @@
       <c r="C1486" s="29"/>
       <c r="D1486" s="29"/>
       <c r="E1486" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1486" s="30" t="s">
         <v>87</v>
@@ -51442,7 +51443,7 @@
       <c r="C1487" s="29"/>
       <c r="D1487" s="29"/>
       <c r="E1487" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1487" s="30" t="s">
         <v>87</v>
@@ -51452,7 +51453,7 @@
       <c r="I1487" s="30"/>
       <c r="J1487" s="29"/>
       <c r="K1487" s="29"/>
-      <c r="L1487" s="29" t="s">
+      <c r="L1487" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1487" s="30" t="s">
@@ -51477,7 +51478,7 @@
       <c r="C1488" s="29"/>
       <c r="D1488" s="29"/>
       <c r="E1488" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1488" s="30" t="s">
         <v>75</v>
@@ -51487,7 +51488,7 @@
       <c r="I1488" s="30"/>
       <c r="J1488" s="29"/>
       <c r="K1488" s="29"/>
-      <c r="L1488" s="29" t="s">
+      <c r="L1488" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1488" s="30" t="s">
@@ -51523,7 +51524,7 @@
       <c r="J1489" s="29"/>
       <c r="K1489" s="29"/>
       <c r="L1489" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1489" s="30" t="s">
         <v>71</v>
@@ -51710,7 +51711,7 @@
       <c r="C1495" s="29"/>
       <c r="D1495" s="29"/>
       <c r="E1495" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F1495" s="30" t="s">
         <v>81</v>
@@ -51861,7 +51862,7 @@
       <c r="J1499" s="29"/>
       <c r="K1499" s="29"/>
       <c r="L1499" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1499" s="30" t="s">
         <v>62</v>
@@ -51944,12 +51945,12 @@
         <v>1340</v>
       </c>
       <c r="B1502" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1502" s="29"/>
       <c r="D1502" s="29"/>
       <c r="E1502" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F1502" s="30" t="s">
         <v>68</v>
@@ -51977,7 +51978,7 @@
         <v>1341</v>
       </c>
       <c r="B1503" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1503" s="29"/>
       <c r="D1503" s="29"/>
@@ -52014,7 +52015,7 @@
         <v>1341</v>
       </c>
       <c r="B1504" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1504" s="29"/>
       <c r="D1504" s="29"/>
@@ -52045,7 +52046,7 @@
         <v>1342</v>
       </c>
       <c r="B1505" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1505" s="29"/>
       <c r="D1505" s="29"/>
@@ -52078,7 +52079,7 @@
         <v>1343</v>
       </c>
       <c r="B1506" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1506" s="29"/>
       <c r="D1506" s="29"/>
@@ -52113,7 +52114,7 @@
         <v>1344</v>
       </c>
       <c r="B1507" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1507" s="29"/>
       <c r="D1507" s="29"/>
@@ -52150,7 +52151,7 @@
         <v>1344</v>
       </c>
       <c r="B1508" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1508" s="29"/>
       <c r="D1508" s="29"/>
@@ -52181,12 +52182,12 @@
         <v>1345</v>
       </c>
       <c r="B1509" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1509" s="29"/>
       <c r="D1509" s="29"/>
       <c r="E1509" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1509" s="30" t="s">
         <v>81</v>
@@ -52214,7 +52215,7 @@
         <v>1345</v>
       </c>
       <c r="B1510" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1510" s="29"/>
       <c r="D1510" s="29"/>
@@ -52228,7 +52229,7 @@
       <c r="J1510" s="29"/>
       <c r="K1510" s="29"/>
       <c r="L1510" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1510" s="30"/>
       <c r="N1510" s="30"/>
@@ -52249,7 +52250,7 @@
         <v>1346</v>
       </c>
       <c r="B1511" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1511" s="29"/>
       <c r="D1511" s="29"/>
@@ -52278,12 +52279,12 @@
         <v>1347</v>
       </c>
       <c r="B1512" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1512" s="29"/>
       <c r="D1512" s="29"/>
       <c r="E1512" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1512" s="30" t="s">
         <v>81</v>
@@ -52309,7 +52310,7 @@
         <v>1348</v>
       </c>
       <c r="B1513" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1513" s="29"/>
       <c r="D1513" s="29"/>
@@ -52346,7 +52347,7 @@
         <v>1349</v>
       </c>
       <c r="B1514" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1514" s="29"/>
       <c r="D1514" s="29"/>
@@ -52377,7 +52378,7 @@
         <v>1350</v>
       </c>
       <c r="B1515" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1515" s="29"/>
       <c r="D1515" s="29"/>
@@ -52408,7 +52409,7 @@
         <v>1351</v>
       </c>
       <c r="B1516" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1516" s="29"/>
       <c r="D1516" s="29"/>
@@ -52443,7 +52444,7 @@
         <v>1352</v>
       </c>
       <c r="B1517" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1517" s="29"/>
       <c r="D1517" s="29"/>
@@ -52474,7 +52475,7 @@
         <v>1353</v>
       </c>
       <c r="B1518" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1518" s="29"/>
       <c r="D1518" s="29"/>
@@ -52513,7 +52514,7 @@
         <v>1354</v>
       </c>
       <c r="B1519" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1519" s="29"/>
       <c r="D1519" s="29"/>
@@ -52546,7 +52547,7 @@
         <v>1354</v>
       </c>
       <c r="B1520" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1520" s="29"/>
       <c r="D1520" s="29"/>
@@ -52575,7 +52576,7 @@
         <v>1355</v>
       </c>
       <c r="B1521" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1521" s="29"/>
       <c r="D1521" s="29"/>
@@ -52604,7 +52605,7 @@
         <v>1356</v>
       </c>
       <c r="B1522" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1522" s="29"/>
       <c r="D1522" s="29"/>
@@ -52637,7 +52638,7 @@
         <v>1357</v>
       </c>
       <c r="B1523" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1523" s="29"/>
       <c r="D1523" s="29"/>
@@ -52652,7 +52653,7 @@
       <c r="I1523" s="30"/>
       <c r="J1523" s="29"/>
       <c r="K1523" s="29"/>
-      <c r="L1523" s="29" t="s">
+      <c r="L1523" s="26" t="s">
         <v>153</v>
       </c>
       <c r="M1523" s="30" t="s">
@@ -52674,7 +52675,7 @@
         <v>1358</v>
       </c>
       <c r="B1524" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1524" s="29"/>
       <c r="D1524" s="29"/>
@@ -52709,12 +52710,12 @@
         <v>1359</v>
       </c>
       <c r="B1525" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1525" s="29"/>
       <c r="D1525" s="29"/>
       <c r="E1525" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F1525" s="30" t="s">
         <v>130</v>
@@ -52740,12 +52741,12 @@
         <v>1360</v>
       </c>
       <c r="B1526" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1526" s="29"/>
       <c r="D1526" s="29"/>
       <c r="E1526" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1526" s="30" t="s">
         <v>75</v>
@@ -52777,12 +52778,12 @@
         <v>1361</v>
       </c>
       <c r="B1527" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1527" s="29"/>
       <c r="D1527" s="29"/>
       <c r="E1527" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F1527" s="30" t="s">
         <v>118</v>
@@ -52808,12 +52809,12 @@
         <v>1362</v>
       </c>
       <c r="B1528" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1528" s="29"/>
       <c r="D1528" s="29"/>
       <c r="E1528" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F1528" s="30" t="s">
         <v>81</v>
@@ -52843,12 +52844,12 @@
         <v>1363</v>
       </c>
       <c r="B1529" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1529" s="29"/>
       <c r="D1529" s="29"/>
       <c r="E1529" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1529" s="30" t="s">
         <v>118</v>
@@ -52874,12 +52875,12 @@
         <v>1364</v>
       </c>
       <c r="B1530" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1530" s="29"/>
       <c r="D1530" s="29"/>
       <c r="E1530" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1530" s="30" t="s">
         <v>103</v>
@@ -52907,7 +52908,7 @@
         <v>1365</v>
       </c>
       <c r="B1531" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1531" s="29"/>
       <c r="D1531" s="29"/>
@@ -52940,7 +52941,7 @@
         <v>1366</v>
       </c>
       <c r="B1532" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1532" s="29"/>
       <c r="D1532" s="29"/>
@@ -52975,11 +52976,11 @@
         <v>1367</v>
       </c>
       <c r="B1533" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1533" s="29"/>
       <c r="D1533" s="29"/>
-      <c r="E1533" s="29" t="s">
+      <c r="E1533" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1533" s="30" t="s">
@@ -53006,11 +53007,11 @@
         <v>1368</v>
       </c>
       <c r="B1534" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1534" s="29"/>
       <c r="D1534" s="29"/>
-      <c r="E1534" s="29" t="s">
+      <c r="E1534" s="26" t="s">
         <v>153</v>
       </c>
       <c r="F1534" s="30" t="s">
@@ -53039,7 +53040,7 @@
         <v>1369</v>
       </c>
       <c r="B1535" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1535" s="29"/>
       <c r="D1535" s="29"/>
@@ -53072,7 +53073,7 @@
         <v>1370</v>
       </c>
       <c r="B1536" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1536" s="29"/>
       <c r="D1536" s="29"/>
@@ -53107,12 +53108,12 @@
         <v>1371</v>
       </c>
       <c r="B1537" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1537" s="29"/>
       <c r="D1537" s="29"/>
       <c r="E1537" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F1537" s="30" t="s">
         <v>108</v>
@@ -53138,7 +53139,7 @@
         <v>1372</v>
       </c>
       <c r="B1538" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1538" s="29"/>
       <c r="D1538" s="29"/>
@@ -53169,7 +53170,7 @@
         <v>1373</v>
       </c>
       <c r="B1539" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1539" s="29"/>
       <c r="D1539" s="29"/>
@@ -53193,6 +53194,7 @@
       <c r="T1539" s="30"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T1539"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added xG data to remaining Week 1 matches
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-ptfc-orl-041716.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-ptfc-orl-041716.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19580" yWindow="3300" windowWidth="29720" windowHeight="20980" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="340" windowWidth="16520" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">match!$A$1:$T$1539</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">match!$A$1:$U$1539</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5292" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5294" uniqueCount="183">
   <si>
     <t>event</t>
   </si>
@@ -566,6 +566,12 @@
   <si>
     <t>Hickmann Alves</t>
   </si>
+  <si>
+    <t>xG</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
@@ -618,7 +624,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,6 +683,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB6DDE8"/>
         <bgColor rgb="FFB6DDE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -826,7 +838,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -905,6 +917,9 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1276,10 +1291,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1539"/>
+  <dimension ref="A1:U1539"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A634" workbookViewId="0">
+      <pane xSplit="10" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E663" sqref="E663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1290,7 +1306,7 @@
     <col min="5" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="6.1640625" customWidth="1"/>
     <col min="8" max="8" width="7.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" customWidth="1"/>
     <col min="11" max="11" width="7" customWidth="1"/>
     <col min="12" max="12" width="11.1640625" customWidth="1"/>
@@ -1304,7 +1320,7 @@
     <col min="20" max="20" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="13.5" customHeight="1">
+    <row r="1" spans="1:21" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1365,8 +1381,11 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U1" s="36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="13.5" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1424,7 +1443,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="13.5" customHeight="1">
+    <row r="3" spans="1:21" ht="13.5" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
@@ -1482,7 +1501,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="13.5" customHeight="1">
+    <row r="4" spans="1:21" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
@@ -1540,7 +1559,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="13.5" customHeight="1">
+    <row r="5" spans="1:21" ht="13.5" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
@@ -1598,7 +1617,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="13.5" customHeight="1">
+    <row r="6" spans="1:21" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
@@ -1654,7 +1673,7 @@
       </c>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="13.5" customHeight="1">
+    <row r="7" spans="1:21" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -1708,7 +1727,7 @@
       </c>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="13.5" customHeight="1">
+    <row r="8" spans="1:21" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -1758,7 +1777,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" ht="13.5" customHeight="1">
+    <row r="9" spans="1:21" ht="13.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -1808,7 +1827,7 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="1:20" ht="13.5" customHeight="1">
+    <row r="10" spans="1:21" ht="13.5" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -1858,7 +1877,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="13.5" customHeight="1">
+    <row r="11" spans="1:21" ht="13.5" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="11" t="s">
@@ -1908,7 +1927,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="13.5" customHeight="1">
+    <row r="12" spans="1:21" ht="13.5" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
@@ -1956,7 +1975,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="13.5" customHeight="1">
+    <row r="13" spans="1:21" ht="13.5" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
@@ -2004,7 +2023,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="13.5" customHeight="1">
+    <row r="14" spans="1:21" ht="13.5" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -2050,7 +2069,7 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="13.5" customHeight="1">
+    <row r="15" spans="1:21" ht="13.5" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -2096,7 +2115,7 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="13.5" customHeight="1">
+    <row r="16" spans="1:21" ht="13.5" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="11" t="s">
@@ -5380,7 +5399,7 @@
       <c r="S112" s="17"/>
       <c r="T112" s="17"/>
     </row>
-    <row r="113" spans="1:20" ht="13.5" customHeight="1">
+    <row r="113" spans="1:21" ht="13.5" customHeight="1">
       <c r="A113" s="26">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -5417,7 +5436,7 @@
       <c r="S113" s="17"/>
       <c r="T113" s="17"/>
     </row>
-    <row r="114" spans="1:20" ht="13.5" customHeight="1">
+    <row r="114" spans="1:21" ht="13.5" customHeight="1">
       <c r="A114" s="26">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -5454,7 +5473,7 @@
       <c r="S114" s="17"/>
       <c r="T114" s="17"/>
     </row>
-    <row r="115" spans="1:20" ht="13.5" customHeight="1">
+    <row r="115" spans="1:21" ht="13.5" customHeight="1">
       <c r="A115" s="26">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -5485,7 +5504,7 @@
       <c r="S115" s="17"/>
       <c r="T115" s="17"/>
     </row>
-    <row r="116" spans="1:20" ht="13.5" customHeight="1">
+    <row r="116" spans="1:21" ht="13.5" customHeight="1">
       <c r="A116" s="26">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -5521,8 +5540,11 @@
       </c>
       <c r="S116" s="17"/>
       <c r="T116" s="17"/>
-    </row>
-    <row r="117" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U116" s="37">
+        <v>7.1179418849357107E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" ht="13.5" customHeight="1">
       <c r="A117" s="26">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -5559,7 +5581,7 @@
       <c r="S117" s="17"/>
       <c r="T117" s="17"/>
     </row>
-    <row r="118" spans="1:20" ht="13.5" customHeight="1">
+    <row r="118" spans="1:21" ht="13.5" customHeight="1">
       <c r="A118" s="26">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -5596,7 +5618,7 @@
       <c r="S118" s="17"/>
       <c r="T118" s="17"/>
     </row>
-    <row r="119" spans="1:20" ht="13.5" customHeight="1">
+    <row r="119" spans="1:21" ht="13.5" customHeight="1">
       <c r="A119" s="26">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -5629,7 +5651,7 @@
       <c r="S119" s="17"/>
       <c r="T119" s="17"/>
     </row>
-    <row r="120" spans="1:20" ht="13.5" customHeight="1">
+    <row r="120" spans="1:21" ht="13.5" customHeight="1">
       <c r="A120" s="26">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -5662,7 +5684,7 @@
       <c r="S120" s="17"/>
       <c r="T120" s="17"/>
     </row>
-    <row r="121" spans="1:20" ht="13.5" customHeight="1">
+    <row r="121" spans="1:21" ht="13.5" customHeight="1">
       <c r="A121" s="26">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -5699,7 +5721,7 @@
       <c r="S121" s="17"/>
       <c r="T121" s="17"/>
     </row>
-    <row r="122" spans="1:20" ht="13.5" customHeight="1">
+    <row r="122" spans="1:21" ht="13.5" customHeight="1">
       <c r="A122" s="26">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -5730,7 +5752,7 @@
       <c r="S122" s="17"/>
       <c r="T122" s="17"/>
     </row>
-    <row r="123" spans="1:20" ht="13.5" customHeight="1">
+    <row r="123" spans="1:21" ht="13.5" customHeight="1">
       <c r="A123" s="26">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -5763,7 +5785,7 @@
       <c r="S123" s="17"/>
       <c r="T123" s="17"/>
     </row>
-    <row r="124" spans="1:20" ht="13.5" customHeight="1">
+    <row r="124" spans="1:21" ht="13.5" customHeight="1">
       <c r="A124" s="26">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -5794,7 +5816,7 @@
       <c r="S124" s="17"/>
       <c r="T124" s="17"/>
     </row>
-    <row r="125" spans="1:20" ht="13.5" customHeight="1">
+    <row r="125" spans="1:21" ht="13.5" customHeight="1">
       <c r="A125" s="26">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -5831,7 +5853,7 @@
       <c r="S125" s="17"/>
       <c r="T125" s="17"/>
     </row>
-    <row r="126" spans="1:20" ht="13.5" customHeight="1">
+    <row r="126" spans="1:21" ht="13.5" customHeight="1">
       <c r="A126" s="26">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -5862,7 +5884,7 @@
       <c r="S126" s="17"/>
       <c r="T126" s="17"/>
     </row>
-    <row r="127" spans="1:20" ht="13.5" customHeight="1">
+    <row r="127" spans="1:21" ht="13.5" customHeight="1">
       <c r="A127" s="26">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -5895,7 +5917,7 @@
       <c r="S127" s="17"/>
       <c r="T127" s="17"/>
     </row>
-    <row r="128" spans="1:20" ht="13.5" customHeight="1">
+    <row r="128" spans="1:21" ht="13.5" customHeight="1">
       <c r="A128" s="26">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -7536,7 +7558,7 @@
       <c r="S176" s="17"/>
       <c r="T176" s="17"/>
     </row>
-    <row r="177" spans="1:20" ht="13.5" customHeight="1">
+    <row r="177" spans="1:21" ht="13.5" customHeight="1">
       <c r="A177" s="26">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -7569,7 +7591,7 @@
       <c r="S177" s="17"/>
       <c r="T177" s="17"/>
     </row>
-    <row r="178" spans="1:20" ht="13.5" customHeight="1">
+    <row r="178" spans="1:21" ht="13.5" customHeight="1">
       <c r="A178" s="26">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -7606,7 +7628,7 @@
       <c r="S178" s="17"/>
       <c r="T178" s="17"/>
     </row>
-    <row r="179" spans="1:20" ht="13.5" customHeight="1">
+    <row r="179" spans="1:21" ht="13.5" customHeight="1">
       <c r="A179" s="26">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -7641,7 +7663,7 @@
       <c r="S179" s="17"/>
       <c r="T179" s="17"/>
     </row>
-    <row r="180" spans="1:20" ht="13.5" customHeight="1">
+    <row r="180" spans="1:21" ht="13.5" customHeight="1">
       <c r="A180" s="26">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -7684,7 +7706,7 @@
       </c>
       <c r="T180" s="17"/>
     </row>
-    <row r="181" spans="1:20" ht="13.5" customHeight="1">
+    <row r="181" spans="1:21" ht="13.5" customHeight="1">
       <c r="A181" s="26">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -7720,8 +7742,11 @@
       <c r="R181" s="17"/>
       <c r="S181" s="17"/>
       <c r="T181" s="17"/>
-    </row>
-    <row r="182" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U181" s="37">
+        <v>5.2929781563048998E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21" ht="13.5" customHeight="1">
       <c r="A182" s="26">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -7760,7 +7785,7 @@
       </c>
       <c r="T182" s="17"/>
     </row>
-    <row r="183" spans="1:20" ht="13.5" customHeight="1">
+    <row r="183" spans="1:21" ht="13.5" customHeight="1">
       <c r="A183" s="26">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -7797,7 +7822,7 @@
       <c r="S183" s="17"/>
       <c r="T183" s="17"/>
     </row>
-    <row r="184" spans="1:20" ht="13.5" customHeight="1">
+    <row r="184" spans="1:21" ht="13.5" customHeight="1">
       <c r="A184" s="26">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -7830,7 +7855,7 @@
       <c r="S184" s="17"/>
       <c r="T184" s="17"/>
     </row>
-    <row r="185" spans="1:20" ht="13.5" customHeight="1">
+    <row r="185" spans="1:21" ht="13.5" customHeight="1">
       <c r="A185" s="26">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -7865,7 +7890,7 @@
       <c r="S185" s="17"/>
       <c r="T185" s="17"/>
     </row>
-    <row r="186" spans="1:20" ht="13.5" customHeight="1">
+    <row r="186" spans="1:21" ht="13.5" customHeight="1">
       <c r="A186" s="26">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -7896,7 +7921,7 @@
       <c r="S186" s="17"/>
       <c r="T186" s="17"/>
     </row>
-    <row r="187" spans="1:20" ht="13.5" customHeight="1">
+    <row r="187" spans="1:21" ht="13.5" customHeight="1">
       <c r="A187" s="26">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -7933,7 +7958,7 @@
       <c r="S187" s="17"/>
       <c r="T187" s="17"/>
     </row>
-    <row r="188" spans="1:20" ht="13.5" customHeight="1">
+    <row r="188" spans="1:21" ht="13.5" customHeight="1">
       <c r="A188" s="26">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -7964,7 +7989,7 @@
       <c r="S188" s="17"/>
       <c r="T188" s="17"/>
     </row>
-    <row r="189" spans="1:20" ht="13.5" customHeight="1">
+    <row r="189" spans="1:21" ht="13.5" customHeight="1">
       <c r="A189" s="26">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -7995,7 +8020,7 @@
       <c r="S189" s="17"/>
       <c r="T189" s="17"/>
     </row>
-    <row r="190" spans="1:20" ht="13.5" customHeight="1">
+    <row r="190" spans="1:21" ht="13.5" customHeight="1">
       <c r="A190" s="26">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -8032,7 +8057,7 @@
       <c r="S190" s="17"/>
       <c r="T190" s="17"/>
     </row>
-    <row r="191" spans="1:20" ht="13.5" customHeight="1">
+    <row r="191" spans="1:21" ht="13.5" customHeight="1">
       <c r="A191" s="26">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -8071,7 +8096,7 @@
       <c r="S191" s="17"/>
       <c r="T191" s="17"/>
     </row>
-    <row r="192" spans="1:20" ht="13.5" customHeight="1">
+    <row r="192" spans="1:21" ht="13.5" customHeight="1">
       <c r="A192" s="26">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -9178,7 +9203,7 @@
       </c>
       <c r="T224" s="17"/>
     </row>
-    <row r="225" spans="1:20" ht="13.5" customHeight="1">
+    <row r="225" spans="1:21" ht="13.5" customHeight="1">
       <c r="A225" s="26">
         <f t="shared" si="3"/>
         <v>185</v>
@@ -9218,8 +9243,11 @@
       <c r="R225" s="17"/>
       <c r="S225" s="17"/>
       <c r="T225" s="17"/>
-    </row>
-    <row r="226" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U225" s="37">
+        <v>0.19031599657989201</v>
+      </c>
+    </row>
+    <row r="226" spans="1:21" ht="13.5" customHeight="1">
       <c r="A226" s="26">
         <f t="shared" si="3"/>
         <v>186</v>
@@ -9248,7 +9276,7 @@
       <c r="S226" s="17"/>
       <c r="T226" s="17"/>
     </row>
-    <row r="227" spans="1:20" ht="13.5" customHeight="1">
+    <row r="227" spans="1:21" ht="13.5" customHeight="1">
       <c r="A227" s="26">
         <f t="shared" si="3"/>
         <v>187</v>
@@ -9281,7 +9309,7 @@
       <c r="S227" s="17"/>
       <c r="T227" s="17"/>
     </row>
-    <row r="228" spans="1:20" ht="13.5" customHeight="1">
+    <row r="228" spans="1:21" ht="13.5" customHeight="1">
       <c r="A228" s="26">
         <f t="shared" si="3"/>
         <v>188</v>
@@ -9312,7 +9340,7 @@
       <c r="S228" s="17"/>
       <c r="T228" s="17"/>
     </row>
-    <row r="229" spans="1:20" ht="13.5" customHeight="1">
+    <row r="229" spans="1:21" ht="13.5" customHeight="1">
       <c r="A229" s="26">
         <f t="shared" si="3"/>
         <v>189</v>
@@ -9343,7 +9371,7 @@
       <c r="S229" s="17"/>
       <c r="T229" s="17"/>
     </row>
-    <row r="230" spans="1:20" ht="13.5" customHeight="1">
+    <row r="230" spans="1:21" ht="13.5" customHeight="1">
       <c r="A230" s="26">
         <f t="shared" si="3"/>
         <v>190</v>
@@ -9374,7 +9402,7 @@
       <c r="S230" s="17"/>
       <c r="T230" s="17"/>
     </row>
-    <row r="231" spans="1:20" ht="13.5" customHeight="1">
+    <row r="231" spans="1:21" ht="13.5" customHeight="1">
       <c r="A231" s="26">
         <f t="shared" si="3"/>
         <v>191</v>
@@ -9405,7 +9433,7 @@
       <c r="S231" s="17"/>
       <c r="T231" s="17"/>
     </row>
-    <row r="232" spans="1:20" ht="13.5" customHeight="1">
+    <row r="232" spans="1:21" ht="13.5" customHeight="1">
       <c r="A232" s="26">
         <f t="shared" si="3"/>
         <v>192</v>
@@ -9436,7 +9464,7 @@
       <c r="S232" s="17"/>
       <c r="T232" s="17"/>
     </row>
-    <row r="233" spans="1:20" ht="13.5" customHeight="1">
+    <row r="233" spans="1:21" ht="13.5" customHeight="1">
       <c r="A233" s="26">
         <f t="shared" si="3"/>
         <v>193</v>
@@ -9467,7 +9495,7 @@
       <c r="S233" s="17"/>
       <c r="T233" s="17"/>
     </row>
-    <row r="234" spans="1:20" ht="13.5" customHeight="1">
+    <row r="234" spans="1:21" ht="13.5" customHeight="1">
       <c r="A234" s="26">
         <f t="shared" si="3"/>
         <v>194</v>
@@ -9504,7 +9532,7 @@
       <c r="S234" s="17"/>
       <c r="T234" s="17"/>
     </row>
-    <row r="235" spans="1:20" ht="13.5" customHeight="1">
+    <row r="235" spans="1:21" ht="13.5" customHeight="1">
       <c r="A235" s="26">
         <f t="shared" si="3"/>
         <v>195</v>
@@ -9541,7 +9569,7 @@
       <c r="S235" s="17"/>
       <c r="T235" s="17"/>
     </row>
-    <row r="236" spans="1:20" ht="13.5" customHeight="1">
+    <row r="236" spans="1:21" ht="13.5" customHeight="1">
       <c r="A236" s="26">
         <f t="shared" si="3"/>
         <v>196</v>
@@ -9572,7 +9600,7 @@
       <c r="S236" s="17"/>
       <c r="T236" s="17"/>
     </row>
-    <row r="237" spans="1:20" ht="13.5" customHeight="1">
+    <row r="237" spans="1:21" ht="13.5" customHeight="1">
       <c r="A237" s="26">
         <f t="shared" si="3"/>
         <v>197</v>
@@ -9607,7 +9635,7 @@
       <c r="S237" s="17"/>
       <c r="T237" s="17"/>
     </row>
-    <row r="238" spans="1:20" ht="13.5" customHeight="1">
+    <row r="238" spans="1:21" ht="13.5" customHeight="1">
       <c r="A238" s="26">
         <f t="shared" si="3"/>
         <v>198</v>
@@ -9638,7 +9666,7 @@
       <c r="S238" s="17"/>
       <c r="T238" s="17"/>
     </row>
-    <row r="239" spans="1:20" ht="13.5" customHeight="1">
+    <row r="239" spans="1:21" ht="13.5" customHeight="1">
       <c r="A239" s="26">
         <f t="shared" si="3"/>
         <v>199</v>
@@ -9669,7 +9697,7 @@
       <c r="S239" s="17"/>
       <c r="T239" s="17"/>
     </row>
-    <row r="240" spans="1:20" ht="13.5" customHeight="1">
+    <row r="240" spans="1:21" ht="13.5" customHeight="1">
       <c r="A240" s="26">
         <f t="shared" si="3"/>
         <v>200</v>
@@ -17164,7 +17192,7 @@
       <c r="S464" s="17"/>
       <c r="T464" s="17"/>
     </row>
-    <row r="465" spans="1:20" ht="13.5" customHeight="1">
+    <row r="465" spans="1:21" ht="13.5" customHeight="1">
       <c r="A465" s="26">
         <f t="shared" si="6"/>
         <v>420</v>
@@ -17204,8 +17232,11 @@
       </c>
       <c r="S465" s="17"/>
       <c r="T465" s="17"/>
-    </row>
-    <row r="466" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U465" s="37">
+        <v>0.30833923649837902</v>
+      </c>
+    </row>
+    <row r="466" spans="1:21" ht="13.5" customHeight="1">
       <c r="A466" s="26">
         <f t="shared" si="6"/>
         <v>421</v>
@@ -17234,7 +17265,7 @@
       <c r="S466" s="17"/>
       <c r="T466" s="17"/>
     </row>
-    <row r="467" spans="1:20" ht="13.5" customHeight="1">
+    <row r="467" spans="1:21" ht="13.5" customHeight="1">
       <c r="A467" s="26">
         <f t="shared" si="6"/>
         <v>422</v>
@@ -17263,7 +17294,7 @@
       <c r="S467" s="17"/>
       <c r="T467" s="17"/>
     </row>
-    <row r="468" spans="1:20" ht="13.5" customHeight="1">
+    <row r="468" spans="1:21" ht="13.5" customHeight="1">
       <c r="A468" s="26">
         <f t="shared" si="6"/>
         <v>423</v>
@@ -17298,7 +17329,7 @@
       <c r="S468" s="17"/>
       <c r="T468" s="17"/>
     </row>
-    <row r="469" spans="1:20" ht="13.5" customHeight="1">
+    <row r="469" spans="1:21" ht="13.5" customHeight="1">
       <c r="A469" s="26">
         <f t="shared" si="6"/>
         <v>424</v>
@@ -17331,7 +17362,7 @@
       <c r="S469" s="17"/>
       <c r="T469" s="17"/>
     </row>
-    <row r="470" spans="1:20" ht="13.5" customHeight="1">
+    <row r="470" spans="1:21" ht="13.5" customHeight="1">
       <c r="A470" s="26">
         <f t="shared" si="6"/>
         <v>425</v>
@@ -17366,7 +17397,7 @@
       <c r="S470" s="17"/>
       <c r="T470" s="17"/>
     </row>
-    <row r="471" spans="1:20" ht="13.5" customHeight="1">
+    <row r="471" spans="1:21" ht="13.5" customHeight="1">
       <c r="A471" s="26">
         <f t="shared" si="6"/>
         <v>426</v>
@@ -17403,7 +17434,7 @@
       <c r="S471" s="17"/>
       <c r="T471" s="17"/>
     </row>
-    <row r="472" spans="1:20" ht="13.5" customHeight="1">
+    <row r="472" spans="1:21" ht="13.5" customHeight="1">
       <c r="A472" s="26">
         <f t="shared" si="6"/>
         <v>427</v>
@@ -17436,7 +17467,7 @@
       <c r="S472" s="17"/>
       <c r="T472" s="17"/>
     </row>
-    <row r="473" spans="1:20" ht="13.5" customHeight="1">
+    <row r="473" spans="1:21" ht="13.5" customHeight="1">
       <c r="A473" s="26">
         <f t="shared" si="6"/>
         <v>428</v>
@@ -17473,7 +17504,7 @@
       <c r="S473" s="17"/>
       <c r="T473" s="17"/>
     </row>
-    <row r="474" spans="1:20" ht="13.5" customHeight="1">
+    <row r="474" spans="1:21" ht="13.5" customHeight="1">
       <c r="A474" s="26">
         <f t="shared" si="6"/>
         <v>428</v>
@@ -17504,7 +17535,7 @@
       <c r="S474" s="17"/>
       <c r="T474" s="17"/>
     </row>
-    <row r="475" spans="1:20" ht="13.5" customHeight="1">
+    <row r="475" spans="1:21" ht="13.5" customHeight="1">
       <c r="A475" s="26">
         <f t="shared" si="6"/>
         <v>429</v>
@@ -17537,7 +17568,7 @@
       <c r="S475" s="17"/>
       <c r="T475" s="17"/>
     </row>
-    <row r="476" spans="1:20" ht="13.5" customHeight="1">
+    <row r="476" spans="1:21" ht="13.5" customHeight="1">
       <c r="A476" s="26">
         <f t="shared" si="6"/>
         <v>430</v>
@@ -17576,7 +17607,7 @@
       <c r="S476" s="17"/>
       <c r="T476" s="17"/>
     </row>
-    <row r="477" spans="1:20" ht="13.5" customHeight="1">
+    <row r="477" spans="1:21" ht="13.5" customHeight="1">
       <c r="A477" s="26">
         <f t="shared" si="6"/>
         <v>431</v>
@@ -17607,7 +17638,7 @@
       <c r="S477" s="17"/>
       <c r="T477" s="17"/>
     </row>
-    <row r="478" spans="1:20" ht="13.5" customHeight="1">
+    <row r="478" spans="1:21" ht="13.5" customHeight="1">
       <c r="A478" s="26">
         <f t="shared" si="6"/>
         <v>432</v>
@@ -17646,7 +17677,7 @@
       </c>
       <c r="T478" s="17"/>
     </row>
-    <row r="479" spans="1:20" ht="13.5" customHeight="1">
+    <row r="479" spans="1:21" ht="13.5" customHeight="1">
       <c r="A479" s="26">
         <f t="shared" si="6"/>
         <v>433</v>
@@ -17687,7 +17718,7 @@
       <c r="S479" s="17"/>
       <c r="T479" s="17"/>
     </row>
-    <row r="480" spans="1:20" ht="13.5" customHeight="1">
+    <row r="480" spans="1:21" ht="13.5" customHeight="1">
       <c r="A480" s="26">
         <f t="shared" ref="A480:A543" si="7">IF(OR(F480="",F480=""),A479,A479+1)</f>
         <v>434</v>
@@ -18244,7 +18275,7 @@
       <c r="S496" s="17"/>
       <c r="T496" s="17"/>
     </row>
-    <row r="497" spans="1:20" ht="13.5" customHeight="1">
+    <row r="497" spans="1:21" ht="13.5" customHeight="1">
       <c r="A497" s="26">
         <f t="shared" si="7"/>
         <v>450</v>
@@ -18277,7 +18308,7 @@
       <c r="S497" s="17"/>
       <c r="T497" s="17"/>
     </row>
-    <row r="498" spans="1:20" ht="13.5" customHeight="1">
+    <row r="498" spans="1:21" ht="13.5" customHeight="1">
       <c r="A498" s="26">
         <f t="shared" si="7"/>
         <v>451</v>
@@ -18308,7 +18339,7 @@
       <c r="S498" s="17"/>
       <c r="T498" s="17"/>
     </row>
-    <row r="499" spans="1:20" ht="13.5" customHeight="1">
+    <row r="499" spans="1:21" ht="13.5" customHeight="1">
       <c r="A499" s="26">
         <f t="shared" si="7"/>
         <v>452</v>
@@ -18343,7 +18374,7 @@
       <c r="S499" s="17"/>
       <c r="T499" s="17"/>
     </row>
-    <row r="500" spans="1:20" ht="13.5" customHeight="1">
+    <row r="500" spans="1:21" ht="13.5" customHeight="1">
       <c r="A500" s="26">
         <f t="shared" si="7"/>
         <v>453</v>
@@ -18380,7 +18411,7 @@
       <c r="S500" s="17"/>
       <c r="T500" s="17"/>
     </row>
-    <row r="501" spans="1:20" ht="13.5" customHeight="1">
+    <row r="501" spans="1:21" ht="13.5" customHeight="1">
       <c r="A501" s="26">
         <f t="shared" si="7"/>
         <v>454</v>
@@ -18411,7 +18442,7 @@
       <c r="S501" s="17"/>
       <c r="T501" s="17"/>
     </row>
-    <row r="502" spans="1:20" ht="13.5" customHeight="1">
+    <row r="502" spans="1:21" ht="13.5" customHeight="1">
       <c r="A502" s="26">
         <f t="shared" si="7"/>
         <v>455</v>
@@ -18446,7 +18477,7 @@
       <c r="S502" s="17"/>
       <c r="T502" s="17"/>
     </row>
-    <row r="503" spans="1:20" ht="13.5" customHeight="1">
+    <row r="503" spans="1:21" ht="13.5" customHeight="1">
       <c r="A503" s="26">
         <f t="shared" si="7"/>
         <v>456</v>
@@ -18479,7 +18510,7 @@
       <c r="S503" s="17"/>
       <c r="T503" s="17"/>
     </row>
-    <row r="504" spans="1:20" ht="13.5" customHeight="1">
+    <row r="504" spans="1:21" ht="13.5" customHeight="1">
       <c r="A504" s="26">
         <f t="shared" si="7"/>
         <v>457</v>
@@ -18514,7 +18545,7 @@
       <c r="S504" s="17"/>
       <c r="T504" s="17"/>
     </row>
-    <row r="505" spans="1:20" ht="13.5" customHeight="1">
+    <row r="505" spans="1:21" ht="13.5" customHeight="1">
       <c r="A505" s="26">
         <f t="shared" si="7"/>
         <v>458</v>
@@ -18545,7 +18576,7 @@
       <c r="S505" s="17"/>
       <c r="T505" s="17"/>
     </row>
-    <row r="506" spans="1:20" ht="13.5" customHeight="1">
+    <row r="506" spans="1:21" ht="13.5" customHeight="1">
       <c r="A506" s="26">
         <f t="shared" si="7"/>
         <v>459</v>
@@ -18579,8 +18610,11 @@
       <c r="R506" s="17"/>
       <c r="S506" s="17"/>
       <c r="T506" s="17"/>
-    </row>
-    <row r="507" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U506" s="37">
+        <v>3.4543911121878101E-2</v>
+      </c>
+    </row>
+    <row r="507" spans="1:21" ht="13.5" customHeight="1">
       <c r="A507" s="26">
         <f t="shared" si="7"/>
         <v>459</v>
@@ -18617,7 +18651,7 @@
       <c r="S507" s="17"/>
       <c r="T507" s="17"/>
     </row>
-    <row r="508" spans="1:20" ht="13.5" customHeight="1">
+    <row r="508" spans="1:21" ht="13.5" customHeight="1">
       <c r="A508" s="26">
         <f t="shared" si="7"/>
         <v>460</v>
@@ -18658,7 +18692,7 @@
       <c r="S508" s="17"/>
       <c r="T508" s="17"/>
     </row>
-    <row r="509" spans="1:20" ht="13.5" customHeight="1">
+    <row r="509" spans="1:21" ht="13.5" customHeight="1">
       <c r="A509" s="26">
         <f t="shared" si="7"/>
         <v>461</v>
@@ -18691,7 +18725,7 @@
       <c r="S509" s="17"/>
       <c r="T509" s="17"/>
     </row>
-    <row r="510" spans="1:20" ht="13.5" customHeight="1">
+    <row r="510" spans="1:21" ht="13.5" customHeight="1">
       <c r="A510" s="26">
         <f t="shared" si="7"/>
         <v>462</v>
@@ -18724,7 +18758,7 @@
       <c r="S510" s="17"/>
       <c r="T510" s="17"/>
     </row>
-    <row r="511" spans="1:20" ht="13.5" customHeight="1">
+    <row r="511" spans="1:21" ht="13.5" customHeight="1">
       <c r="A511" s="26">
         <f t="shared" si="7"/>
         <v>462</v>
@@ -18753,7 +18787,7 @@
       <c r="S511" s="17"/>
       <c r="T511" s="17"/>
     </row>
-    <row r="512" spans="1:20" ht="13.5" customHeight="1">
+    <row r="512" spans="1:21" ht="13.5" customHeight="1">
       <c r="A512" s="26">
         <f t="shared" si="7"/>
         <v>463</v>
@@ -19306,7 +19340,7 @@
       <c r="S528" s="17"/>
       <c r="T528" s="17"/>
     </row>
-    <row r="529" spans="1:20" ht="13.5" customHeight="1">
+    <row r="529" spans="1:21" ht="13.5" customHeight="1">
       <c r="A529" s="26">
         <f t="shared" si="7"/>
         <v>478</v>
@@ -19343,7 +19377,7 @@
       <c r="S529" s="17"/>
       <c r="T529" s="17"/>
     </row>
-    <row r="530" spans="1:20" ht="13.5" customHeight="1">
+    <row r="530" spans="1:21" ht="13.5" customHeight="1">
       <c r="A530" s="26">
         <f t="shared" si="7"/>
         <v>478</v>
@@ -19374,7 +19408,7 @@
       <c r="S530" s="17"/>
       <c r="T530" s="17"/>
     </row>
-    <row r="531" spans="1:20" ht="13.5" customHeight="1">
+    <row r="531" spans="1:21" ht="13.5" customHeight="1">
       <c r="A531" s="26">
         <f t="shared" si="7"/>
         <v>479</v>
@@ -19409,7 +19443,7 @@
       <c r="S531" s="17"/>
       <c r="T531" s="17"/>
     </row>
-    <row r="532" spans="1:20" ht="13.5" customHeight="1">
+    <row r="532" spans="1:21" ht="13.5" customHeight="1">
       <c r="A532" s="26">
         <f t="shared" si="7"/>
         <v>480</v>
@@ -19443,8 +19477,11 @@
       <c r="R532" s="17"/>
       <c r="S532" s="17"/>
       <c r="T532" s="17"/>
-    </row>
-    <row r="533" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U532" s="37">
+        <v>9.6813604788476906E-2</v>
+      </c>
+    </row>
+    <row r="533" spans="1:21" ht="13.5" customHeight="1">
       <c r="A533" s="26">
         <f t="shared" si="7"/>
         <v>480</v>
@@ -19479,7 +19516,7 @@
       <c r="S533" s="17"/>
       <c r="T533" s="17"/>
     </row>
-    <row r="534" spans="1:20" ht="13.5" customHeight="1">
+    <row r="534" spans="1:21" ht="13.5" customHeight="1">
       <c r="A534" s="26">
         <f t="shared" si="7"/>
         <v>481</v>
@@ -19512,7 +19549,7 @@
       <c r="S534" s="17"/>
       <c r="T534" s="17"/>
     </row>
-    <row r="535" spans="1:20" ht="13.5" customHeight="1">
+    <row r="535" spans="1:21" ht="13.5" customHeight="1">
       <c r="A535" s="26">
         <f t="shared" si="7"/>
         <v>482</v>
@@ -19543,7 +19580,7 @@
       <c r="S535" s="17"/>
       <c r="T535" s="17"/>
     </row>
-    <row r="536" spans="1:20" ht="13.5" customHeight="1">
+    <row r="536" spans="1:21" ht="13.5" customHeight="1">
       <c r="A536" s="26">
         <f t="shared" si="7"/>
         <v>483</v>
@@ -19574,7 +19611,7 @@
       <c r="S536" s="17"/>
       <c r="T536" s="17"/>
     </row>
-    <row r="537" spans="1:20" ht="13.5" customHeight="1">
+    <row r="537" spans="1:21" ht="13.5" customHeight="1">
       <c r="A537" s="26">
         <f t="shared" si="7"/>
         <v>484</v>
@@ -19611,7 +19648,7 @@
       <c r="S537" s="17"/>
       <c r="T537" s="17"/>
     </row>
-    <row r="538" spans="1:20" ht="13.5" customHeight="1">
+    <row r="538" spans="1:21" ht="13.5" customHeight="1">
       <c r="A538" s="26">
         <f t="shared" si="7"/>
         <v>485</v>
@@ -19648,7 +19685,7 @@
       <c r="S538" s="17"/>
       <c r="T538" s="17"/>
     </row>
-    <row r="539" spans="1:20" ht="13.5" customHeight="1">
+    <row r="539" spans="1:21" ht="13.5" customHeight="1">
       <c r="A539" s="26">
         <f t="shared" si="7"/>
         <v>486</v>
@@ -19681,7 +19718,7 @@
       <c r="S539" s="17"/>
       <c r="T539" s="17"/>
     </row>
-    <row r="540" spans="1:20" ht="13.5" customHeight="1">
+    <row r="540" spans="1:21" ht="13.5" customHeight="1">
       <c r="A540" s="26">
         <f t="shared" si="7"/>
         <v>487</v>
@@ -19712,7 +19749,7 @@
       <c r="S540" s="17"/>
       <c r="T540" s="17"/>
     </row>
-    <row r="541" spans="1:20" ht="13.5" customHeight="1">
+    <row r="541" spans="1:21" ht="13.5" customHeight="1">
       <c r="A541" s="26">
         <f t="shared" si="7"/>
         <v>488</v>
@@ -19743,7 +19780,7 @@
       <c r="S541" s="17"/>
       <c r="T541" s="17"/>
     </row>
-    <row r="542" spans="1:20" ht="13.5" customHeight="1">
+    <row r="542" spans="1:21" ht="13.5" customHeight="1">
       <c r="A542" s="26">
         <f t="shared" si="7"/>
         <v>489</v>
@@ -19776,7 +19813,7 @@
       <c r="S542" s="17"/>
       <c r="T542" s="17"/>
     </row>
-    <row r="543" spans="1:20" ht="13.5" customHeight="1">
+    <row r="543" spans="1:21" ht="13.5" customHeight="1">
       <c r="A543" s="26">
         <f t="shared" si="7"/>
         <v>490</v>
@@ -19807,7 +19844,7 @@
       <c r="S543" s="17"/>
       <c r="T543" s="17"/>
     </row>
-    <row r="544" spans="1:20" ht="13.5" customHeight="1">
+    <row r="544" spans="1:21" ht="13.5" customHeight="1">
       <c r="A544" s="26">
         <f t="shared" ref="A544:A607" si="8">IF(OR(F544="",F544=""),A543,A543+1)</f>
         <v>491</v>
@@ -24206,7 +24243,7 @@
       <c r="S672" s="17"/>
       <c r="T672" s="17"/>
     </row>
-    <row r="673" spans="1:20" ht="13.5" customHeight="1">
+    <row r="673" spans="1:21" ht="13.5" customHeight="1">
       <c r="A673" s="26">
         <f t="shared" si="10"/>
         <v>617</v>
@@ -24243,7 +24280,7 @@
       <c r="S673" s="17"/>
       <c r="T673" s="17"/>
     </row>
-    <row r="674" spans="1:20" ht="13.5" customHeight="1">
+    <row r="674" spans="1:21" ht="13.5" customHeight="1">
       <c r="A674" s="26">
         <f t="shared" si="10"/>
         <v>617</v>
@@ -24274,7 +24311,7 @@
       <c r="S674" s="17"/>
       <c r="T674" s="17"/>
     </row>
-    <row r="675" spans="1:20" ht="13.5" customHeight="1">
+    <row r="675" spans="1:21" ht="13.5" customHeight="1">
       <c r="A675" s="26">
         <f t="shared" si="10"/>
         <v>618</v>
@@ -24288,12 +24325,12 @@
         <v>141</v>
       </c>
       <c r="F675" s="27" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="G675" s="17"/>
       <c r="H675" s="17"/>
       <c r="I675" s="27" t="s">
-        <v>34</v>
+        <v>182</v>
       </c>
       <c r="J675" s="26" t="s">
         <v>20</v>
@@ -24303,19 +24340,24 @@
         <v>158</v>
       </c>
       <c r="M675" s="27" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="N675" s="17"/>
       <c r="O675" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="P675" s="17"/>
+      <c r="P675" s="17" t="s">
+        <v>55</v>
+      </c>
       <c r="Q675" s="17"/>
       <c r="R675" s="17"/>
       <c r="S675" s="17"/>
       <c r="T675" s="17"/>
-    </row>
-    <row r="676" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U675" s="38">
+        <v>2.23381794716856E-2</v>
+      </c>
+    </row>
+    <row r="676" spans="1:21" ht="13.5" customHeight="1">
       <c r="A676" s="26">
         <f t="shared" si="10"/>
         <v>619</v>
@@ -24352,7 +24394,7 @@
       <c r="S676" s="17"/>
       <c r="T676" s="17"/>
     </row>
-    <row r="677" spans="1:20" ht="13.5" customHeight="1">
+    <row r="677" spans="1:21" ht="13.5" customHeight="1">
       <c r="A677" s="26">
         <f t="shared" si="10"/>
         <v>620</v>
@@ -24383,7 +24425,7 @@
       <c r="S677" s="17"/>
       <c r="T677" s="17"/>
     </row>
-    <row r="678" spans="1:20" ht="13.5" customHeight="1">
+    <row r="678" spans="1:21" ht="13.5" customHeight="1">
       <c r="A678" s="26">
         <f t="shared" si="10"/>
         <v>621</v>
@@ -24414,7 +24456,7 @@
       <c r="S678" s="17"/>
       <c r="T678" s="17"/>
     </row>
-    <row r="679" spans="1:20" ht="13.5" customHeight="1">
+    <row r="679" spans="1:21" ht="13.5" customHeight="1">
       <c r="A679" s="26">
         <f t="shared" si="10"/>
         <v>622</v>
@@ -24451,7 +24493,7 @@
       <c r="S679" s="17"/>
       <c r="T679" s="17"/>
     </row>
-    <row r="680" spans="1:20" ht="13.5" customHeight="1">
+    <row r="680" spans="1:21" ht="13.5" customHeight="1">
       <c r="A680" s="26">
         <f t="shared" si="10"/>
         <v>623</v>
@@ -24484,7 +24526,7 @@
       <c r="S680" s="17"/>
       <c r="T680" s="17"/>
     </row>
-    <row r="681" spans="1:20" ht="13.5" customHeight="1">
+    <row r="681" spans="1:21" ht="13.5" customHeight="1">
       <c r="A681" s="26">
         <f t="shared" si="10"/>
         <v>624</v>
@@ -24521,7 +24563,7 @@
       <c r="S681" s="17"/>
       <c r="T681" s="17"/>
     </row>
-    <row r="682" spans="1:20" ht="13.5" customHeight="1">
+    <row r="682" spans="1:21" ht="13.5" customHeight="1">
       <c r="A682" s="26">
         <f t="shared" si="10"/>
         <v>625</v>
@@ -24556,7 +24598,7 @@
       <c r="S682" s="17"/>
       <c r="T682" s="17"/>
     </row>
-    <row r="683" spans="1:20" ht="13.5" customHeight="1">
+    <row r="683" spans="1:21" ht="13.5" customHeight="1">
       <c r="A683" s="26">
         <f t="shared" si="10"/>
         <v>626</v>
@@ -24591,7 +24633,7 @@
       <c r="S683" s="17"/>
       <c r="T683" s="17"/>
     </row>
-    <row r="684" spans="1:20" ht="13.5" customHeight="1">
+    <row r="684" spans="1:21" ht="13.5" customHeight="1">
       <c r="A684" s="26">
         <f t="shared" si="10"/>
         <v>627</v>
@@ -24624,7 +24666,7 @@
       <c r="S684" s="17"/>
       <c r="T684" s="17"/>
     </row>
-    <row r="685" spans="1:20" ht="13.5" customHeight="1">
+    <row r="685" spans="1:21" ht="13.5" customHeight="1">
       <c r="A685" s="26">
         <f t="shared" si="10"/>
         <v>628</v>
@@ -24655,7 +24697,7 @@
       <c r="S685" s="17"/>
       <c r="T685" s="17"/>
     </row>
-    <row r="686" spans="1:20" ht="13.5" customHeight="1">
+    <row r="686" spans="1:21" ht="13.5" customHeight="1">
       <c r="A686" s="26">
         <f t="shared" si="10"/>
         <v>629</v>
@@ -24692,7 +24734,7 @@
       <c r="S686" s="17"/>
       <c r="T686" s="17"/>
     </row>
-    <row r="687" spans="1:20" ht="13.5" customHeight="1">
+    <row r="687" spans="1:21" ht="13.5" customHeight="1">
       <c r="A687" s="26">
         <f t="shared" si="10"/>
         <v>630</v>
@@ -24729,7 +24771,7 @@
       <c r="S687" s="17"/>
       <c r="T687" s="17"/>
     </row>
-    <row r="688" spans="1:20" ht="13.5" customHeight="1">
+    <row r="688" spans="1:21" ht="13.5" customHeight="1">
       <c r="A688" s="26">
         <f t="shared" si="10"/>
         <v>631</v>
@@ -25824,7 +25866,7 @@
       <c r="S720" s="17"/>
       <c r="T720" s="17"/>
     </row>
-    <row r="721" spans="1:20" ht="13.5" customHeight="1">
+    <row r="721" spans="1:21" ht="13.5" customHeight="1">
       <c r="A721" s="26">
         <f t="shared" si="10"/>
         <v>663</v>
@@ -25857,7 +25899,7 @@
       <c r="S721" s="17"/>
       <c r="T721" s="17"/>
     </row>
-    <row r="722" spans="1:20" ht="13.5" customHeight="1">
+    <row r="722" spans="1:21" ht="13.5" customHeight="1">
       <c r="A722" s="26">
         <f t="shared" si="10"/>
         <v>664</v>
@@ -25888,7 +25930,7 @@
       <c r="S722" s="17"/>
       <c r="T722" s="17"/>
     </row>
-    <row r="723" spans="1:20" ht="13.5" customHeight="1">
+    <row r="723" spans="1:21" ht="13.5" customHeight="1">
       <c r="A723" s="26">
         <f t="shared" si="10"/>
         <v>665</v>
@@ -25925,7 +25967,7 @@
       <c r="S723" s="17"/>
       <c r="T723" s="17"/>
     </row>
-    <row r="724" spans="1:20" ht="13.5" customHeight="1">
+    <row r="724" spans="1:21" ht="13.5" customHeight="1">
       <c r="A724" s="26">
         <f t="shared" si="10"/>
         <v>666</v>
@@ -25962,7 +26004,7 @@
       <c r="S724" s="17"/>
       <c r="T724" s="17"/>
     </row>
-    <row r="725" spans="1:20" ht="13.5" customHeight="1">
+    <row r="725" spans="1:21" ht="13.5" customHeight="1">
       <c r="A725" s="26">
         <f t="shared" si="10"/>
         <v>667</v>
@@ -25993,7 +26035,7 @@
       <c r="S725" s="17"/>
       <c r="T725" s="17"/>
     </row>
-    <row r="726" spans="1:20" ht="13.5" customHeight="1">
+    <row r="726" spans="1:21" ht="13.5" customHeight="1">
       <c r="A726" s="26">
         <f t="shared" si="10"/>
         <v>668</v>
@@ -26026,7 +26068,7 @@
       <c r="S726" s="17"/>
       <c r="T726" s="17"/>
     </row>
-    <row r="727" spans="1:20" ht="13.5" customHeight="1">
+    <row r="727" spans="1:21" ht="13.5" customHeight="1">
       <c r="A727" s="26">
         <f t="shared" si="10"/>
         <v>669</v>
@@ -26059,7 +26101,7 @@
       <c r="S727" s="17"/>
       <c r="T727" s="17"/>
     </row>
-    <row r="728" spans="1:20" ht="13.5" customHeight="1">
+    <row r="728" spans="1:21" ht="13.5" customHeight="1">
       <c r="A728" s="26">
         <f t="shared" si="10"/>
         <v>670</v>
@@ -26090,7 +26132,7 @@
       <c r="S728" s="17"/>
       <c r="T728" s="17"/>
     </row>
-    <row r="729" spans="1:20" ht="13.5" customHeight="1">
+    <row r="729" spans="1:21" ht="13.5" customHeight="1">
       <c r="A729" s="26">
         <f t="shared" si="10"/>
         <v>671</v>
@@ -26127,7 +26169,7 @@
       <c r="S729" s="17"/>
       <c r="T729" s="17"/>
     </row>
-    <row r="730" spans="1:20" ht="13.5" customHeight="1">
+    <row r="730" spans="1:21" ht="13.5" customHeight="1">
       <c r="A730" s="26">
         <f t="shared" si="10"/>
         <v>672</v>
@@ -26160,7 +26202,7 @@
       <c r="S730" s="17"/>
       <c r="T730" s="17"/>
     </row>
-    <row r="731" spans="1:20" ht="13.5" customHeight="1">
+    <row r="731" spans="1:21" ht="13.5" customHeight="1">
       <c r="A731" s="26">
         <f t="shared" si="10"/>
         <v>673</v>
@@ -26191,7 +26233,7 @@
       <c r="S731" s="17"/>
       <c r="T731" s="17"/>
     </row>
-    <row r="732" spans="1:20" ht="13.5" customHeight="1">
+    <row r="732" spans="1:21" ht="13.5" customHeight="1">
       <c r="A732" s="26">
         <f t="shared" si="10"/>
         <v>674</v>
@@ -26234,7 +26276,7 @@
       <c r="S732" s="17"/>
       <c r="T732" s="17"/>
     </row>
-    <row r="733" spans="1:20" ht="13.5" customHeight="1">
+    <row r="733" spans="1:21" ht="13.5" customHeight="1">
       <c r="A733" s="26">
         <f t="shared" si="10"/>
         <v>675</v>
@@ -26265,7 +26307,7 @@
       <c r="S733" s="17"/>
       <c r="T733" s="17"/>
     </row>
-    <row r="734" spans="1:20" ht="13.5" customHeight="1">
+    <row r="734" spans="1:21" ht="13.5" customHeight="1">
       <c r="A734" s="26">
         <f t="shared" si="10"/>
         <v>676</v>
@@ -26297,8 +26339,11 @@
       </c>
       <c r="S734" s="17"/>
       <c r="T734" s="17"/>
-    </row>
-    <row r="735" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U734" s="37">
+        <v>9.3192435930874007E-2</v>
+      </c>
+    </row>
+    <row r="735" spans="1:21" ht="13.5" customHeight="1">
       <c r="A735" s="26">
         <f t="shared" si="10"/>
         <v>677</v>
@@ -26341,7 +26386,7 @@
       <c r="S735" s="17"/>
       <c r="T735" s="17"/>
     </row>
-    <row r="736" spans="1:20" ht="13.5" customHeight="1">
+    <row r="736" spans="1:21" ht="13.5" customHeight="1">
       <c r="A736" s="26">
         <f t="shared" ref="A736:A799" si="11">IF(OR(F736="",F736=""),A735,A735+1)</f>
         <v>678</v>
@@ -26374,7 +26419,7 @@
       <c r="S736" s="17"/>
       <c r="T736" s="17"/>
     </row>
-    <row r="737" spans="1:20" ht="13.5" customHeight="1">
+    <row r="737" spans="1:21" ht="13.5" customHeight="1">
       <c r="A737" s="26">
         <f t="shared" si="11"/>
         <v>679</v>
@@ -26413,7 +26458,7 @@
       <c r="S737" s="27"/>
       <c r="T737" s="17"/>
     </row>
-    <row r="738" spans="1:20" ht="13.5" customHeight="1">
+    <row r="738" spans="1:21" ht="13.5" customHeight="1">
       <c r="A738" s="26">
         <f t="shared" si="11"/>
         <v>680</v>
@@ -26459,8 +26504,11 @@
       <c r="T738" s="27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="739" spans="1:20" ht="13.5" customHeight="1">
+      <c r="U738" s="37">
+        <v>0.31599800851481702</v>
+      </c>
+    </row>
+    <row r="739" spans="1:21" ht="13.5" customHeight="1">
       <c r="A739" s="26">
         <f t="shared" si="11"/>
         <v>681</v>
@@ -26493,7 +26541,7 @@
       <c r="S739" s="17"/>
       <c r="T739" s="17"/>
     </row>
-    <row r="740" spans="1:20" ht="13.5" customHeight="1">
+    <row r="740" spans="1:21" ht="13.5" customHeight="1">
       <c r="A740" s="26">
         <f t="shared" si="11"/>
         <v>682</v>
@@ -26524,7 +26572,7 @@
       <c r="S740" s="17"/>
       <c r="T740" s="17"/>
     </row>
-    <row r="741" spans="1:20" ht="13.5" customHeight="1">
+    <row r="741" spans="1:21" ht="13.5" customHeight="1">
       <c r="A741" s="26">
         <f t="shared" si="11"/>
         <v>683</v>
@@ -26557,7 +26605,7 @@
       <c r="S741" s="17"/>
       <c r="T741" s="17"/>
     </row>
-    <row r="742" spans="1:20" ht="13.5" customHeight="1">
+    <row r="742" spans="1:21" ht="13.5" customHeight="1">
       <c r="A742" s="26">
         <f t="shared" si="11"/>
         <v>683</v>
@@ -26586,7 +26634,7 @@
       <c r="S742" s="17"/>
       <c r="T742" s="17"/>
     </row>
-    <row r="743" spans="1:20" ht="13.5" customHeight="1">
+    <row r="743" spans="1:21" ht="13.5" customHeight="1">
       <c r="A743" s="26">
         <f t="shared" si="11"/>
         <v>684</v>
@@ -26619,7 +26667,7 @@
       <c r="S743" s="17"/>
       <c r="T743" s="17"/>
     </row>
-    <row r="744" spans="1:20" ht="13.5" customHeight="1">
+    <row r="744" spans="1:21" ht="13.5" customHeight="1">
       <c r="A744" s="26">
         <f t="shared" si="11"/>
         <v>685</v>
@@ -26654,7 +26702,7 @@
       <c r="S744" s="17"/>
       <c r="T744" s="17"/>
     </row>
-    <row r="745" spans="1:20" ht="13.5" customHeight="1">
+    <row r="745" spans="1:21" ht="13.5" customHeight="1">
       <c r="A745" s="26">
         <f t="shared" si="11"/>
         <v>686</v>
@@ -26685,7 +26733,7 @@
       <c r="S745" s="17"/>
       <c r="T745" s="17"/>
     </row>
-    <row r="746" spans="1:20" ht="13.5" customHeight="1">
+    <row r="746" spans="1:21" ht="13.5" customHeight="1">
       <c r="A746" s="26">
         <f t="shared" si="11"/>
         <v>687</v>
@@ -26720,7 +26768,7 @@
       <c r="S746" s="17"/>
       <c r="T746" s="17"/>
     </row>
-    <row r="747" spans="1:20" ht="13.5" customHeight="1">
+    <row r="747" spans="1:21" ht="13.5" customHeight="1">
       <c r="A747" s="26">
         <f t="shared" si="11"/>
         <v>688</v>
@@ -26753,7 +26801,7 @@
       <c r="S747" s="17"/>
       <c r="T747" s="17"/>
     </row>
-    <row r="748" spans="1:20" ht="13.5" customHeight="1">
+    <row r="748" spans="1:21" ht="13.5" customHeight="1">
       <c r="A748" s="26">
         <f t="shared" si="11"/>
         <v>689</v>
@@ -26784,7 +26832,7 @@
       <c r="S748" s="17"/>
       <c r="T748" s="17"/>
     </row>
-    <row r="749" spans="1:20" ht="13.5" customHeight="1">
+    <row r="749" spans="1:21" ht="13.5" customHeight="1">
       <c r="A749" s="26">
         <f t="shared" si="11"/>
         <v>690</v>
@@ -26821,7 +26869,7 @@
       <c r="S749" s="17"/>
       <c r="T749" s="17"/>
     </row>
-    <row r="750" spans="1:20" ht="13.5" customHeight="1">
+    <row r="750" spans="1:21" ht="13.5" customHeight="1">
       <c r="A750" s="26">
         <f t="shared" si="11"/>
         <v>691</v>
@@ -26856,7 +26904,7 @@
       <c r="S750" s="17"/>
       <c r="T750" s="17"/>
     </row>
-    <row r="751" spans="1:20" ht="13.5" customHeight="1">
+    <row r="751" spans="1:21" ht="13.5" customHeight="1">
       <c r="A751" s="26">
         <f t="shared" si="11"/>
         <v>692</v>
@@ -26887,7 +26935,7 @@
       <c r="S751" s="17"/>
       <c r="T751" s="17"/>
     </row>
-    <row r="752" spans="1:20" ht="13.5" customHeight="1">
+    <row r="752" spans="1:21" ht="13.5" customHeight="1">
       <c r="A752" s="26">
         <f t="shared" si="11"/>
         <v>693</v>
@@ -38648,7 +38696,7 @@
       <c r="S1104" s="30"/>
       <c r="T1104" s="30"/>
     </row>
-    <row r="1105" spans="1:20" ht="15" customHeight="1">
+    <row r="1105" spans="1:21" ht="15" customHeight="1">
       <c r="A1105" s="26">
         <f t="shared" si="16"/>
         <v>1015</v>
@@ -38681,7 +38729,7 @@
       <c r="S1105" s="30"/>
       <c r="T1105" s="30"/>
     </row>
-    <row r="1106" spans="1:20" ht="15" customHeight="1">
+    <row r="1106" spans="1:21" ht="15" customHeight="1">
       <c r="A1106" s="26">
         <f t="shared" si="16"/>
         <v>1015</v>
@@ -38710,7 +38758,7 @@
       <c r="S1106" s="30"/>
       <c r="T1106" s="30"/>
     </row>
-    <row r="1107" spans="1:20" ht="15" customHeight="1">
+    <row r="1107" spans="1:21" ht="15" customHeight="1">
       <c r="A1107" s="26">
         <f t="shared" si="16"/>
         <v>1016</v>
@@ -38745,7 +38793,7 @@
       <c r="S1107" s="30"/>
       <c r="T1107" s="30"/>
     </row>
-    <row r="1108" spans="1:20" ht="15" customHeight="1">
+    <row r="1108" spans="1:21" ht="15" customHeight="1">
       <c r="A1108" s="26">
         <f t="shared" si="16"/>
         <v>1017</v>
@@ -38776,7 +38824,7 @@
       <c r="S1108" s="30"/>
       <c r="T1108" s="30"/>
     </row>
-    <row r="1109" spans="1:20" ht="15" customHeight="1">
+    <row r="1109" spans="1:21" ht="15" customHeight="1">
       <c r="A1109" s="26">
         <f t="shared" si="16"/>
         <v>1018</v>
@@ -38814,8 +38862,11 @@
       </c>
       <c r="S1109" s="30"/>
       <c r="T1109" s="30"/>
-    </row>
-    <row r="1110" spans="1:20" ht="15" customHeight="1">
+      <c r="U1109" s="37">
+        <v>0.172072843491759</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:21" ht="15" customHeight="1">
       <c r="A1110" s="26">
         <f t="shared" si="16"/>
         <v>1019</v>
@@ -38848,7 +38899,7 @@
       <c r="S1110" s="30"/>
       <c r="T1110" s="30"/>
     </row>
-    <row r="1111" spans="1:20" ht="15" customHeight="1">
+    <row r="1111" spans="1:21" ht="15" customHeight="1">
       <c r="A1111" s="26">
         <f t="shared" si="16"/>
         <v>1019</v>
@@ -38877,7 +38928,7 @@
       <c r="S1111" s="30"/>
       <c r="T1111" s="30"/>
     </row>
-    <row r="1112" spans="1:20" ht="15" customHeight="1">
+    <row r="1112" spans="1:21" ht="15" customHeight="1">
       <c r="A1112" s="26">
         <f t="shared" si="16"/>
         <v>1020</v>
@@ -38912,7 +38963,7 @@
       <c r="S1112" s="30"/>
       <c r="T1112" s="30"/>
     </row>
-    <row r="1113" spans="1:20" ht="15" customHeight="1">
+    <row r="1113" spans="1:21" ht="15" customHeight="1">
       <c r="A1113" s="26">
         <f t="shared" si="16"/>
         <v>1021</v>
@@ -38947,7 +38998,7 @@
       <c r="S1113" s="30"/>
       <c r="T1113" s="30"/>
     </row>
-    <row r="1114" spans="1:20" ht="15" customHeight="1">
+    <row r="1114" spans="1:21" ht="15" customHeight="1">
       <c r="A1114" s="26">
         <f t="shared" si="16"/>
         <v>1022</v>
@@ -38982,7 +39033,7 @@
       <c r="S1114" s="30"/>
       <c r="T1114" s="30"/>
     </row>
-    <row r="1115" spans="1:20" ht="15" customHeight="1">
+    <row r="1115" spans="1:21" ht="15" customHeight="1">
       <c r="A1115" s="26">
         <f t="shared" si="16"/>
         <v>1023</v>
@@ -39017,7 +39068,7 @@
       <c r="S1115" s="30"/>
       <c r="T1115" s="30"/>
     </row>
-    <row r="1116" spans="1:20" ht="15" customHeight="1">
+    <row r="1116" spans="1:21" ht="15" customHeight="1">
       <c r="A1116" s="26">
         <f t="shared" si="16"/>
         <v>1024</v>
@@ -39048,7 +39099,7 @@
       <c r="S1116" s="30"/>
       <c r="T1116" s="30"/>
     </row>
-    <row r="1117" spans="1:20" ht="15" customHeight="1">
+    <row r="1117" spans="1:21" ht="15" customHeight="1">
       <c r="A1117" s="26">
         <f t="shared" si="16"/>
         <v>1025</v>
@@ -39079,7 +39130,7 @@
       <c r="S1117" s="30"/>
       <c r="T1117" s="30"/>
     </row>
-    <row r="1118" spans="1:20" ht="15" customHeight="1">
+    <row r="1118" spans="1:21" ht="15" customHeight="1">
       <c r="A1118" s="26">
         <f t="shared" si="16"/>
         <v>1026</v>
@@ -39112,7 +39163,7 @@
       <c r="S1118" s="30"/>
       <c r="T1118" s="30"/>
     </row>
-    <row r="1119" spans="1:20" ht="15" customHeight="1">
+    <row r="1119" spans="1:21" ht="15" customHeight="1">
       <c r="A1119" s="26">
         <f t="shared" si="16"/>
         <v>1027</v>
@@ -39151,7 +39202,7 @@
       <c r="S1119" s="30"/>
       <c r="T1119" s="30"/>
     </row>
-    <row r="1120" spans="1:20" ht="15" customHeight="1">
+    <row r="1120" spans="1:21" ht="15" customHeight="1">
       <c r="A1120" s="26">
         <f t="shared" ref="A1120:A1183" si="17">IF(OR(F1120="",F1120=""),A1119,A1119+1)</f>
         <v>1028</v>
@@ -41312,7 +41363,7 @@
       <c r="S1184" s="30"/>
       <c r="T1184" s="30"/>
     </row>
-    <row r="1185" spans="1:20" ht="15" customHeight="1">
+    <row r="1185" spans="1:21" ht="15" customHeight="1">
       <c r="A1185" s="26">
         <f t="shared" si="18"/>
         <v>1082</v>
@@ -41343,7 +41394,7 @@
       <c r="S1185" s="30"/>
       <c r="T1185" s="30"/>
     </row>
-    <row r="1186" spans="1:20" ht="15" customHeight="1">
+    <row r="1186" spans="1:21" ht="15" customHeight="1">
       <c r="A1186" s="26">
         <f t="shared" si="18"/>
         <v>1083</v>
@@ -41381,8 +41432,11 @@
       </c>
       <c r="S1186" s="30"/>
       <c r="T1186" s="30"/>
-    </row>
-    <row r="1187" spans="1:20" ht="15" customHeight="1">
+      <c r="U1186" s="37">
+        <v>0.19178571493639801</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:21" ht="15" customHeight="1">
       <c r="A1187" s="26">
         <f t="shared" si="18"/>
         <v>1084</v>
@@ -41419,7 +41473,7 @@
       <c r="S1187" s="30"/>
       <c r="T1187" s="30"/>
     </row>
-    <row r="1188" spans="1:20" ht="15" customHeight="1">
+    <row r="1188" spans="1:21" ht="15" customHeight="1">
       <c r="A1188" s="26">
         <f t="shared" si="18"/>
         <v>1084</v>
@@ -41448,7 +41502,7 @@
       <c r="S1188" s="30"/>
       <c r="T1188" s="30"/>
     </row>
-    <row r="1189" spans="1:20" ht="15" customHeight="1">
+    <row r="1189" spans="1:21" ht="15" customHeight="1">
       <c r="A1189" s="26">
         <f t="shared" si="18"/>
         <v>1085</v>
@@ -41485,7 +41539,7 @@
       <c r="S1189" s="30"/>
       <c r="T1189" s="30"/>
     </row>
-    <row r="1190" spans="1:20" ht="15" customHeight="1">
+    <row r="1190" spans="1:21" ht="15" customHeight="1">
       <c r="A1190" s="26">
         <f t="shared" si="18"/>
         <v>1086</v>
@@ -41516,7 +41570,7 @@
       <c r="S1190" s="30"/>
       <c r="T1190" s="30"/>
     </row>
-    <row r="1191" spans="1:20" ht="15" customHeight="1">
+    <row r="1191" spans="1:21" ht="15" customHeight="1">
       <c r="A1191" s="26">
         <f t="shared" si="18"/>
         <v>1087</v>
@@ -41547,7 +41601,7 @@
       <c r="S1191" s="30"/>
       <c r="T1191" s="30"/>
     </row>
-    <row r="1192" spans="1:20" ht="15" customHeight="1">
+    <row r="1192" spans="1:21" ht="15" customHeight="1">
       <c r="A1192" s="26">
         <f t="shared" si="18"/>
         <v>1088</v>
@@ -41582,7 +41636,7 @@
       <c r="S1192" s="30"/>
       <c r="T1192" s="30"/>
     </row>
-    <row r="1193" spans="1:20" ht="15" customHeight="1">
+    <row r="1193" spans="1:21" ht="15" customHeight="1">
       <c r="A1193" s="26">
         <f t="shared" si="18"/>
         <v>1089</v>
@@ -41613,7 +41667,7 @@
       <c r="S1193" s="30"/>
       <c r="T1193" s="30"/>
     </row>
-    <row r="1194" spans="1:20" ht="15" customHeight="1">
+    <row r="1194" spans="1:21" ht="15" customHeight="1">
       <c r="A1194" s="26">
         <f t="shared" si="18"/>
         <v>1090</v>
@@ -41644,7 +41698,7 @@
       <c r="S1194" s="30"/>
       <c r="T1194" s="30"/>
     </row>
-    <row r="1195" spans="1:20" ht="15" customHeight="1">
+    <row r="1195" spans="1:21" ht="15" customHeight="1">
       <c r="A1195" s="26">
         <f t="shared" si="18"/>
         <v>1091</v>
@@ -41677,7 +41731,7 @@
       <c r="S1195" s="30"/>
       <c r="T1195" s="30"/>
     </row>
-    <row r="1196" spans="1:20" ht="15" customHeight="1">
+    <row r="1196" spans="1:21" ht="15" customHeight="1">
       <c r="A1196" s="26">
         <f t="shared" si="18"/>
         <v>1092</v>
@@ -41708,7 +41762,7 @@
       <c r="S1196" s="30"/>
       <c r="T1196" s="30"/>
     </row>
-    <row r="1197" spans="1:20" ht="15" customHeight="1">
+    <row r="1197" spans="1:21" ht="15" customHeight="1">
       <c r="A1197" s="26">
         <f t="shared" si="18"/>
         <v>1093</v>
@@ -41743,7 +41797,7 @@
       <c r="S1197" s="30"/>
       <c r="T1197" s="30"/>
     </row>
-    <row r="1198" spans="1:20" ht="15" customHeight="1">
+    <row r="1198" spans="1:21" ht="15" customHeight="1">
       <c r="A1198" s="26">
         <f t="shared" si="18"/>
         <v>1094</v>
@@ -41774,7 +41828,7 @@
       <c r="S1198" s="30"/>
       <c r="T1198" s="30"/>
     </row>
-    <row r="1199" spans="1:20" ht="15" customHeight="1">
+    <row r="1199" spans="1:21" ht="15" customHeight="1">
       <c r="A1199" s="26">
         <f t="shared" si="18"/>
         <v>1095</v>
@@ -41809,7 +41863,7 @@
       <c r="S1199" s="30"/>
       <c r="T1199" s="30"/>
     </row>
-    <row r="1200" spans="1:20" ht="15" customHeight="1">
+    <row r="1200" spans="1:21" ht="15" customHeight="1">
       <c r="A1200" s="26">
         <f t="shared" si="18"/>
         <v>1095</v>
@@ -41840,7 +41894,7 @@
       <c r="S1200" s="30"/>
       <c r="T1200" s="30"/>
     </row>
-    <row r="1201" spans="1:20" ht="15" customHeight="1">
+    <row r="1201" spans="1:21" ht="15" customHeight="1">
       <c r="A1201" s="26">
         <f t="shared" si="18"/>
         <v>1096</v>
@@ -41873,7 +41927,7 @@
       <c r="S1201" s="30"/>
       <c r="T1201" s="30"/>
     </row>
-    <row r="1202" spans="1:20" ht="15" customHeight="1">
+    <row r="1202" spans="1:21" ht="15" customHeight="1">
       <c r="A1202" s="26">
         <f t="shared" si="18"/>
         <v>1097</v>
@@ -41904,7 +41958,7 @@
       <c r="S1202" s="30"/>
       <c r="T1202" s="30"/>
     </row>
-    <row r="1203" spans="1:20" ht="15" customHeight="1">
+    <row r="1203" spans="1:21" ht="15" customHeight="1">
       <c r="A1203" s="26">
         <f t="shared" si="18"/>
         <v>1098</v>
@@ -41933,7 +41987,7 @@
       <c r="S1203" s="30"/>
       <c r="T1203" s="30"/>
     </row>
-    <row r="1204" spans="1:20" ht="15" customHeight="1">
+    <row r="1204" spans="1:21" ht="15" customHeight="1">
       <c r="A1204" s="26">
         <f t="shared" si="18"/>
         <v>1099</v>
@@ -41964,7 +42018,7 @@
       <c r="S1204" s="30"/>
       <c r="T1204" s="30"/>
     </row>
-    <row r="1205" spans="1:20" ht="15" customHeight="1">
+    <row r="1205" spans="1:21" ht="15" customHeight="1">
       <c r="A1205" s="26">
         <f t="shared" si="18"/>
         <v>1100</v>
@@ -42004,8 +42058,11 @@
       </c>
       <c r="S1205" s="30"/>
       <c r="T1205" s="30"/>
-    </row>
-    <row r="1206" spans="1:20" ht="15" customHeight="1">
+      <c r="U1205" s="37">
+        <v>1.68213516142382E-2</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:21" ht="15" customHeight="1">
       <c r="A1206" s="26">
         <f t="shared" si="18"/>
         <v>1100</v>
@@ -42036,7 +42093,7 @@
       <c r="S1206" s="30"/>
       <c r="T1206" s="30"/>
     </row>
-    <row r="1207" spans="1:20" ht="15" customHeight="1">
+    <row r="1207" spans="1:21" ht="15" customHeight="1">
       <c r="A1207" s="26">
         <f t="shared" si="18"/>
         <v>1101</v>
@@ -42071,7 +42128,7 @@
       <c r="S1207" s="30"/>
       <c r="T1207" s="30"/>
     </row>
-    <row r="1208" spans="1:20" ht="15" customHeight="1">
+    <row r="1208" spans="1:21" ht="15" customHeight="1">
       <c r="A1208" s="26">
         <f t="shared" si="18"/>
         <v>1102</v>
@@ -42106,7 +42163,7 @@
       <c r="S1208" s="30"/>
       <c r="T1208" s="30"/>
     </row>
-    <row r="1209" spans="1:20" ht="15" customHeight="1">
+    <row r="1209" spans="1:21" ht="15" customHeight="1">
       <c r="A1209" s="26">
         <f t="shared" si="18"/>
         <v>1103</v>
@@ -42141,7 +42198,7 @@
       <c r="S1209" s="30"/>
       <c r="T1209" s="30"/>
     </row>
-    <row r="1210" spans="1:20" ht="15" customHeight="1">
+    <row r="1210" spans="1:21" ht="15" customHeight="1">
       <c r="A1210" s="26">
         <f t="shared" si="18"/>
         <v>1104</v>
@@ -42175,8 +42232,11 @@
       </c>
       <c r="S1210" s="30"/>
       <c r="T1210" s="30"/>
-    </row>
-    <row r="1211" spans="1:20" ht="15" customHeight="1">
+      <c r="U1210" s="37">
+        <v>8.4739171785904302E-2</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:21" ht="15" customHeight="1">
       <c r="A1211" s="26">
         <f t="shared" si="18"/>
         <v>1105</v>
@@ -42209,7 +42269,7 @@
       <c r="S1211" s="30"/>
       <c r="T1211" s="30"/>
     </row>
-    <row r="1212" spans="1:20" ht="15" customHeight="1">
+    <row r="1212" spans="1:21" ht="15" customHeight="1">
       <c r="A1212" s="26">
         <f t="shared" si="18"/>
         <v>1105</v>
@@ -42238,7 +42298,7 @@
       <c r="S1212" s="30"/>
       <c r="T1212" s="30"/>
     </row>
-    <row r="1213" spans="1:20" ht="15" customHeight="1">
+    <row r="1213" spans="1:21" ht="15" customHeight="1">
       <c r="A1213" s="26">
         <f t="shared" si="18"/>
         <v>1106</v>
@@ -42271,7 +42331,7 @@
       <c r="S1213" s="30"/>
       <c r="T1213" s="30"/>
     </row>
-    <row r="1214" spans="1:20" ht="15" customHeight="1">
+    <row r="1214" spans="1:21" ht="15" customHeight="1">
       <c r="A1214" s="26">
         <f t="shared" si="18"/>
         <v>1107</v>
@@ -42302,7 +42362,7 @@
       <c r="S1214" s="30"/>
       <c r="T1214" s="30"/>
     </row>
-    <row r="1215" spans="1:20" ht="15" customHeight="1">
+    <row r="1215" spans="1:21" ht="15" customHeight="1">
       <c r="A1215" s="26">
         <f t="shared" si="18"/>
         <v>1108</v>
@@ -42333,7 +42393,7 @@
       <c r="S1215" s="30"/>
       <c r="T1215" s="30"/>
     </row>
-    <row r="1216" spans="1:20" ht="15" customHeight="1">
+    <row r="1216" spans="1:21" ht="15" customHeight="1">
       <c r="A1216" s="26">
         <f t="shared" si="18"/>
         <v>1109</v>
@@ -42364,7 +42424,7 @@
       <c r="S1216" s="30"/>
       <c r="T1216" s="30"/>
     </row>
-    <row r="1217" spans="1:20" ht="15" customHeight="1">
+    <row r="1217" spans="1:21" ht="15" customHeight="1">
       <c r="A1217" s="26">
         <f t="shared" si="18"/>
         <v>1110</v>
@@ -42395,7 +42455,7 @@
       <c r="S1217" s="30"/>
       <c r="T1217" s="30"/>
     </row>
-    <row r="1218" spans="1:20" ht="15" customHeight="1">
+    <row r="1218" spans="1:21" ht="15" customHeight="1">
       <c r="A1218" s="26">
         <f t="shared" si="18"/>
         <v>1111</v>
@@ -42426,7 +42486,7 @@
       <c r="S1218" s="30"/>
       <c r="T1218" s="30"/>
     </row>
-    <row r="1219" spans="1:20" ht="15" customHeight="1">
+    <row r="1219" spans="1:21" ht="15" customHeight="1">
       <c r="A1219" s="26">
         <f t="shared" si="18"/>
         <v>1112</v>
@@ -42459,7 +42519,7 @@
       <c r="S1219" s="30"/>
       <c r="T1219" s="30"/>
     </row>
-    <row r="1220" spans="1:20" ht="15" customHeight="1">
+    <row r="1220" spans="1:21" ht="15" customHeight="1">
       <c r="A1220" s="26">
         <f t="shared" si="18"/>
         <v>1113</v>
@@ -42490,7 +42550,7 @@
       <c r="S1220" s="30"/>
       <c r="T1220" s="30"/>
     </row>
-    <row r="1221" spans="1:20" ht="15" customHeight="1">
+    <row r="1221" spans="1:21" ht="15" customHeight="1">
       <c r="A1221" s="26">
         <f t="shared" si="18"/>
         <v>1114</v>
@@ -42525,7 +42585,7 @@
       <c r="S1221" s="30"/>
       <c r="T1221" s="30"/>
     </row>
-    <row r="1222" spans="1:20" ht="15" customHeight="1">
+    <row r="1222" spans="1:21" ht="15" customHeight="1">
       <c r="A1222" s="26">
         <f t="shared" si="18"/>
         <v>1115</v>
@@ -42560,7 +42620,7 @@
       <c r="S1222" s="30"/>
       <c r="T1222" s="30"/>
     </row>
-    <row r="1223" spans="1:20" ht="15" customHeight="1">
+    <row r="1223" spans="1:21" ht="15" customHeight="1">
       <c r="A1223" s="26">
         <f t="shared" si="18"/>
         <v>1116</v>
@@ -42597,7 +42657,7 @@
       <c r="S1223" s="30"/>
       <c r="T1223" s="30"/>
     </row>
-    <row r="1224" spans="1:20" ht="15" customHeight="1">
+    <row r="1224" spans="1:21" ht="15" customHeight="1">
       <c r="A1224" s="26">
         <f t="shared" si="18"/>
         <v>1117</v>
@@ -42634,7 +42694,7 @@
       <c r="S1224" s="30"/>
       <c r="T1224" s="30"/>
     </row>
-    <row r="1225" spans="1:20" ht="15" customHeight="1">
+    <row r="1225" spans="1:21" ht="15" customHeight="1">
       <c r="A1225" s="26">
         <f t="shared" si="18"/>
         <v>1118</v>
@@ -42669,7 +42729,7 @@
       <c r="S1225" s="30"/>
       <c r="T1225" s="30"/>
     </row>
-    <row r="1226" spans="1:20" ht="15" customHeight="1">
+    <row r="1226" spans="1:21" ht="15" customHeight="1">
       <c r="A1226" s="26">
         <f t="shared" si="18"/>
         <v>1119</v>
@@ -42704,7 +42764,7 @@
       <c r="S1226" s="30"/>
       <c r="T1226" s="30"/>
     </row>
-    <row r="1227" spans="1:20" ht="15" customHeight="1">
+    <row r="1227" spans="1:21" ht="15" customHeight="1">
       <c r="A1227" s="26">
         <f t="shared" si="18"/>
         <v>1120</v>
@@ -42737,7 +42797,7 @@
       <c r="S1227" s="30"/>
       <c r="T1227" s="30"/>
     </row>
-    <row r="1228" spans="1:20" ht="15" customHeight="1">
+    <row r="1228" spans="1:21" ht="15" customHeight="1">
       <c r="A1228" s="26">
         <f t="shared" si="18"/>
         <v>1121</v>
@@ -42768,7 +42828,7 @@
       <c r="S1228" s="30"/>
       <c r="T1228" s="30"/>
     </row>
-    <row r="1229" spans="1:20" ht="15" customHeight="1">
+    <row r="1229" spans="1:21" ht="15" customHeight="1">
       <c r="A1229" s="26">
         <f t="shared" si="18"/>
         <v>1122</v>
@@ -42806,8 +42866,11 @@
       </c>
       <c r="S1229" s="30"/>
       <c r="T1229" s="30"/>
-    </row>
-    <row r="1230" spans="1:20" ht="15" customHeight="1">
+      <c r="U1229" s="37">
+        <v>0.148794146766627</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:21" ht="15" customHeight="1">
       <c r="A1230" s="26">
         <f t="shared" si="18"/>
         <v>1123</v>
@@ -42842,7 +42905,7 @@
       <c r="S1230" s="30"/>
       <c r="T1230" s="30"/>
     </row>
-    <row r="1231" spans="1:20" ht="15" customHeight="1">
+    <row r="1231" spans="1:21" ht="15" customHeight="1">
       <c r="A1231" s="26">
         <f t="shared" si="18"/>
         <v>1123</v>
@@ -42871,7 +42934,7 @@
       <c r="S1231" s="30"/>
       <c r="T1231" s="30"/>
     </row>
-    <row r="1232" spans="1:20" ht="15" customHeight="1">
+    <row r="1232" spans="1:21" ht="15" customHeight="1">
       <c r="A1232" s="26">
         <f t="shared" si="18"/>
         <v>1124</v>
@@ -44514,7 +44577,7 @@
       <c r="S1280" s="30"/>
       <c r="T1280" s="30"/>
     </row>
-    <row r="1281" spans="1:20" ht="15" customHeight="1">
+    <row r="1281" spans="1:21" ht="15" customHeight="1">
       <c r="A1281" s="26">
         <f t="shared" si="19"/>
         <v>1161</v>
@@ -44545,7 +44608,7 @@
       <c r="S1281" s="30"/>
       <c r="T1281" s="30"/>
     </row>
-    <row r="1282" spans="1:20" ht="15" customHeight="1">
+    <row r="1282" spans="1:21" ht="15" customHeight="1">
       <c r="A1282" s="26">
         <f t="shared" si="19"/>
         <v>1162</v>
@@ -44580,7 +44643,7 @@
       <c r="S1282" s="30"/>
       <c r="T1282" s="30"/>
     </row>
-    <row r="1283" spans="1:20" ht="15" customHeight="1">
+    <row r="1283" spans="1:21" ht="15" customHeight="1">
       <c r="A1283" s="26">
         <f t="shared" si="19"/>
         <v>1163</v>
@@ -44613,7 +44676,7 @@
       <c r="S1283" s="30"/>
       <c r="T1283" s="30"/>
     </row>
-    <row r="1284" spans="1:20" ht="15" customHeight="1">
+    <row r="1284" spans="1:21" ht="15" customHeight="1">
       <c r="A1284" s="26">
         <f t="shared" si="19"/>
         <v>1164</v>
@@ -44644,7 +44707,7 @@
       <c r="S1284" s="30"/>
       <c r="T1284" s="30"/>
     </row>
-    <row r="1285" spans="1:20" ht="15" customHeight="1">
+    <row r="1285" spans="1:21" ht="15" customHeight="1">
       <c r="A1285" s="26">
         <f t="shared" si="19"/>
         <v>1165</v>
@@ -44677,7 +44740,7 @@
       <c r="S1285" s="30"/>
       <c r="T1285" s="30"/>
     </row>
-    <row r="1286" spans="1:20" ht="15" customHeight="1">
+    <row r="1286" spans="1:21" ht="15" customHeight="1">
       <c r="A1286" s="26">
         <f t="shared" si="19"/>
         <v>1166</v>
@@ -44708,7 +44771,7 @@
       <c r="S1286" s="30"/>
       <c r="T1286" s="30"/>
     </row>
-    <row r="1287" spans="1:20" ht="15" customHeight="1">
+    <row r="1287" spans="1:21" ht="15" customHeight="1">
       <c r="A1287" s="26">
         <f t="shared" si="19"/>
         <v>1167</v>
@@ -44743,7 +44806,7 @@
       <c r="S1287" s="30"/>
       <c r="T1287" s="30"/>
     </row>
-    <row r="1288" spans="1:20" ht="15" customHeight="1">
+    <row r="1288" spans="1:21" ht="15" customHeight="1">
       <c r="A1288" s="26">
         <f t="shared" si="19"/>
         <v>1168</v>
@@ -44778,7 +44841,7 @@
       <c r="S1288" s="30"/>
       <c r="T1288" s="30"/>
     </row>
-    <row r="1289" spans="1:20" ht="15" customHeight="1">
+    <row r="1289" spans="1:21" ht="15" customHeight="1">
       <c r="A1289" s="26">
         <f t="shared" si="19"/>
         <v>1168</v>
@@ -44809,7 +44872,7 @@
       <c r="S1289" s="30"/>
       <c r="T1289" s="30"/>
     </row>
-    <row r="1290" spans="1:20" ht="15" customHeight="1">
+    <row r="1290" spans="1:21" ht="15" customHeight="1">
       <c r="A1290" s="26">
         <f t="shared" si="19"/>
         <v>1169</v>
@@ -44840,7 +44903,7 @@
       <c r="S1290" s="30"/>
       <c r="T1290" s="30"/>
     </row>
-    <row r="1291" spans="1:20" ht="15" customHeight="1">
+    <row r="1291" spans="1:21" ht="15" customHeight="1">
       <c r="A1291" s="26">
         <f t="shared" si="19"/>
         <v>1170</v>
@@ -44871,7 +44934,7 @@
       <c r="S1291" s="30"/>
       <c r="T1291" s="30"/>
     </row>
-    <row r="1292" spans="1:20" ht="15" customHeight="1">
+    <row r="1292" spans="1:21" ht="15" customHeight="1">
       <c r="A1292" s="26">
         <f t="shared" si="19"/>
         <v>1170</v>
@@ -44906,7 +44969,7 @@
       </c>
       <c r="T1292" s="30"/>
     </row>
-    <row r="1293" spans="1:20" ht="15" customHeight="1">
+    <row r="1293" spans="1:21" ht="15" customHeight="1">
       <c r="A1293" s="26">
         <f t="shared" si="19"/>
         <v>1171</v>
@@ -44939,7 +45002,7 @@
       <c r="S1293" s="30"/>
       <c r="T1293" s="30"/>
     </row>
-    <row r="1294" spans="1:20" ht="15" customHeight="1">
+    <row r="1294" spans="1:21" ht="15" customHeight="1">
       <c r="A1294" s="26">
         <f t="shared" si="19"/>
         <v>1171</v>
@@ -44968,7 +45031,7 @@
       <c r="S1294" s="30"/>
       <c r="T1294" s="30"/>
     </row>
-    <row r="1295" spans="1:20" ht="15" customHeight="1">
+    <row r="1295" spans="1:21" ht="15" customHeight="1">
       <c r="A1295" s="26">
         <f t="shared" si="19"/>
         <v>1172</v>
@@ -45008,8 +45071,11 @@
       <c r="R1295" s="30"/>
       <c r="S1295" s="30"/>
       <c r="T1295" s="30"/>
-    </row>
-    <row r="1296" spans="1:20" ht="15" customHeight="1">
+      <c r="U1295" s="37">
+        <v>0.15023310959771399</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:21" ht="15" customHeight="1">
       <c r="A1296" s="26">
         <f t="shared" si="19"/>
         <v>1173</v>
@@ -46098,7 +46164,7 @@
       <c r="S1328" s="30"/>
       <c r="T1328" s="30"/>
     </row>
-    <row r="1329" spans="1:20" ht="15" customHeight="1">
+    <row r="1329" spans="1:21" ht="15" customHeight="1">
       <c r="A1329" s="26">
         <f t="shared" si="20"/>
         <v>1203</v>
@@ -46135,7 +46201,7 @@
       <c r="S1329" s="30"/>
       <c r="T1329" s="30"/>
     </row>
-    <row r="1330" spans="1:20" ht="15" customHeight="1">
+    <row r="1330" spans="1:21" ht="15" customHeight="1">
       <c r="A1330" s="26">
         <f t="shared" si="20"/>
         <v>1204</v>
@@ -46168,7 +46234,7 @@
       <c r="S1330" s="30"/>
       <c r="T1330" s="30"/>
     </row>
-    <row r="1331" spans="1:20" ht="15" customHeight="1">
+    <row r="1331" spans="1:21" ht="15" customHeight="1">
       <c r="A1331" s="26">
         <f t="shared" si="20"/>
         <v>1204</v>
@@ -46197,7 +46263,7 @@
       <c r="S1331" s="30"/>
       <c r="T1331" s="30"/>
     </row>
-    <row r="1332" spans="1:20" ht="15" customHeight="1">
+    <row r="1332" spans="1:21" ht="15" customHeight="1">
       <c r="A1332" s="26">
         <f t="shared" si="20"/>
         <v>1205</v>
@@ -46232,7 +46298,7 @@
       <c r="S1332" s="30"/>
       <c r="T1332" s="30"/>
     </row>
-    <row r="1333" spans="1:20" ht="15" customHeight="1">
+    <row r="1333" spans="1:21" ht="15" customHeight="1">
       <c r="A1333" s="26">
         <f t="shared" si="20"/>
         <v>1206</v>
@@ -46269,7 +46335,7 @@
       <c r="S1333" s="30"/>
       <c r="T1333" s="30"/>
     </row>
-    <row r="1334" spans="1:20" ht="15" customHeight="1">
+    <row r="1334" spans="1:21" ht="15" customHeight="1">
       <c r="A1334" s="26">
         <f t="shared" si="20"/>
         <v>1206</v>
@@ -46298,7 +46364,7 @@
       <c r="S1334" s="30"/>
       <c r="T1334" s="30"/>
     </row>
-    <row r="1335" spans="1:20" ht="15" customHeight="1">
+    <row r="1335" spans="1:21" ht="15" customHeight="1">
       <c r="A1335" s="26">
         <f t="shared" si="20"/>
         <v>1207</v>
@@ -46335,7 +46401,7 @@
       <c r="S1335" s="30"/>
       <c r="T1335" s="30"/>
     </row>
-    <row r="1336" spans="1:20" ht="15" customHeight="1">
+    <row r="1336" spans="1:21" ht="15" customHeight="1">
       <c r="A1336" s="26">
         <f t="shared" si="20"/>
         <v>1208</v>
@@ -46368,7 +46434,7 @@
       <c r="S1336" s="30"/>
       <c r="T1336" s="30"/>
     </row>
-    <row r="1337" spans="1:20" ht="15" customHeight="1">
+    <row r="1337" spans="1:21" ht="15" customHeight="1">
       <c r="A1337" s="26">
         <f t="shared" si="20"/>
         <v>1208</v>
@@ -46397,7 +46463,7 @@
       <c r="S1337" s="30"/>
       <c r="T1337" s="30"/>
     </row>
-    <row r="1338" spans="1:20" ht="15" customHeight="1">
+    <row r="1338" spans="1:21" ht="15" customHeight="1">
       <c r="A1338" s="26">
         <f t="shared" si="20"/>
         <v>1209</v>
@@ -46434,7 +46500,7 @@
       <c r="S1338" s="30"/>
       <c r="T1338" s="30"/>
     </row>
-    <row r="1339" spans="1:20" ht="15" customHeight="1">
+    <row r="1339" spans="1:21" ht="15" customHeight="1">
       <c r="A1339" s="26">
         <f t="shared" si="20"/>
         <v>1210</v>
@@ -46467,7 +46533,7 @@
       <c r="S1339" s="30"/>
       <c r="T1339" s="30"/>
     </row>
-    <row r="1340" spans="1:20" ht="15" customHeight="1">
+    <row r="1340" spans="1:21" ht="15" customHeight="1">
       <c r="A1340" s="26">
         <f t="shared" si="20"/>
         <v>1211</v>
@@ -46498,7 +46564,7 @@
       <c r="S1340" s="30"/>
       <c r="T1340" s="30"/>
     </row>
-    <row r="1341" spans="1:20" ht="15" customHeight="1">
+    <row r="1341" spans="1:21" ht="15" customHeight="1">
       <c r="A1341" s="26">
         <f t="shared" si="20"/>
         <v>1212</v>
@@ -46529,7 +46595,7 @@
       <c r="S1341" s="30"/>
       <c r="T1341" s="30"/>
     </row>
-    <row r="1342" spans="1:20" ht="15" customHeight="1">
+    <row r="1342" spans="1:21" ht="15" customHeight="1">
       <c r="A1342" s="26">
         <f t="shared" si="20"/>
         <v>1213</v>
@@ -46569,8 +46635,11 @@
       <c r="R1342" s="30"/>
       <c r="S1342" s="30"/>
       <c r="T1342" s="30"/>
-    </row>
-    <row r="1343" spans="1:20" ht="15" customHeight="1">
+      <c r="U1342" s="37">
+        <v>9.7282674747586104E-2</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:21" ht="15" customHeight="1">
       <c r="A1343" s="26">
         <f t="shared" si="20"/>
         <v>1214</v>
@@ -46603,7 +46672,7 @@
       <c r="S1343" s="30"/>
       <c r="T1343" s="30"/>
     </row>
-    <row r="1344" spans="1:20" ht="15" customHeight="1">
+    <row r="1344" spans="1:21" ht="15" customHeight="1">
       <c r="A1344" s="26">
         <f t="shared" si="20"/>
         <v>1215</v>
@@ -46634,7 +46703,7 @@
       <c r="S1344" s="30"/>
       <c r="T1344" s="30"/>
     </row>
-    <row r="1345" spans="1:20" ht="15" customHeight="1">
+    <row r="1345" spans="1:21" ht="15" customHeight="1">
       <c r="A1345" s="26">
         <f t="shared" si="20"/>
         <v>1216</v>
@@ -46663,7 +46732,7 @@
       <c r="S1345" s="30"/>
       <c r="T1345" s="30"/>
     </row>
-    <row r="1346" spans="1:20" ht="15" customHeight="1">
+    <row r="1346" spans="1:21" ht="15" customHeight="1">
       <c r="A1346" s="26">
         <f t="shared" si="20"/>
         <v>1216</v>
@@ -46698,7 +46767,7 @@
       </c>
       <c r="T1346" s="30"/>
     </row>
-    <row r="1347" spans="1:20" ht="15" customHeight="1">
+    <row r="1347" spans="1:21" ht="15" customHeight="1">
       <c r="A1347" s="26">
         <f t="shared" si="20"/>
         <v>1217</v>
@@ -46731,7 +46800,7 @@
       <c r="S1347" s="30"/>
       <c r="T1347" s="30"/>
     </row>
-    <row r="1348" spans="1:20" ht="15" customHeight="1">
+    <row r="1348" spans="1:21" ht="15" customHeight="1">
       <c r="A1348" s="26">
         <f t="shared" si="20"/>
         <v>1218</v>
@@ -46766,7 +46835,7 @@
       <c r="S1348" s="30"/>
       <c r="T1348" s="30"/>
     </row>
-    <row r="1349" spans="1:20" ht="15" customHeight="1">
+    <row r="1349" spans="1:21" ht="15" customHeight="1">
       <c r="A1349" s="26">
         <f t="shared" si="20"/>
         <v>1219</v>
@@ -46803,7 +46872,7 @@
       <c r="S1349" s="30"/>
       <c r="T1349" s="30"/>
     </row>
-    <row r="1350" spans="1:20" ht="15" customHeight="1">
+    <row r="1350" spans="1:21" ht="15" customHeight="1">
       <c r="A1350" s="26">
         <f t="shared" si="20"/>
         <v>1220</v>
@@ -46838,7 +46907,7 @@
       <c r="S1350" s="30"/>
       <c r="T1350" s="30"/>
     </row>
-    <row r="1351" spans="1:20" ht="15" customHeight="1">
+    <row r="1351" spans="1:21" ht="15" customHeight="1">
       <c r="A1351" s="26">
         <f t="shared" si="20"/>
         <v>1221</v>
@@ -46873,7 +46942,7 @@
       <c r="S1351" s="30"/>
       <c r="T1351" s="30"/>
     </row>
-    <row r="1352" spans="1:20" ht="15" customHeight="1">
+    <row r="1352" spans="1:21" ht="15" customHeight="1">
       <c r="A1352" s="26">
         <f t="shared" si="20"/>
         <v>1222</v>
@@ -46908,7 +46977,7 @@
       <c r="S1352" s="30"/>
       <c r="T1352" s="30"/>
     </row>
-    <row r="1353" spans="1:20" ht="15" customHeight="1">
+    <row r="1353" spans="1:21" ht="15" customHeight="1">
       <c r="A1353" s="26">
         <f t="shared" si="20"/>
         <v>1223</v>
@@ -46943,7 +47012,7 @@
       <c r="S1353" s="30"/>
       <c r="T1353" s="30"/>
     </row>
-    <row r="1354" spans="1:20" ht="15" customHeight="1">
+    <row r="1354" spans="1:21" ht="15" customHeight="1">
       <c r="A1354" s="26">
         <f t="shared" si="20"/>
         <v>1224</v>
@@ -46976,7 +47045,7 @@
       <c r="S1354" s="30"/>
       <c r="T1354" s="30"/>
     </row>
-    <row r="1355" spans="1:20" ht="15" customHeight="1">
+    <row r="1355" spans="1:21" ht="15" customHeight="1">
       <c r="A1355" s="26">
         <f t="shared" si="20"/>
         <v>1224</v>
@@ -47011,7 +47080,7 @@
       </c>
       <c r="T1355" s="30"/>
     </row>
-    <row r="1356" spans="1:20" ht="15" customHeight="1">
+    <row r="1356" spans="1:21" ht="15" customHeight="1">
       <c r="A1356" s="26">
         <f t="shared" si="20"/>
         <v>1225</v>
@@ -47051,8 +47120,9 @@
         <v>47</v>
       </c>
       <c r="T1356" s="30"/>
-    </row>
-    <row r="1357" spans="1:20" ht="15" customHeight="1">
+      <c r="U1356" s="37"/>
+    </row>
+    <row r="1357" spans="1:21" ht="15" customHeight="1">
       <c r="A1357" s="26">
         <f t="shared" si="20"/>
         <v>1226</v>
@@ -47087,7 +47157,7 @@
       <c r="S1357" s="30"/>
       <c r="T1357" s="30"/>
     </row>
-    <row r="1358" spans="1:20" ht="15" customHeight="1">
+    <row r="1358" spans="1:21" ht="15" customHeight="1">
       <c r="A1358" s="26">
         <f t="shared" si="20"/>
         <v>1227</v>
@@ -47122,7 +47192,7 @@
       <c r="S1358" s="30"/>
       <c r="T1358" s="30"/>
     </row>
-    <row r="1359" spans="1:20" ht="15" customHeight="1">
+    <row r="1359" spans="1:21" ht="15" customHeight="1">
       <c r="A1359" s="26">
         <f t="shared" si="20"/>
         <v>1227</v>
@@ -47153,7 +47223,7 @@
       <c r="S1359" s="30"/>
       <c r="T1359" s="30"/>
     </row>
-    <row r="1360" spans="1:20" ht="15" customHeight="1">
+    <row r="1360" spans="1:21" ht="15" customHeight="1">
       <c r="A1360" s="26">
         <f t="shared" si="20"/>
         <v>1228</v>
@@ -47716,7 +47786,7 @@
       <c r="S1376" s="30"/>
       <c r="T1376" s="30"/>
     </row>
-    <row r="1377" spans="1:20" ht="15" customHeight="1">
+    <row r="1377" spans="1:21" ht="15" customHeight="1">
       <c r="A1377" s="26">
         <f t="shared" si="21"/>
         <v>1240</v>
@@ -47753,7 +47823,7 @@
       <c r="S1377" s="30"/>
       <c r="T1377" s="30"/>
     </row>
-    <row r="1378" spans="1:20" ht="15" customHeight="1">
+    <row r="1378" spans="1:21" ht="15" customHeight="1">
       <c r="A1378" s="26">
         <f t="shared" si="21"/>
         <v>1241</v>
@@ -47792,7 +47862,7 @@
       <c r="S1378" s="30"/>
       <c r="T1378" s="30"/>
     </row>
-    <row r="1379" spans="1:20" ht="15" customHeight="1">
+    <row r="1379" spans="1:21" ht="15" customHeight="1">
       <c r="A1379" s="26">
         <f t="shared" si="21"/>
         <v>1242</v>
@@ -47825,7 +47895,7 @@
       <c r="S1379" s="30"/>
       <c r="T1379" s="30"/>
     </row>
-    <row r="1380" spans="1:20" ht="15" customHeight="1">
+    <row r="1380" spans="1:21" ht="15" customHeight="1">
       <c r="A1380" s="26">
         <f t="shared" si="21"/>
         <v>1243</v>
@@ -47856,7 +47926,7 @@
       <c r="S1380" s="30"/>
       <c r="T1380" s="30"/>
     </row>
-    <row r="1381" spans="1:20" ht="15" customHeight="1">
+    <row r="1381" spans="1:21" ht="15" customHeight="1">
       <c r="A1381" s="26">
         <f t="shared" si="21"/>
         <v>1244</v>
@@ -47893,7 +47963,7 @@
       <c r="S1381" s="30"/>
       <c r="T1381" s="30"/>
     </row>
-    <row r="1382" spans="1:20" ht="15" customHeight="1">
+    <row r="1382" spans="1:21" ht="15" customHeight="1">
       <c r="A1382" s="26">
         <f t="shared" si="21"/>
         <v>1244</v>
@@ -47924,7 +47994,7 @@
       <c r="S1382" s="30"/>
       <c r="T1382" s="30"/>
     </row>
-    <row r="1383" spans="1:20" ht="15" customHeight="1">
+    <row r="1383" spans="1:21" ht="15" customHeight="1">
       <c r="A1383" s="26">
         <f t="shared" si="21"/>
         <v>1245</v>
@@ -47959,7 +48029,7 @@
       <c r="S1383" s="30"/>
       <c r="T1383" s="30"/>
     </row>
-    <row r="1384" spans="1:20" ht="15" customHeight="1">
+    <row r="1384" spans="1:21" ht="15" customHeight="1">
       <c r="A1384" s="26">
         <f t="shared" si="21"/>
         <v>1246</v>
@@ -47994,7 +48064,7 @@
       <c r="S1384" s="30"/>
       <c r="T1384" s="30"/>
     </row>
-    <row r="1385" spans="1:20" ht="15" customHeight="1">
+    <row r="1385" spans="1:21" ht="15" customHeight="1">
       <c r="A1385" s="26">
         <f t="shared" si="21"/>
         <v>1247</v>
@@ -48036,8 +48106,11 @@
       </c>
       <c r="S1385" s="30"/>
       <c r="T1385" s="30"/>
-    </row>
-    <row r="1386" spans="1:20" ht="15" customHeight="1">
+      <c r="U1385" s="37">
+        <v>0.11459250821766399</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:21" ht="15" customHeight="1">
       <c r="A1386" s="26">
         <f t="shared" si="21"/>
         <v>1247</v>
@@ -48066,7 +48139,7 @@
       <c r="S1386" s="30"/>
       <c r="T1386" s="30"/>
     </row>
-    <row r="1387" spans="1:20" ht="15" customHeight="1">
+    <row r="1387" spans="1:21" ht="15" customHeight="1">
       <c r="A1387" s="26">
         <f t="shared" si="21"/>
         <v>1248</v>
@@ -48105,7 +48178,7 @@
       <c r="S1387" s="30"/>
       <c r="T1387" s="30"/>
     </row>
-    <row r="1388" spans="1:20" ht="15" customHeight="1">
+    <row r="1388" spans="1:21" ht="15" customHeight="1">
       <c r="A1388" s="26">
         <f t="shared" si="21"/>
         <v>1248</v>
@@ -48134,7 +48207,7 @@
       <c r="S1388" s="30"/>
       <c r="T1388" s="30"/>
     </row>
-    <row r="1389" spans="1:20" ht="15" customHeight="1">
+    <row r="1389" spans="1:21" ht="15" customHeight="1">
       <c r="A1389" s="26">
         <f t="shared" si="21"/>
         <v>1249</v>
@@ -48167,7 +48240,7 @@
       <c r="S1389" s="30"/>
       <c r="T1389" s="30"/>
     </row>
-    <row r="1390" spans="1:20" ht="15" customHeight="1">
+    <row r="1390" spans="1:21" ht="15" customHeight="1">
       <c r="A1390" s="26">
         <f t="shared" si="21"/>
         <v>1250</v>
@@ -48198,7 +48271,7 @@
       <c r="S1390" s="30"/>
       <c r="T1390" s="30"/>
     </row>
-    <row r="1391" spans="1:20" ht="15" customHeight="1">
+    <row r="1391" spans="1:21" ht="15" customHeight="1">
       <c r="A1391" s="26">
         <f t="shared" si="21"/>
         <v>1251</v>
@@ -48229,7 +48302,7 @@
       <c r="S1391" s="30"/>
       <c r="T1391" s="30"/>
     </row>
-    <row r="1392" spans="1:20" ht="15" customHeight="1">
+    <row r="1392" spans="1:21" ht="15" customHeight="1">
       <c r="A1392" s="26">
         <f t="shared" si="21"/>
         <v>1252</v>
@@ -48260,7 +48333,7 @@
       <c r="S1392" s="30"/>
       <c r="T1392" s="30"/>
     </row>
-    <row r="1393" spans="1:20" ht="15" customHeight="1">
+    <row r="1393" spans="1:21" ht="15" customHeight="1">
       <c r="A1393" s="26">
         <f t="shared" si="21"/>
         <v>1253</v>
@@ -48297,7 +48370,7 @@
       <c r="S1393" s="30"/>
       <c r="T1393" s="30"/>
     </row>
-    <row r="1394" spans="1:20" ht="15" customHeight="1">
+    <row r="1394" spans="1:21" ht="15" customHeight="1">
       <c r="A1394" s="26">
         <f t="shared" si="21"/>
         <v>1253</v>
@@ -48328,7 +48401,7 @@
       <c r="S1394" s="30"/>
       <c r="T1394" s="30"/>
     </row>
-    <row r="1395" spans="1:20" ht="15" customHeight="1">
+    <row r="1395" spans="1:21" ht="15" customHeight="1">
       <c r="A1395" s="26">
         <f t="shared" si="21"/>
         <v>1254</v>
@@ -48359,7 +48432,7 @@
       <c r="S1395" s="30"/>
       <c r="T1395" s="30"/>
     </row>
-    <row r="1396" spans="1:20" ht="15" customHeight="1">
+    <row r="1396" spans="1:21" ht="15" customHeight="1">
       <c r="A1396" s="26">
         <f t="shared" si="21"/>
         <v>1255</v>
@@ -48392,7 +48465,7 @@
       <c r="S1396" s="30"/>
       <c r="T1396" s="30"/>
     </row>
-    <row r="1397" spans="1:20" ht="15" customHeight="1">
+    <row r="1397" spans="1:21" ht="15" customHeight="1">
       <c r="A1397" s="26">
         <f t="shared" si="21"/>
         <v>1255</v>
@@ -48421,7 +48494,7 @@
       <c r="S1397" s="30"/>
       <c r="T1397" s="30"/>
     </row>
-    <row r="1398" spans="1:20" ht="15" customHeight="1">
+    <row r="1398" spans="1:21" ht="15" customHeight="1">
       <c r="A1398" s="26">
         <f t="shared" si="21"/>
         <v>1256</v>
@@ -48455,8 +48528,11 @@
       <c r="R1398" s="30"/>
       <c r="S1398" s="30"/>
       <c r="T1398" s="30"/>
-    </row>
-    <row r="1399" spans="1:20" ht="15" customHeight="1">
+      <c r="U1398" s="37">
+        <v>0.27604661066046898</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:21" ht="15" customHeight="1">
       <c r="A1399" s="26">
         <f t="shared" si="21"/>
         <v>1256</v>
@@ -48487,7 +48563,7 @@
       <c r="S1399" s="30"/>
       <c r="T1399" s="30"/>
     </row>
-    <row r="1400" spans="1:20" ht="15" customHeight="1">
+    <row r="1400" spans="1:21" ht="15" customHeight="1">
       <c r="A1400" s="26">
         <f t="shared" si="21"/>
         <v>1256</v>
@@ -48522,7 +48598,7 @@
       <c r="S1400" s="30"/>
       <c r="T1400" s="30"/>
     </row>
-    <row r="1401" spans="1:20" ht="15" customHeight="1">
+    <row r="1401" spans="1:21" ht="15" customHeight="1">
       <c r="A1401" s="26">
         <f t="shared" si="21"/>
         <v>1257</v>
@@ -48551,7 +48627,7 @@
       <c r="S1401" s="30"/>
       <c r="T1401" s="30"/>
     </row>
-    <row r="1402" spans="1:20" ht="15" customHeight="1">
+    <row r="1402" spans="1:21" ht="15" customHeight="1">
       <c r="A1402" s="26">
         <f t="shared" si="21"/>
         <v>1258</v>
@@ -48586,7 +48662,7 @@
       <c r="S1402" s="30"/>
       <c r="T1402" s="30"/>
     </row>
-    <row r="1403" spans="1:20" ht="15" customHeight="1">
+    <row r="1403" spans="1:21" ht="15" customHeight="1">
       <c r="A1403" s="26">
         <f t="shared" si="21"/>
         <v>1259</v>
@@ -48617,7 +48693,7 @@
       <c r="S1403" s="30"/>
       <c r="T1403" s="30"/>
     </row>
-    <row r="1404" spans="1:20" ht="15" customHeight="1">
+    <row r="1404" spans="1:21" ht="15" customHeight="1">
       <c r="A1404" s="26">
         <f t="shared" si="21"/>
         <v>1260</v>
@@ -48648,7 +48724,7 @@
       <c r="S1404" s="30"/>
       <c r="T1404" s="30"/>
     </row>
-    <row r="1405" spans="1:20" ht="15" customHeight="1">
+    <row r="1405" spans="1:21" ht="15" customHeight="1">
       <c r="A1405" s="26">
         <f t="shared" si="21"/>
         <v>1261</v>
@@ -48687,7 +48763,7 @@
       </c>
       <c r="T1405" s="30"/>
     </row>
-    <row r="1406" spans="1:20" ht="15" customHeight="1">
+    <row r="1406" spans="1:21" ht="15" customHeight="1">
       <c r="A1406" s="26">
         <f t="shared" si="21"/>
         <v>1262</v>
@@ -48724,7 +48800,7 @@
       <c r="S1406" s="30"/>
       <c r="T1406" s="30"/>
     </row>
-    <row r="1407" spans="1:20" ht="15" customHeight="1">
+    <row r="1407" spans="1:21" ht="15" customHeight="1">
       <c r="A1407" s="26">
         <f t="shared" si="21"/>
         <v>1262</v>
@@ -48753,7 +48829,7 @@
       <c r="S1407" s="30"/>
       <c r="T1407" s="30"/>
     </row>
-    <row r="1408" spans="1:20" ht="15" customHeight="1">
+    <row r="1408" spans="1:21" ht="15" customHeight="1">
       <c r="A1408" s="26">
         <f t="shared" si="21"/>
         <v>1263</v>
@@ -50428,7 +50504,7 @@
       <c r="S1456" s="30"/>
       <c r="T1456" s="30"/>
     </row>
-    <row r="1457" spans="1:20" ht="15" customHeight="1">
+    <row r="1457" spans="1:21" ht="15" customHeight="1">
       <c r="A1457" s="26">
         <f t="shared" si="22"/>
         <v>1303</v>
@@ -50459,7 +50535,7 @@
       <c r="S1457" s="30"/>
       <c r="T1457" s="30"/>
     </row>
-    <row r="1458" spans="1:20" ht="15" customHeight="1">
+    <row r="1458" spans="1:21" ht="15" customHeight="1">
       <c r="A1458" s="26">
         <f t="shared" si="22"/>
         <v>1304</v>
@@ -50490,7 +50566,7 @@
       <c r="S1458" s="30"/>
       <c r="T1458" s="30"/>
     </row>
-    <row r="1459" spans="1:20" ht="15" customHeight="1">
+    <row r="1459" spans="1:21" ht="15" customHeight="1">
       <c r="A1459" s="26">
         <f t="shared" si="22"/>
         <v>1305</v>
@@ -50525,7 +50601,7 @@
       <c r="S1459" s="30"/>
       <c r="T1459" s="30"/>
     </row>
-    <row r="1460" spans="1:20" ht="15" customHeight="1">
+    <row r="1460" spans="1:21" ht="15" customHeight="1">
       <c r="A1460" s="26">
         <f t="shared" si="22"/>
         <v>1306</v>
@@ -50564,7 +50640,7 @@
       <c r="S1460" s="30"/>
       <c r="T1460" s="30"/>
     </row>
-    <row r="1461" spans="1:20" ht="15" customHeight="1">
+    <row r="1461" spans="1:21" ht="15" customHeight="1">
       <c r="A1461" s="26">
         <f t="shared" si="22"/>
         <v>1306</v>
@@ -50593,7 +50669,7 @@
       <c r="S1461" s="30"/>
       <c r="T1461" s="30"/>
     </row>
-    <row r="1462" spans="1:20" ht="15" customHeight="1">
+    <row r="1462" spans="1:21" ht="15" customHeight="1">
       <c r="A1462" s="26">
         <f t="shared" si="22"/>
         <v>1307</v>
@@ -50631,8 +50707,11 @@
       </c>
       <c r="S1462" s="30"/>
       <c r="T1462" s="30"/>
-    </row>
-    <row r="1463" spans="1:20" ht="15" customHeight="1">
+      <c r="U1462" s="37">
+        <v>0.181337353980843</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:21" ht="15" customHeight="1">
       <c r="A1463" s="26">
         <f t="shared" si="22"/>
         <v>1308</v>
@@ -50665,7 +50744,7 @@
       <c r="S1463" s="30"/>
       <c r="T1463" s="30"/>
     </row>
-    <row r="1464" spans="1:20" ht="15" customHeight="1">
+    <row r="1464" spans="1:21" ht="15" customHeight="1">
       <c r="A1464" s="26">
         <f t="shared" si="22"/>
         <v>1308</v>
@@ -50694,7 +50773,7 @@
       <c r="S1464" s="30"/>
       <c r="T1464" s="30"/>
     </row>
-    <row r="1465" spans="1:20" ht="15" customHeight="1">
+    <row r="1465" spans="1:21" ht="15" customHeight="1">
       <c r="A1465" s="26">
         <f t="shared" si="22"/>
         <v>1309</v>
@@ -50729,7 +50808,7 @@
       <c r="S1465" s="30"/>
       <c r="T1465" s="30"/>
     </row>
-    <row r="1466" spans="1:20" ht="15" customHeight="1">
+    <row r="1466" spans="1:21" ht="15" customHeight="1">
       <c r="A1466" s="26">
         <f t="shared" si="22"/>
         <v>1310</v>
@@ -50760,7 +50839,7 @@
       <c r="S1466" s="30"/>
       <c r="T1466" s="30"/>
     </row>
-    <row r="1467" spans="1:20" ht="15" customHeight="1">
+    <row r="1467" spans="1:21" ht="15" customHeight="1">
       <c r="A1467" s="26">
         <f t="shared" si="22"/>
         <v>1311</v>
@@ -50797,7 +50876,7 @@
       <c r="S1467" s="30"/>
       <c r="T1467" s="30"/>
     </row>
-    <row r="1468" spans="1:20" ht="15" customHeight="1">
+    <row r="1468" spans="1:21" ht="15" customHeight="1">
       <c r="A1468" s="26">
         <f t="shared" si="22"/>
         <v>1311</v>
@@ -50830,7 +50909,7 @@
       <c r="S1468" s="30"/>
       <c r="T1468" s="30"/>
     </row>
-    <row r="1469" spans="1:20" ht="15" customHeight="1">
+    <row r="1469" spans="1:21" ht="15" customHeight="1">
       <c r="A1469" s="26">
         <f t="shared" si="22"/>
         <v>1312</v>
@@ -50863,7 +50942,7 @@
       <c r="S1469" s="30"/>
       <c r="T1469" s="30"/>
     </row>
-    <row r="1470" spans="1:20" ht="15" customHeight="1">
+    <row r="1470" spans="1:21" ht="15" customHeight="1">
       <c r="A1470" s="26">
         <f t="shared" si="22"/>
         <v>1313</v>
@@ -50894,7 +50973,7 @@
       <c r="S1470" s="30"/>
       <c r="T1470" s="30"/>
     </row>
-    <row r="1471" spans="1:20" ht="15" customHeight="1">
+    <row r="1471" spans="1:21" ht="15" customHeight="1">
       <c r="A1471" s="26">
         <f t="shared" si="22"/>
         <v>1314</v>
@@ -50929,7 +51008,7 @@
       <c r="S1471" s="30"/>
       <c r="T1471" s="30"/>
     </row>
-    <row r="1472" spans="1:20" ht="15" customHeight="1">
+    <row r="1472" spans="1:21" ht="15" customHeight="1">
       <c r="A1472" s="26">
         <f t="shared" si="22"/>
         <v>1315</v>
@@ -51502,7 +51581,7 @@
       <c r="S1488" s="30"/>
       <c r="T1488" s="30"/>
     </row>
-    <row r="1489" spans="1:20" ht="15" customHeight="1">
+    <row r="1489" spans="1:21" ht="15" customHeight="1">
       <c r="A1489" s="26">
         <f t="shared" si="22"/>
         <v>1329</v>
@@ -51537,7 +51616,7 @@
       <c r="S1489" s="30"/>
       <c r="T1489" s="30"/>
     </row>
-    <row r="1490" spans="1:20" ht="15" customHeight="1">
+    <row r="1490" spans="1:21" ht="15" customHeight="1">
       <c r="A1490" s="26">
         <f t="shared" si="22"/>
         <v>1330</v>
@@ -51575,8 +51654,11 @@
       </c>
       <c r="S1490" s="30"/>
       <c r="T1490" s="30"/>
-    </row>
-    <row r="1491" spans="1:20" ht="15" customHeight="1">
+      <c r="U1490" s="37">
+        <v>0.122410464203298</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:21" ht="15" customHeight="1">
       <c r="A1491" s="26">
         <f t="shared" si="22"/>
         <v>1331</v>
@@ -51605,7 +51687,7 @@
       <c r="S1491" s="30"/>
       <c r="T1491" s="30"/>
     </row>
-    <row r="1492" spans="1:20" ht="15" customHeight="1">
+    <row r="1492" spans="1:21" ht="15" customHeight="1">
       <c r="A1492" s="26">
         <f t="shared" si="22"/>
         <v>1332</v>
@@ -51638,7 +51720,7 @@
       <c r="S1492" s="30"/>
       <c r="T1492" s="30"/>
     </row>
-    <row r="1493" spans="1:20" ht="15" customHeight="1">
+    <row r="1493" spans="1:21" ht="15" customHeight="1">
       <c r="A1493" s="26">
         <f t="shared" si="22"/>
         <v>1333</v>
@@ -51671,7 +51753,7 @@
       <c r="S1493" s="30"/>
       <c r="T1493" s="30"/>
     </row>
-    <row r="1494" spans="1:20" ht="15" customHeight="1">
+    <row r="1494" spans="1:21" ht="15" customHeight="1">
       <c r="A1494" s="26">
         <f t="shared" si="22"/>
         <v>1334</v>
@@ -51700,7 +51782,7 @@
       <c r="S1494" s="30"/>
       <c r="T1494" s="30"/>
     </row>
-    <row r="1495" spans="1:20" ht="15" customHeight="1">
+    <row r="1495" spans="1:21" ht="15" customHeight="1">
       <c r="A1495" s="26">
         <f t="shared" si="22"/>
         <v>1335</v>
@@ -51735,7 +51817,7 @@
       <c r="S1495" s="30"/>
       <c r="T1495" s="30"/>
     </row>
-    <row r="1496" spans="1:20" ht="15" customHeight="1">
+    <row r="1496" spans="1:21" ht="15" customHeight="1">
       <c r="A1496" s="26">
         <f t="shared" si="22"/>
         <v>1336</v>
@@ -51770,7 +51852,7 @@
       <c r="S1496" s="30"/>
       <c r="T1496" s="30"/>
     </row>
-    <row r="1497" spans="1:20" ht="15" customHeight="1">
+    <row r="1497" spans="1:21" ht="15" customHeight="1">
       <c r="A1497" s="26">
         <f t="shared" si="22"/>
         <v>1337</v>
@@ -51805,7 +51887,7 @@
       <c r="S1497" s="30"/>
       <c r="T1497" s="30"/>
     </row>
-    <row r="1498" spans="1:20" ht="15" customHeight="1">
+    <row r="1498" spans="1:21" ht="15" customHeight="1">
       <c r="A1498" s="26">
         <f t="shared" si="22"/>
         <v>1338</v>
@@ -51840,7 +51922,7 @@
       <c r="S1498" s="30"/>
       <c r="T1498" s="30"/>
     </row>
-    <row r="1499" spans="1:20" ht="15" customHeight="1">
+    <row r="1499" spans="1:21" ht="15" customHeight="1">
       <c r="A1499" s="26">
         <f t="shared" si="22"/>
         <v>1339</v>
@@ -51875,7 +51957,7 @@
       <c r="S1499" s="30"/>
       <c r="T1499" s="30"/>
     </row>
-    <row r="1500" spans="1:20" ht="15" customHeight="1">
+    <row r="1500" spans="1:21" ht="15" customHeight="1">
       <c r="A1500" s="26">
         <f t="shared" si="22"/>
         <v>1339</v>
@@ -51910,7 +51992,7 @@
       </c>
       <c r="T1500" s="30"/>
     </row>
-    <row r="1501" spans="1:20" ht="15" customHeight="1">
+    <row r="1501" spans="1:21" ht="15" customHeight="1">
       <c r="A1501" s="26">
         <f t="shared" si="22"/>
         <v>1339</v>
@@ -51939,7 +52021,7 @@
       </c>
       <c r="T1501" s="30"/>
     </row>
-    <row r="1502" spans="1:20" ht="15" customHeight="1">
+    <row r="1502" spans="1:21" ht="15" customHeight="1">
       <c r="A1502" s="26">
         <f t="shared" si="22"/>
         <v>1340</v>
@@ -51972,7 +52054,7 @@
       <c r="S1502" s="30"/>
       <c r="T1502" s="30"/>
     </row>
-    <row r="1503" spans="1:20" ht="15" customHeight="1">
+    <row r="1503" spans="1:21" ht="15" customHeight="1">
       <c r="A1503" s="26">
         <f t="shared" si="22"/>
         <v>1341</v>
@@ -52009,7 +52091,7 @@
       <c r="S1503" s="30"/>
       <c r="T1503" s="30"/>
     </row>
-    <row r="1504" spans="1:20" ht="15" customHeight="1">
+    <row r="1504" spans="1:21" ht="15" customHeight="1">
       <c r="A1504" s="26">
         <f t="shared" ref="A1504:A1539" si="23">IF(OR(F1504="",F1504=""),A1503,A1503+1)</f>
         <v>1341</v>
@@ -52040,7 +52122,7 @@
       <c r="S1504" s="30"/>
       <c r="T1504" s="30"/>
     </row>
-    <row r="1505" spans="1:20" ht="15" customHeight="1">
+    <row r="1505" spans="1:21" ht="15" customHeight="1">
       <c r="A1505" s="26">
         <f t="shared" si="23"/>
         <v>1342</v>
@@ -52073,7 +52155,7 @@
       <c r="S1505" s="30"/>
       <c r="T1505" s="30"/>
     </row>
-    <row r="1506" spans="1:20" ht="15" customHeight="1">
+    <row r="1506" spans="1:21" ht="15" customHeight="1">
       <c r="A1506" s="26">
         <f t="shared" si="23"/>
         <v>1343</v>
@@ -52108,7 +52190,7 @@
       <c r="S1506" s="30"/>
       <c r="T1506" s="30"/>
     </row>
-    <row r="1507" spans="1:20" ht="15" customHeight="1">
+    <row r="1507" spans="1:21" ht="15" customHeight="1">
       <c r="A1507" s="26">
         <f t="shared" si="23"/>
         <v>1344</v>
@@ -52145,7 +52227,7 @@
       <c r="S1507" s="30"/>
       <c r="T1507" s="30"/>
     </row>
-    <row r="1508" spans="1:20" ht="15" customHeight="1">
+    <row r="1508" spans="1:21" ht="15" customHeight="1">
       <c r="A1508" s="26">
         <f t="shared" si="23"/>
         <v>1344</v>
@@ -52176,7 +52258,7 @@
       <c r="S1508" s="30"/>
       <c r="T1508" s="30"/>
     </row>
-    <row r="1509" spans="1:20" ht="15" customHeight="1">
+    <row r="1509" spans="1:21" ht="15" customHeight="1">
       <c r="A1509" s="26">
         <f t="shared" si="23"/>
         <v>1345</v>
@@ -52209,7 +52291,7 @@
       <c r="S1509" s="30"/>
       <c r="T1509" s="30"/>
     </row>
-    <row r="1510" spans="1:20" ht="15" customHeight="1">
+    <row r="1510" spans="1:21" ht="15" customHeight="1">
       <c r="A1510" s="26">
         <f t="shared" si="23"/>
         <v>1345</v>
@@ -52244,7 +52326,7 @@
       </c>
       <c r="T1510" s="30"/>
     </row>
-    <row r="1511" spans="1:20" ht="15" customHeight="1">
+    <row r="1511" spans="1:21" ht="15" customHeight="1">
       <c r="A1511" s="26">
         <f t="shared" si="23"/>
         <v>1346</v>
@@ -52273,7 +52355,7 @@
       <c r="S1511" s="30"/>
       <c r="T1511" s="30"/>
     </row>
-    <row r="1512" spans="1:20" ht="15" customHeight="1">
+    <row r="1512" spans="1:21" ht="15" customHeight="1">
       <c r="A1512" s="26">
         <f t="shared" si="23"/>
         <v>1347</v>
@@ -52304,7 +52386,7 @@
       <c r="S1512" s="30"/>
       <c r="T1512" s="30"/>
     </row>
-    <row r="1513" spans="1:20" ht="15" customHeight="1">
+    <row r="1513" spans="1:21" ht="15" customHeight="1">
       <c r="A1513" s="26">
         <f t="shared" si="23"/>
         <v>1348</v>
@@ -52341,7 +52423,7 @@
       <c r="S1513" s="30"/>
       <c r="T1513" s="30"/>
     </row>
-    <row r="1514" spans="1:20" ht="15" customHeight="1">
+    <row r="1514" spans="1:21" ht="15" customHeight="1">
       <c r="A1514" s="26">
         <f t="shared" si="23"/>
         <v>1349</v>
@@ -52372,7 +52454,7 @@
       <c r="S1514" s="30"/>
       <c r="T1514" s="30"/>
     </row>
-    <row r="1515" spans="1:20" ht="15" customHeight="1">
+    <row r="1515" spans="1:21" ht="15" customHeight="1">
       <c r="A1515" s="26">
         <f t="shared" si="23"/>
         <v>1350</v>
@@ -52403,7 +52485,7 @@
       <c r="S1515" s="30"/>
       <c r="T1515" s="30"/>
     </row>
-    <row r="1516" spans="1:20" ht="15" customHeight="1">
+    <row r="1516" spans="1:21" ht="15" customHeight="1">
       <c r="A1516" s="26">
         <f t="shared" si="23"/>
         <v>1351</v>
@@ -52438,7 +52520,7 @@
       <c r="S1516" s="30"/>
       <c r="T1516" s="30"/>
     </row>
-    <row r="1517" spans="1:20" ht="15" customHeight="1">
+    <row r="1517" spans="1:21" ht="15" customHeight="1">
       <c r="A1517" s="26">
         <f t="shared" si="23"/>
         <v>1352</v>
@@ -52469,7 +52551,7 @@
       <c r="S1517" s="30"/>
       <c r="T1517" s="30"/>
     </row>
-    <row r="1518" spans="1:20" ht="15" customHeight="1">
+    <row r="1518" spans="1:21" ht="15" customHeight="1">
       <c r="A1518" s="26">
         <f t="shared" si="23"/>
         <v>1353</v>
@@ -52507,8 +52589,11 @@
       </c>
       <c r="S1518" s="30"/>
       <c r="T1518" s="30"/>
-    </row>
-    <row r="1519" spans="1:20" ht="15" customHeight="1">
+      <c r="U1518" s="37">
+        <v>0.15868161532487801</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:21" ht="15" customHeight="1">
       <c r="A1519" s="26">
         <f t="shared" si="23"/>
         <v>1354</v>
@@ -52541,7 +52626,7 @@
       <c r="S1519" s="30"/>
       <c r="T1519" s="30"/>
     </row>
-    <row r="1520" spans="1:20" ht="15" customHeight="1">
+    <row r="1520" spans="1:21" ht="15" customHeight="1">
       <c r="A1520" s="26">
         <f t="shared" si="23"/>
         <v>1354</v>
@@ -53194,7 +53279,7 @@
       <c r="T1539" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T1539"/>
+  <autoFilter ref="A1:U1539"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added fouls.won/conceded to blank poss.action columns
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-ptfc-orl-041716.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-ptfc-orl-041716.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/wosostats/source/excel/nwsl-2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="match" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">match!$A$1:$T$1544</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">match!$A$1:$U$1544</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6901" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6909" uniqueCount="188">
   <si>
     <t>event</t>
   </si>
@@ -589,15 +589,21 @@
   <si>
     <t>xG</t>
   </si>
+  <si>
+    <t>fouls.won</t>
+  </si>
+  <si>
+    <t>fouls.conceded</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -638,6 +644,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -807,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -873,10 +886,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1224,9 +1238,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1544"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomLeft" activeCell="F1048" sqref="F1048"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48670,7 +48684,7 @@
     <row r="1297" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1297" s="1">
         <f t="shared" si="19"/>
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B1297" s="29">
         <v>75</v>
@@ -48680,7 +48694,9 @@
       <c r="E1297" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="F1297" s="30"/>
+      <c r="F1297" s="35" t="s">
+        <v>186</v>
+      </c>
       <c r="G1297" s="30"/>
       <c r="H1297" s="30"/>
       <c r="I1297" s="30"/>
@@ -48706,7 +48722,7 @@
     <row r="1298" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1298" s="1">
         <f t="shared" si="19"/>
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B1298" s="29">
         <v>75</v>
@@ -48740,7 +48756,7 @@
     <row r="1299" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1299" s="1">
         <f t="shared" si="19"/>
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B1299" s="29">
         <v>75</v>
@@ -48770,7 +48786,7 @@
     <row r="1300" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1300" s="1">
         <f t="shared" si="19"/>
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="B1300" s="29">
         <v>75</v>
@@ -48814,7 +48830,7 @@
     <row r="1301" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1301" s="1">
         <f t="shared" si="19"/>
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B1301" s="29">
         <v>75</v>
@@ -48848,7 +48864,7 @@
     <row r="1302" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1302" s="1">
         <f t="shared" si="19"/>
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B1302" s="29">
         <v>75</v>
@@ -48878,7 +48894,7 @@
     <row r="1303" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1303" s="1">
         <f t="shared" si="19"/>
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B1303" s="29">
         <v>75</v>
@@ -48912,7 +48928,7 @@
     <row r="1304" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1304" s="1">
         <f t="shared" si="19"/>
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B1304" s="29">
         <v>75</v>
@@ -48950,7 +48966,7 @@
     <row r="1305" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1305" s="1">
         <f t="shared" si="19"/>
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="B1305" s="29">
         <v>75</v>
@@ -48982,7 +48998,7 @@
     <row r="1306" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1306" s="1">
         <f t="shared" si="19"/>
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="B1306" s="29">
         <v>75</v>
@@ -49014,7 +49030,7 @@
     <row r="1307" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1307" s="1">
         <f t="shared" si="19"/>
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B1307" s="29">
         <v>75</v>
@@ -49046,7 +49062,7 @@
     <row r="1308" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1308" s="1">
         <f t="shared" si="19"/>
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="B1308" s="29">
         <v>75</v>
@@ -49078,7 +49094,7 @@
     <row r="1309" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1309" s="1">
         <f t="shared" si="19"/>
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="B1309" s="29">
         <v>76</v>
@@ -49114,7 +49130,7 @@
     <row r="1310" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1310" s="1">
         <f t="shared" si="19"/>
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="B1310" s="29">
         <v>76</v>
@@ -49146,7 +49162,7 @@
     <row r="1311" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1311" s="1">
         <f t="shared" ref="A1311:A1374" si="20">IF(OR(F1311="",F1311=""),A1310,A1310+1)</f>
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B1311" s="29">
         <v>76</v>
@@ -49182,7 +49198,7 @@
     <row r="1312" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1312" s="1">
         <f t="shared" si="20"/>
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B1312" s="29">
         <v>76</v>
@@ -49218,7 +49234,7 @@
     <row r="1313" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1313" s="1">
         <f t="shared" si="20"/>
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B1313" s="29">
         <v>76</v>
@@ -49254,7 +49270,7 @@
     <row r="1314" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1314" s="1">
         <f t="shared" si="20"/>
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B1314" s="29">
         <v>76</v>
@@ -49286,7 +49302,7 @@
     <row r="1315" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1315" s="1">
         <f t="shared" si="20"/>
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B1315" s="29">
         <v>76</v>
@@ -49322,7 +49338,7 @@
     <row r="1316" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1316" s="1">
         <f t="shared" si="20"/>
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B1316" s="29">
         <v>76</v>
@@ -49354,7 +49370,7 @@
     <row r="1317" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1317" s="1">
         <f t="shared" si="20"/>
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B1317" s="29">
         <v>76</v>
@@ -49390,7 +49406,7 @@
     <row r="1318" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1318" s="1">
         <f t="shared" si="20"/>
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B1318" s="29">
         <v>76</v>
@@ -49428,7 +49444,7 @@
     <row r="1319" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1319" s="1">
         <f t="shared" si="20"/>
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B1319" s="29">
         <v>76</v>
@@ -49460,7 +49476,7 @@
     <row r="1320" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1320" s="1">
         <f t="shared" si="20"/>
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B1320" s="29">
         <v>76</v>
@@ -49492,7 +49508,7 @@
     <row r="1321" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1321" s="1">
         <f t="shared" si="20"/>
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B1321" s="29">
         <v>76</v>
@@ -49526,7 +49542,7 @@
     <row r="1322" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1322" s="1">
         <f t="shared" si="20"/>
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B1322" s="29">
         <v>76</v>
@@ -49562,7 +49578,7 @@
     <row r="1323" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1323" s="1">
         <f t="shared" si="20"/>
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B1323" s="29">
         <v>76</v>
@@ -49594,7 +49610,7 @@
     <row r="1324" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1324" s="1">
         <f t="shared" si="20"/>
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B1324" s="29">
         <v>76</v>
@@ -49626,7 +49642,7 @@
     <row r="1325" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1325" s="1">
         <f t="shared" si="20"/>
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B1325" s="29">
         <v>76</v>
@@ -49658,7 +49674,7 @@
     <row r="1326" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1326" s="1">
         <f t="shared" si="20"/>
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="B1326" s="29">
         <v>76</v>
@@ -49690,7 +49706,7 @@
     <row r="1327" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1327" s="1">
         <f t="shared" si="20"/>
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="B1327" s="29">
         <v>76</v>
@@ -49726,7 +49742,7 @@
     <row r="1328" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1328" s="1">
         <f t="shared" si="20"/>
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="B1328" s="29">
         <v>76</v>
@@ -49762,7 +49778,7 @@
     <row r="1329" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1329" s="1">
         <f t="shared" si="20"/>
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="B1329" s="29">
         <v>76</v>
@@ -49798,7 +49814,7 @@
     <row r="1330" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1330" s="1">
         <f t="shared" si="20"/>
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="B1330" s="29">
         <v>76</v>
@@ -49830,7 +49846,7 @@
     <row r="1331" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1331" s="1">
         <f t="shared" si="20"/>
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B1331" s="29">
         <v>76</v>
@@ -49866,7 +49882,7 @@
     <row r="1332" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1332" s="1">
         <f t="shared" si="20"/>
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B1332" s="29">
         <v>76</v>
@@ -49898,7 +49914,7 @@
     <row r="1333" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1333" s="1">
         <f t="shared" si="20"/>
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="B1333" s="29">
         <v>76</v>
@@ -49936,7 +49952,7 @@
     <row r="1334" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1334" s="1">
         <f t="shared" si="20"/>
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B1334" s="29">
         <v>76</v>
@@ -49974,7 +49990,7 @@
     <row r="1335" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1335" s="1">
         <f t="shared" si="20"/>
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="B1335" s="29">
         <v>77</v>
@@ -50008,7 +50024,7 @@
     <row r="1336" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1336" s="1">
         <f t="shared" si="20"/>
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="B1336" s="29">
         <v>77</v>
@@ -50038,7 +50054,7 @@
     <row r="1337" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1337" s="1">
         <f t="shared" si="20"/>
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="B1337" s="29">
         <v>77</v>
@@ -50074,7 +50090,7 @@
     <row r="1338" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1338" s="1">
         <f t="shared" si="20"/>
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="B1338" s="29">
         <v>77</v>
@@ -50112,7 +50128,7 @@
     <row r="1339" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1339" s="1">
         <f t="shared" si="20"/>
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="B1339" s="29">
         <v>77</v>
@@ -50142,7 +50158,7 @@
     <row r="1340" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1340" s="1">
         <f t="shared" si="20"/>
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="B1340" s="29">
         <v>77</v>
@@ -50180,7 +50196,7 @@
     <row r="1341" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1341" s="1">
         <f t="shared" si="20"/>
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="B1341" s="29">
         <v>77</v>
@@ -50214,7 +50230,7 @@
     <row r="1342" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1342" s="1">
         <f t="shared" si="20"/>
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="B1342" s="29">
         <v>77</v>
@@ -50244,7 +50260,7 @@
     <row r="1343" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1343" s="1">
         <f t="shared" si="20"/>
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="B1343" s="29">
         <v>78</v>
@@ -50282,7 +50298,7 @@
     <row r="1344" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1344" s="1">
         <f t="shared" si="20"/>
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="B1344" s="29">
         <v>78</v>
@@ -50316,7 +50332,7 @@
     <row r="1345" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1345" s="1">
         <f t="shared" si="20"/>
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="B1345" s="29">
         <v>78</v>
@@ -50348,7 +50364,7 @@
     <row r="1346" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1346" s="1">
         <f t="shared" si="20"/>
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="B1346" s="29">
         <v>78</v>
@@ -50380,7 +50396,7 @@
     <row r="1347" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1347" s="1">
         <f t="shared" si="20"/>
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="B1347" s="29">
         <v>78</v>
@@ -50424,7 +50440,7 @@
     <row r="1348" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1348" s="1">
         <f t="shared" si="20"/>
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="B1348" s="29">
         <v>78</v>
@@ -50458,7 +50474,7 @@
     <row r="1349" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1349" s="1">
         <f t="shared" si="20"/>
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B1349" s="29">
         <v>78</v>
@@ -50490,7 +50506,7 @@
     <row r="1350" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1350" s="1">
         <f t="shared" si="20"/>
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="B1350" s="29">
         <v>78</v>
@@ -50520,7 +50536,7 @@
     <row r="1351" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1351" s="1">
         <f t="shared" si="20"/>
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="B1351" s="29">
         <v>78</v>
@@ -50530,7 +50546,9 @@
       <c r="E1351" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="F1351" s="30"/>
+      <c r="F1351" s="35" t="s">
+        <v>186</v>
+      </c>
       <c r="G1351" s="30"/>
       <c r="H1351" s="30"/>
       <c r="I1351" s="30"/>
@@ -50556,7 +50574,7 @@
     <row r="1352" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1352" s="1">
         <f t="shared" si="20"/>
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="B1352" s="29">
         <v>78</v>
@@ -50590,7 +50608,7 @@
     <row r="1353" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1353" s="1">
         <f t="shared" si="20"/>
-        <v>1222</v>
+        <v>1224</v>
       </c>
       <c r="B1353" s="29">
         <v>78</v>
@@ -50626,7 +50644,7 @@
     <row r="1354" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1354" s="1">
         <f t="shared" si="20"/>
-        <v>1223</v>
+        <v>1225</v>
       </c>
       <c r="B1354" s="29">
         <v>79</v>
@@ -50664,7 +50682,7 @@
     <row r="1355" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1355" s="1">
         <f t="shared" si="20"/>
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="B1355" s="29">
         <v>79</v>
@@ -50700,7 +50718,7 @@
     <row r="1356" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1356" s="1">
         <f t="shared" si="20"/>
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="B1356" s="29">
         <v>79</v>
@@ -50736,7 +50754,7 @@
     <row r="1357" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1357" s="1">
         <f t="shared" si="20"/>
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="B1357" s="29">
         <v>79</v>
@@ -50772,7 +50790,7 @@
     <row r="1358" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1358" s="1">
         <f t="shared" si="20"/>
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="B1358" s="29">
         <v>79</v>
@@ -50808,7 +50826,7 @@
     <row r="1359" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1359" s="1">
         <f t="shared" si="20"/>
-        <v>1228</v>
+        <v>1230</v>
       </c>
       <c r="B1359" s="29">
         <v>79</v>
@@ -50842,7 +50860,7 @@
     <row r="1360" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1360" s="1">
         <f t="shared" si="20"/>
-        <v>1228</v>
+        <v>1231</v>
       </c>
       <c r="B1360" s="29">
         <v>79</v>
@@ -50852,7 +50870,9 @@
       <c r="E1360" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F1360" s="30"/>
+      <c r="F1360" s="35" t="s">
+        <v>186</v>
+      </c>
       <c r="G1360" s="30"/>
       <c r="H1360" s="30"/>
       <c r="I1360" s="30"/>
@@ -50878,7 +50898,7 @@
     <row r="1361" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1361" s="1">
         <f t="shared" si="20"/>
-        <v>1229</v>
+        <v>1232</v>
       </c>
       <c r="B1361" s="29">
         <v>80</v>
@@ -50919,7 +50939,7 @@
     <row r="1362" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1362" s="1">
         <f t="shared" si="20"/>
-        <v>1230</v>
+        <v>1233</v>
       </c>
       <c r="B1362" s="29">
         <v>80</v>
@@ -50955,7 +50975,7 @@
     <row r="1363" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1363" s="1">
         <f t="shared" si="20"/>
-        <v>1231</v>
+        <v>1234</v>
       </c>
       <c r="B1363" s="29">
         <v>80</v>
@@ -50991,7 +51011,7 @@
     <row r="1364" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1364" s="1">
         <f t="shared" si="20"/>
-        <v>1231</v>
+        <v>1234</v>
       </c>
       <c r="B1364" s="29">
         <v>80</v>
@@ -51023,7 +51043,7 @@
     <row r="1365" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1365" s="1">
         <f t="shared" si="20"/>
-        <v>1232</v>
+        <v>1235</v>
       </c>
       <c r="B1365" s="29">
         <v>80</v>
@@ -51061,7 +51081,7 @@
     <row r="1366" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1366" s="1">
         <f t="shared" si="20"/>
-        <v>1233</v>
+        <v>1236</v>
       </c>
       <c r="B1366" s="29">
         <v>80</v>
@@ -51093,7 +51113,7 @@
     <row r="1367" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1367" s="1">
         <f t="shared" si="20"/>
-        <v>1234</v>
+        <v>1237</v>
       </c>
       <c r="B1367" s="29">
         <v>80</v>
@@ -51131,7 +51151,7 @@
     <row r="1368" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1368" s="1">
         <f t="shared" si="20"/>
-        <v>1234</v>
+        <v>1237</v>
       </c>
       <c r="B1368" s="29">
         <v>80</v>
@@ -51163,7 +51183,7 @@
     <row r="1369" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1369" s="1">
         <f t="shared" si="20"/>
-        <v>1234</v>
+        <v>1237</v>
       </c>
       <c r="B1369" s="29">
         <v>80</v>
@@ -51195,7 +51215,7 @@
     <row r="1370" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1370" s="1">
         <f t="shared" si="20"/>
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="B1370" s="29">
         <v>80</v>
@@ -51227,7 +51247,7 @@
     <row r="1371" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1371" s="1">
         <f t="shared" si="20"/>
-        <v>1236</v>
+        <v>1239</v>
       </c>
       <c r="B1371" s="29">
         <v>80</v>
@@ -51263,7 +51283,7 @@
     <row r="1372" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1372" s="1">
         <f t="shared" si="20"/>
-        <v>1237</v>
+        <v>1240</v>
       </c>
       <c r="B1372" s="29">
         <v>80</v>
@@ -51299,7 +51319,7 @@
     <row r="1373" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1373" s="1">
         <f t="shared" si="20"/>
-        <v>1238</v>
+        <v>1241</v>
       </c>
       <c r="B1373" s="29">
         <v>80</v>
@@ -51335,7 +51355,7 @@
     <row r="1374" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1374" s="1">
         <f t="shared" si="20"/>
-        <v>1238</v>
+        <v>1241</v>
       </c>
       <c r="B1374" s="29">
         <v>80</v>
@@ -51367,7 +51387,7 @@
     <row r="1375" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1375" s="1">
         <f t="shared" ref="A1375:A1438" si="21">IF(OR(F1375="",F1375=""),A1374,A1374+1)</f>
-        <v>1238</v>
+        <v>1241</v>
       </c>
       <c r="B1375" s="29">
         <v>80</v>
@@ -51399,7 +51419,7 @@
     <row r="1376" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1376" s="1">
         <f t="shared" si="21"/>
-        <v>1239</v>
+        <v>1242</v>
       </c>
       <c r="B1376" s="29">
         <v>80</v>
@@ -51435,7 +51455,7 @@
     <row r="1377" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1377" s="1">
         <f t="shared" si="21"/>
-        <v>1239</v>
+        <v>1242</v>
       </c>
       <c r="B1377" s="29">
         <v>80</v>
@@ -51467,7 +51487,7 @@
     <row r="1378" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1378" s="1">
         <f t="shared" si="21"/>
-        <v>1240</v>
+        <v>1243</v>
       </c>
       <c r="B1378" s="29">
         <v>80</v>
@@ -51499,7 +51519,7 @@
     <row r="1379" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1379" s="1">
         <f t="shared" si="21"/>
-        <v>1241</v>
+        <v>1244</v>
       </c>
       <c r="B1379" s="29">
         <v>80</v>
@@ -51535,7 +51555,7 @@
     <row r="1380" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1380" s="1">
         <f t="shared" si="21"/>
-        <v>1242</v>
+        <v>1245</v>
       </c>
       <c r="B1380" s="29">
         <v>80</v>
@@ -51567,7 +51587,7 @@
     <row r="1381" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1381" s="1">
         <f t="shared" si="21"/>
-        <v>1243</v>
+        <v>1246</v>
       </c>
       <c r="B1381" s="29">
         <v>80</v>
@@ -51603,7 +51623,7 @@
     <row r="1382" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1382" s="1">
         <f t="shared" si="21"/>
-        <v>1244</v>
+        <v>1247</v>
       </c>
       <c r="B1382" s="29">
         <v>80</v>
@@ -51641,7 +51661,7 @@
     <row r="1383" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1383" s="1">
         <f t="shared" si="21"/>
-        <v>1245</v>
+        <v>1248</v>
       </c>
       <c r="B1383" s="29">
         <v>80</v>
@@ -51681,7 +51701,7 @@
     <row r="1384" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1384" s="1">
         <f t="shared" si="21"/>
-        <v>1246</v>
+        <v>1249</v>
       </c>
       <c r="B1384" s="29">
         <v>80</v>
@@ -51715,7 +51735,7 @@
     <row r="1385" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1385" s="1">
         <f t="shared" si="21"/>
-        <v>1247</v>
+        <v>1250</v>
       </c>
       <c r="B1385" s="29">
         <v>80</v>
@@ -51747,7 +51767,7 @@
     <row r="1386" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1386" s="1">
         <f t="shared" si="21"/>
-        <v>1248</v>
+        <v>1251</v>
       </c>
       <c r="B1386" s="29">
         <v>80</v>
@@ -51785,7 +51805,7 @@
     <row r="1387" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1387" s="1">
         <f t="shared" si="21"/>
-        <v>1248</v>
+        <v>1251</v>
       </c>
       <c r="B1387" s="29">
         <v>80</v>
@@ -51817,7 +51837,7 @@
     <row r="1388" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1388" s="1">
         <f t="shared" si="21"/>
-        <v>1249</v>
+        <v>1252</v>
       </c>
       <c r="B1388" s="29">
         <v>81</v>
@@ -51853,7 +51873,7 @@
     <row r="1389" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1389" s="1">
         <f t="shared" si="21"/>
-        <v>1250</v>
+        <v>1253</v>
       </c>
       <c r="B1389" s="29">
         <v>81</v>
@@ -51889,7 +51909,7 @@
     <row r="1390" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1390" s="1">
         <f t="shared" si="21"/>
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="B1390" s="29">
         <v>81</v>
@@ -51935,7 +51955,7 @@
     <row r="1391" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1391" s="1">
         <f t="shared" si="21"/>
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="B1391" s="29">
         <v>81</v>
@@ -51965,7 +51985,7 @@
     <row r="1392" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1392" s="1">
         <f t="shared" si="21"/>
-        <v>1252</v>
+        <v>1255</v>
       </c>
       <c r="B1392" s="29">
         <v>81</v>
@@ -52005,7 +52025,7 @@
     <row r="1393" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1393" s="1">
         <f t="shared" si="21"/>
-        <v>1252</v>
+        <v>1255</v>
       </c>
       <c r="B1393" s="29">
         <v>81</v>
@@ -52035,7 +52055,7 @@
     <row r="1394" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1394" s="1">
         <f t="shared" si="21"/>
-        <v>1253</v>
+        <v>1256</v>
       </c>
       <c r="B1394" s="29">
         <v>81</v>
@@ -52069,7 +52089,7 @@
     <row r="1395" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1395" s="1">
         <f t="shared" si="21"/>
-        <v>1254</v>
+        <v>1257</v>
       </c>
       <c r="B1395" s="29">
         <v>81</v>
@@ -52101,7 +52121,7 @@
     <row r="1396" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1396" s="1">
         <f t="shared" si="21"/>
-        <v>1255</v>
+        <v>1258</v>
       </c>
       <c r="B1396" s="29">
         <v>81</v>
@@ -52133,7 +52153,7 @@
     <row r="1397" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1397" s="1">
         <f t="shared" si="21"/>
-        <v>1256</v>
+        <v>1259</v>
       </c>
       <c r="B1397" s="29">
         <v>81</v>
@@ -52165,7 +52185,7 @@
     <row r="1398" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1398" s="1">
         <f t="shared" si="21"/>
-        <v>1257</v>
+        <v>1260</v>
       </c>
       <c r="B1398" s="29">
         <v>81</v>
@@ -52203,7 +52223,7 @@
     <row r="1399" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1399" s="1">
         <f t="shared" si="21"/>
-        <v>1257</v>
+        <v>1260</v>
       </c>
       <c r="B1399" s="29">
         <v>81</v>
@@ -52235,7 +52255,7 @@
     <row r="1400" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1400" s="1">
         <f t="shared" si="21"/>
-        <v>1258</v>
+        <v>1261</v>
       </c>
       <c r="B1400" s="29">
         <v>82</v>
@@ -52267,7 +52287,7 @@
     <row r="1401" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1401" s="1">
         <f t="shared" si="21"/>
-        <v>1259</v>
+        <v>1262</v>
       </c>
       <c r="B1401" s="29">
         <v>82</v>
@@ -52301,7 +52321,7 @@
     <row r="1402" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1402" s="1">
         <f t="shared" si="21"/>
-        <v>1259</v>
+        <v>1262</v>
       </c>
       <c r="B1402" s="29">
         <v>82</v>
@@ -52331,7 +52351,7 @@
     <row r="1403" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1403" s="1">
         <f t="shared" si="21"/>
-        <v>1260</v>
+        <v>1263</v>
       </c>
       <c r="B1403" s="29">
         <v>82</v>
@@ -52369,7 +52389,7 @@
     <row r="1404" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1404" s="1">
         <f t="shared" si="21"/>
-        <v>1260</v>
+        <v>1263</v>
       </c>
       <c r="B1404" s="29">
         <v>82</v>
@@ -52401,7 +52421,7 @@
     <row r="1405" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1405" s="1">
         <f t="shared" si="21"/>
-        <v>1260</v>
+        <v>1263</v>
       </c>
       <c r="B1405" s="29">
         <v>82</v>
@@ -52437,7 +52457,7 @@
     <row r="1406" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1406" s="1">
         <f t="shared" si="21"/>
-        <v>1261</v>
+        <v>1264</v>
       </c>
       <c r="B1406" s="29">
         <v>82</v>
@@ -52467,7 +52487,7 @@
     <row r="1407" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1407" s="1">
         <f t="shared" si="21"/>
-        <v>1262</v>
+        <v>1265</v>
       </c>
       <c r="B1407" s="29">
         <v>82</v>
@@ -52503,7 +52523,7 @@
     <row r="1408" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1408" s="1">
         <f t="shared" si="21"/>
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="B1408" s="29">
         <v>82</v>
@@ -52535,7 +52555,7 @@
     <row r="1409" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1409" s="1">
         <f t="shared" si="21"/>
-        <v>1264</v>
+        <v>1267</v>
       </c>
       <c r="B1409" s="29">
         <v>82</v>
@@ -52567,7 +52587,7 @@
     <row r="1410" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1410" s="1">
         <f t="shared" si="21"/>
-        <v>1265</v>
+        <v>1268</v>
       </c>
       <c r="B1410" s="29">
         <v>82</v>
@@ -52607,7 +52627,7 @@
     <row r="1411" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1411" s="1">
         <f t="shared" si="21"/>
-        <v>1266</v>
+        <v>1269</v>
       </c>
       <c r="B1411" s="29">
         <v>83</v>
@@ -52645,7 +52665,7 @@
     <row r="1412" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1412" s="1">
         <f t="shared" si="21"/>
-        <v>1266</v>
+        <v>1269</v>
       </c>
       <c r="B1412" s="29">
         <v>83</v>
@@ -52675,7 +52695,7 @@
     <row r="1413" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1413" s="1">
         <f t="shared" si="21"/>
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="B1413" s="29">
         <v>83</v>
@@ -52711,7 +52731,7 @@
     <row r="1414" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1414" s="1">
         <f t="shared" si="21"/>
-        <v>1268</v>
+        <v>1271</v>
       </c>
       <c r="B1414" s="29">
         <v>83</v>
@@ -52749,7 +52769,7 @@
     <row r="1415" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1415" s="1">
         <f t="shared" si="21"/>
-        <v>1269</v>
+        <v>1272</v>
       </c>
       <c r="B1415" s="29">
         <v>83</v>
@@ -52785,7 +52805,7 @@
     <row r="1416" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1416" s="1">
         <f t="shared" si="21"/>
-        <v>1270</v>
+        <v>1273</v>
       </c>
       <c r="B1416" s="29">
         <v>83</v>
@@ -52823,7 +52843,7 @@
     <row r="1417" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1417" s="1">
         <f t="shared" si="21"/>
-        <v>1270</v>
+        <v>1274</v>
       </c>
       <c r="B1417" s="29">
         <v>83</v>
@@ -52833,7 +52853,9 @@
       <c r="E1417" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="F1417" s="30"/>
+      <c r="F1417" s="35" t="s">
+        <v>187</v>
+      </c>
       <c r="G1417" s="30"/>
       <c r="H1417" s="30"/>
       <c r="I1417" s="30"/>
@@ -52861,7 +52883,7 @@
     <row r="1418" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1418" s="1">
         <f t="shared" si="21"/>
-        <v>1271</v>
+        <v>1275</v>
       </c>
       <c r="B1418" s="29">
         <v>84</v>
@@ -52899,7 +52921,7 @@
     <row r="1419" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1419" s="1">
         <f t="shared" si="21"/>
-        <v>1271</v>
+        <v>1275</v>
       </c>
       <c r="B1419" s="29">
         <v>84</v>
@@ -52935,7 +52957,7 @@
     <row r="1420" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1420" s="1">
         <f t="shared" si="21"/>
-        <v>1271</v>
+        <v>1275</v>
       </c>
       <c r="B1420" s="29">
         <v>84</v>
@@ -52965,7 +52987,7 @@
     <row r="1421" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1421" s="1">
         <f t="shared" si="21"/>
-        <v>1272</v>
+        <v>1276</v>
       </c>
       <c r="B1421" s="29">
         <v>84</v>
@@ -52999,7 +53021,7 @@
     <row r="1422" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1422" s="1">
         <f t="shared" si="21"/>
-        <v>1273</v>
+        <v>1277</v>
       </c>
       <c r="B1422" s="29">
         <v>84</v>
@@ -53037,7 +53059,7 @@
     <row r="1423" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1423" s="1">
         <f t="shared" si="21"/>
-        <v>1274</v>
+        <v>1278</v>
       </c>
       <c r="B1423" s="29">
         <v>84</v>
@@ -53069,7 +53091,7 @@
     <row r="1424" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1424" s="1">
         <f t="shared" si="21"/>
-        <v>1275</v>
+        <v>1279</v>
       </c>
       <c r="B1424" s="29">
         <v>84</v>
@@ -53105,7 +53127,7 @@
     <row r="1425" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1425" s="1">
         <f t="shared" si="21"/>
-        <v>1276</v>
+        <v>1280</v>
       </c>
       <c r="B1425" s="29">
         <v>84</v>
@@ -53141,7 +53163,7 @@
     <row r="1426" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1426" s="1">
         <f t="shared" si="21"/>
-        <v>1276</v>
+        <v>1280</v>
       </c>
       <c r="B1426" s="29">
         <v>84</v>
@@ -53173,7 +53195,7 @@
     <row r="1427" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1427" s="1">
         <f t="shared" si="21"/>
-        <v>1277</v>
+        <v>1281</v>
       </c>
       <c r="B1427" s="29">
         <v>84</v>
@@ -53211,7 +53233,7 @@
     <row r="1428" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1428" s="1">
         <f t="shared" si="21"/>
-        <v>1278</v>
+        <v>1282</v>
       </c>
       <c r="B1428" s="29">
         <v>85</v>
@@ -53251,7 +53273,7 @@
     <row r="1429" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1429" s="1">
         <f t="shared" si="21"/>
-        <v>1278</v>
+        <v>1282</v>
       </c>
       <c r="B1429" s="29">
         <v>85</v>
@@ -53281,7 +53303,7 @@
     <row r="1430" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1430" s="1">
         <f t="shared" si="21"/>
-        <v>1279</v>
+        <v>1283</v>
       </c>
       <c r="B1430" s="29">
         <v>85</v>
@@ -53315,7 +53337,7 @@
     <row r="1431" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1431" s="1">
         <f t="shared" si="21"/>
-        <v>1280</v>
+        <v>1284</v>
       </c>
       <c r="B1431" s="29">
         <v>85</v>
@@ -53353,7 +53375,7 @@
     <row r="1432" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1432" s="1">
         <f t="shared" si="21"/>
-        <v>1281</v>
+        <v>1285</v>
       </c>
       <c r="B1432" s="29">
         <v>85</v>
@@ -53393,7 +53415,7 @@
     <row r="1433" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1433" s="1">
         <f t="shared" si="21"/>
-        <v>1282</v>
+        <v>1286</v>
       </c>
       <c r="B1433" s="29">
         <v>85</v>
@@ -53427,7 +53449,7 @@
     <row r="1434" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1434" s="1">
         <f t="shared" si="21"/>
-        <v>1283</v>
+        <v>1287</v>
       </c>
       <c r="B1434" s="29">
         <v>85</v>
@@ -53459,7 +53481,7 @@
     <row r="1435" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1435" s="1">
         <f t="shared" si="21"/>
-        <v>1284</v>
+        <v>1288</v>
       </c>
       <c r="B1435" s="29">
         <v>85</v>
@@ -53497,7 +53519,7 @@
     <row r="1436" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1436" s="1">
         <f t="shared" si="21"/>
-        <v>1285</v>
+        <v>1289</v>
       </c>
       <c r="B1436" s="29">
         <v>85</v>
@@ -53535,7 +53557,7 @@
     <row r="1437" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1437" s="1">
         <f t="shared" si="21"/>
-        <v>1286</v>
+        <v>1290</v>
       </c>
       <c r="B1437" s="29">
         <v>85</v>
@@ -53567,7 +53589,7 @@
     <row r="1438" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1438" s="1">
         <f t="shared" si="21"/>
-        <v>1287</v>
+        <v>1291</v>
       </c>
       <c r="B1438" s="29">
         <v>85</v>
@@ -53603,7 +53625,7 @@
     <row r="1439" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1439" s="1">
         <f t="shared" ref="A1439:A1502" si="22">IF(OR(F1439="",F1439=""),A1438,A1438+1)</f>
-        <v>1288</v>
+        <v>1292</v>
       </c>
       <c r="B1439" s="29">
         <v>85</v>
@@ -53639,7 +53661,7 @@
     <row r="1440" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1440" s="1">
         <f t="shared" si="22"/>
-        <v>1289</v>
+        <v>1293</v>
       </c>
       <c r="B1440" s="29">
         <v>86</v>
@@ -53675,7 +53697,7 @@
     <row r="1441" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1441" s="1">
         <f t="shared" si="22"/>
-        <v>1290</v>
+        <v>1294</v>
       </c>
       <c r="B1441" s="29">
         <v>86</v>
@@ -53711,7 +53733,7 @@
     <row r="1442" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1442" s="1">
         <f t="shared" si="22"/>
-        <v>1291</v>
+        <v>1295</v>
       </c>
       <c r="B1442" s="29">
         <v>86</v>
@@ -53745,7 +53767,7 @@
     <row r="1443" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1443" s="1">
         <f t="shared" si="22"/>
-        <v>1292</v>
+        <v>1296</v>
       </c>
       <c r="B1443" s="29">
         <v>86</v>
@@ -53781,7 +53803,7 @@
     <row r="1444" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1444" s="1">
         <f t="shared" si="22"/>
-        <v>1293</v>
+        <v>1297</v>
       </c>
       <c r="B1444" s="29">
         <v>86</v>
@@ -53817,7 +53839,7 @@
     <row r="1445" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1445" s="1">
         <f t="shared" si="22"/>
-        <v>1294</v>
+        <v>1298</v>
       </c>
       <c r="B1445" s="29">
         <v>86</v>
@@ -53853,7 +53875,7 @@
     <row r="1446" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1446" s="1">
         <f t="shared" si="22"/>
-        <v>1294</v>
+        <v>1298</v>
       </c>
       <c r="B1446" s="29">
         <v>86</v>
@@ -53885,7 +53907,7 @@
     <row r="1447" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1447" s="1">
         <f t="shared" si="22"/>
-        <v>1295</v>
+        <v>1299</v>
       </c>
       <c r="B1447" s="29">
         <v>86</v>
@@ -53917,7 +53939,7 @@
     <row r="1448" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1448" s="1">
         <f t="shared" si="22"/>
-        <v>1296</v>
+        <v>1300</v>
       </c>
       <c r="B1448" s="29">
         <v>86</v>
@@ -53953,7 +53975,7 @@
     <row r="1449" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1449" s="1">
         <f t="shared" si="22"/>
-        <v>1296</v>
+        <v>1300</v>
       </c>
       <c r="B1449" s="29">
         <v>86</v>
@@ -53985,7 +54007,7 @@
     <row r="1450" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1450" s="1">
         <f t="shared" si="22"/>
-        <v>1297</v>
+        <v>1301</v>
       </c>
       <c r="B1450" s="29">
         <v>86</v>
@@ -54017,7 +54039,7 @@
     <row r="1451" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1451" s="1">
         <f t="shared" si="22"/>
-        <v>1298</v>
+        <v>1302</v>
       </c>
       <c r="B1451" s="29">
         <v>86</v>
@@ -54055,7 +54077,7 @@
     <row r="1452" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1452" s="1">
         <f t="shared" si="22"/>
-        <v>1299</v>
+        <v>1303</v>
       </c>
       <c r="B1452" s="29">
         <v>86</v>
@@ -54087,7 +54109,7 @@
     <row r="1453" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1453" s="1">
         <f t="shared" si="22"/>
-        <v>1300</v>
+        <v>1304</v>
       </c>
       <c r="B1453" s="29">
         <v>87</v>
@@ -54119,7 +54141,7 @@
     <row r="1454" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1454" s="1">
         <f t="shared" si="22"/>
-        <v>1301</v>
+        <v>1305</v>
       </c>
       <c r="B1454" s="29">
         <v>87</v>
@@ -54153,7 +54175,7 @@
     <row r="1455" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1455" s="1">
         <f t="shared" si="22"/>
-        <v>1301</v>
+        <v>1305</v>
       </c>
       <c r="B1455" s="29">
         <v>87</v>
@@ -54183,7 +54205,7 @@
     <row r="1456" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1456" s="1">
         <f t="shared" si="22"/>
-        <v>1302</v>
+        <v>1306</v>
       </c>
       <c r="B1456" s="29">
         <v>87</v>
@@ -54219,7 +54241,7 @@
     <row r="1457" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1457" s="1">
         <f t="shared" si="22"/>
-        <v>1303</v>
+        <v>1307</v>
       </c>
       <c r="B1457" s="29">
         <v>87</v>
@@ -54251,7 +54273,7 @@
     <row r="1458" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1458" s="1">
         <f t="shared" si="22"/>
-        <v>1304</v>
+        <v>1308</v>
       </c>
       <c r="B1458" s="29">
         <v>87</v>
@@ -54287,7 +54309,7 @@
     <row r="1459" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1459" s="1">
         <f t="shared" si="22"/>
-        <v>1305</v>
+        <v>1309</v>
       </c>
       <c r="B1459" s="29">
         <v>87</v>
@@ -54325,7 +54347,7 @@
     <row r="1460" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1460" s="1">
         <f t="shared" si="22"/>
-        <v>1306</v>
+        <v>1310</v>
       </c>
       <c r="B1460" s="29">
         <v>87</v>
@@ -54363,7 +54385,7 @@
     <row r="1461" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1461" s="1">
         <f t="shared" si="22"/>
-        <v>1307</v>
+        <v>1311</v>
       </c>
       <c r="B1461" s="29">
         <v>87</v>
@@ -54399,7 +54421,7 @@
     <row r="1462" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1462" s="1">
         <f t="shared" si="22"/>
-        <v>1307</v>
+        <v>1311</v>
       </c>
       <c r="B1462" s="29">
         <v>87</v>
@@ -54431,7 +54453,7 @@
     <row r="1463" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1463" s="1">
         <f t="shared" si="22"/>
-        <v>1308</v>
+        <v>1312</v>
       </c>
       <c r="B1463" s="29">
         <v>87</v>
@@ -54463,7 +54485,7 @@
     <row r="1464" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1464" s="1">
         <f t="shared" si="22"/>
-        <v>1309</v>
+        <v>1313</v>
       </c>
       <c r="B1464" s="29">
         <v>87</v>
@@ -54499,7 +54521,7 @@
     <row r="1465" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1465" s="1">
         <f t="shared" si="22"/>
-        <v>1310</v>
+        <v>1314</v>
       </c>
       <c r="B1465" s="29">
         <v>87</v>
@@ -54539,7 +54561,7 @@
     <row r="1466" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1466" s="1">
         <f t="shared" si="22"/>
-        <v>1310</v>
+        <v>1314</v>
       </c>
       <c r="B1466" s="29">
         <v>87</v>
@@ -54569,7 +54591,7 @@
     <row r="1467" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1467" s="1">
         <f t="shared" si="22"/>
-        <v>1311</v>
+        <v>1315</v>
       </c>
       <c r="B1467" s="29">
         <v>87</v>
@@ -54611,7 +54633,7 @@
     <row r="1468" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1468" s="1">
         <f t="shared" si="22"/>
-        <v>1312</v>
+        <v>1316</v>
       </c>
       <c r="B1468" s="29">
         <v>87</v>
@@ -54645,7 +54667,7 @@
     <row r="1469" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1469" s="1">
         <f t="shared" si="22"/>
-        <v>1312</v>
+        <v>1316</v>
       </c>
       <c r="B1469" s="29">
         <v>87</v>
@@ -54675,7 +54697,7 @@
     <row r="1470" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1470" s="1">
         <f t="shared" si="22"/>
-        <v>1313</v>
+        <v>1317</v>
       </c>
       <c r="B1470" s="29">
         <v>87</v>
@@ -54711,7 +54733,7 @@
     <row r="1471" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1471" s="1">
         <f t="shared" si="22"/>
-        <v>1314</v>
+        <v>1318</v>
       </c>
       <c r="B1471" s="29">
         <v>88</v>
@@ -54743,7 +54765,7 @@
     <row r="1472" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1472" s="1">
         <f t="shared" si="22"/>
-        <v>1315</v>
+        <v>1319</v>
       </c>
       <c r="B1472" s="29">
         <v>88</v>
@@ -54781,7 +54803,7 @@
     <row r="1473" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1473" s="1">
         <f t="shared" si="22"/>
-        <v>1315</v>
+        <v>1319</v>
       </c>
       <c r="B1473" s="29">
         <v>88</v>
@@ -54815,7 +54837,7 @@
     <row r="1474" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1474" s="1">
         <f t="shared" si="22"/>
-        <v>1316</v>
+        <v>1320</v>
       </c>
       <c r="B1474" s="29">
         <v>88</v>
@@ -54849,7 +54871,7 @@
     <row r="1475" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1475" s="1">
         <f t="shared" si="22"/>
-        <v>1317</v>
+        <v>1321</v>
       </c>
       <c r="B1475" s="29">
         <v>88</v>
@@ -54881,7 +54903,7 @@
     <row r="1476" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1476" s="1">
         <f t="shared" si="22"/>
-        <v>1318</v>
+        <v>1322</v>
       </c>
       <c r="B1476" s="29">
         <v>88</v>
@@ -54917,7 +54939,7 @@
     <row r="1477" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1477" s="1">
         <f t="shared" si="22"/>
-        <v>1319</v>
+        <v>1323</v>
       </c>
       <c r="B1477" s="29">
         <v>88</v>
@@ -54955,7 +54977,7 @@
     <row r="1478" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1478" s="1">
         <f t="shared" si="22"/>
-        <v>1319</v>
+        <v>1324</v>
       </c>
       <c r="B1478" s="29">
         <v>88</v>
@@ -54965,7 +54987,9 @@
       <c r="E1478" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="F1478" s="30"/>
+      <c r="F1478" s="35" t="s">
+        <v>186</v>
+      </c>
       <c r="G1478" s="30"/>
       <c r="H1478" s="30"/>
       <c r="I1478" s="30"/>
@@ -54991,7 +55015,7 @@
     <row r="1479" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1479" s="1">
         <f t="shared" si="22"/>
-        <v>1320</v>
+        <v>1325</v>
       </c>
       <c r="B1479" s="29">
         <v>88</v>
@@ -55023,7 +55047,7 @@
     <row r="1480" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1480" s="1">
         <f t="shared" si="22"/>
-        <v>1320</v>
+        <v>1326</v>
       </c>
       <c r="B1480" s="29">
         <v>89</v>
@@ -55033,7 +55057,9 @@
       <c r="E1480" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F1480" s="30"/>
+      <c r="F1480" s="35" t="s">
+        <v>187</v>
+      </c>
       <c r="G1480" s="30"/>
       <c r="H1480" s="30"/>
       <c r="I1480" s="30"/>
@@ -55055,7 +55081,7 @@
     <row r="1481" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1481" s="1">
         <f t="shared" si="22"/>
-        <v>1321</v>
+        <v>1327</v>
       </c>
       <c r="B1481" s="29">
         <v>89</v>
@@ -55087,7 +55113,7 @@
     <row r="1482" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1482" s="1">
         <f t="shared" si="22"/>
-        <v>1322</v>
+        <v>1328</v>
       </c>
       <c r="B1482" s="29">
         <v>89</v>
@@ -55121,7 +55147,7 @@
     <row r="1483" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1483" s="1">
         <f t="shared" si="22"/>
-        <v>1323</v>
+        <v>1329</v>
       </c>
       <c r="B1483" s="29">
         <v>89</v>
@@ -55159,7 +55185,7 @@
     <row r="1484" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1484" s="1">
         <f t="shared" si="22"/>
-        <v>1324</v>
+        <v>1330</v>
       </c>
       <c r="B1484" s="29">
         <v>89</v>
@@ -55195,7 +55221,7 @@
     <row r="1485" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1485" s="1">
         <f t="shared" si="22"/>
-        <v>1325</v>
+        <v>1331</v>
       </c>
       <c r="B1485" s="29">
         <v>89</v>
@@ -55231,7 +55257,7 @@
     <row r="1486" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1486" s="1">
         <f t="shared" si="22"/>
-        <v>1326</v>
+        <v>1332</v>
       </c>
       <c r="B1486" s="29">
         <v>89</v>
@@ -55267,7 +55293,7 @@
     <row r="1487" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1487" s="1">
         <f t="shared" si="22"/>
-        <v>1327</v>
+        <v>1333</v>
       </c>
       <c r="B1487" s="29">
         <v>89</v>
@@ -55303,7 +55329,7 @@
     <row r="1488" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1488" s="1">
         <f t="shared" si="22"/>
-        <v>1327</v>
+        <v>1333</v>
       </c>
       <c r="B1488" s="29">
         <v>89</v>
@@ -55335,7 +55361,7 @@
     <row r="1489" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1489" s="1">
         <f t="shared" si="22"/>
-        <v>1328</v>
+        <v>1334</v>
       </c>
       <c r="B1489" s="29">
         <v>89</v>
@@ -55371,7 +55397,7 @@
     <row r="1490" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1490" s="1">
         <f t="shared" si="22"/>
-        <v>1329</v>
+        <v>1335</v>
       </c>
       <c r="B1490" s="29">
         <v>89</v>
@@ -55403,7 +55429,7 @@
     <row r="1491" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1491" s="1">
         <f t="shared" si="22"/>
-        <v>1330</v>
+        <v>1336</v>
       </c>
       <c r="B1491" s="29">
         <v>89</v>
@@ -55435,7 +55461,7 @@
     <row r="1492" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1492" s="1">
         <f t="shared" si="22"/>
-        <v>1331</v>
+        <v>1337</v>
       </c>
       <c r="B1492" s="29">
         <v>89</v>
@@ -55471,7 +55497,7 @@
     <row r="1493" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1493" s="1">
         <f t="shared" si="22"/>
-        <v>1332</v>
+        <v>1338</v>
       </c>
       <c r="B1493" s="29">
         <v>89</v>
@@ -55507,7 +55533,7 @@
     <row r="1494" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1494" s="1">
         <f t="shared" si="22"/>
-        <v>1333</v>
+        <v>1339</v>
       </c>
       <c r="B1494" s="29">
         <v>89</v>
@@ -55543,7 +55569,7 @@
     <row r="1495" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1495" s="1">
         <f t="shared" si="22"/>
-        <v>1334</v>
+        <v>1340</v>
       </c>
       <c r="B1495" s="29">
         <v>89</v>
@@ -55585,7 +55611,7 @@
     <row r="1496" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1496" s="1">
         <f t="shared" si="22"/>
-        <v>1335</v>
+        <v>1341</v>
       </c>
       <c r="B1496" s="29">
         <v>89</v>
@@ -55615,7 +55641,7 @@
     <row r="1497" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1497" s="1">
         <f t="shared" si="22"/>
-        <v>1336</v>
+        <v>1342</v>
       </c>
       <c r="B1497" s="29">
         <v>90</v>
@@ -55649,7 +55675,7 @@
     <row r="1498" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1498" s="1">
         <f t="shared" si="22"/>
-        <v>1337</v>
+        <v>1343</v>
       </c>
       <c r="B1498" s="29">
         <v>90</v>
@@ -55683,7 +55709,7 @@
     <row r="1499" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1499" s="1">
         <f t="shared" si="22"/>
-        <v>1338</v>
+        <v>1344</v>
       </c>
       <c r="B1499" s="29">
         <v>90</v>
@@ -55713,7 +55739,7 @@
     <row r="1500" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1500" s="1">
         <f t="shared" si="22"/>
-        <v>1339</v>
+        <v>1345</v>
       </c>
       <c r="B1500" s="29">
         <v>90</v>
@@ -55749,7 +55775,7 @@
     <row r="1501" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1501" s="1">
         <f t="shared" si="22"/>
-        <v>1340</v>
+        <v>1346</v>
       </c>
       <c r="B1501" s="29">
         <v>90</v>
@@ -55785,7 +55811,7 @@
     <row r="1502" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1502" s="1">
         <f t="shared" si="22"/>
-        <v>1341</v>
+        <v>1347</v>
       </c>
       <c r="B1502" s="29">
         <v>90</v>
@@ -55821,7 +55847,7 @@
     <row r="1503" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1503" s="1">
         <f t="shared" ref="A1503:A1544" si="23">IF(OR(F1503="",F1503=""),A1502,A1502+1)</f>
-        <v>1342</v>
+        <v>1348</v>
       </c>
       <c r="B1503" s="29">
         <v>90</v>
@@ -55857,7 +55883,7 @@
     <row r="1504" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1504" s="1">
         <f t="shared" si="23"/>
-        <v>1343</v>
+        <v>1349</v>
       </c>
       <c r="B1504" s="29">
         <v>90</v>
@@ -55893,7 +55919,7 @@
     <row r="1505" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1505" s="1">
         <f t="shared" si="23"/>
-        <v>1343</v>
+        <v>1350</v>
       </c>
       <c r="B1505" s="29">
         <v>90</v>
@@ -55903,7 +55929,9 @@
       <c r="E1505" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="F1505" s="30"/>
+      <c r="F1505" s="35" t="s">
+        <v>186</v>
+      </c>
       <c r="G1505" s="30"/>
       <c r="H1505" s="30"/>
       <c r="I1505" s="30"/>
@@ -55929,7 +55957,7 @@
     <row r="1506" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1506" s="1">
         <f t="shared" si="23"/>
-        <v>1343</v>
+        <v>1350</v>
       </c>
       <c r="B1506" s="29">
         <v>90</v>
@@ -55959,7 +55987,7 @@
     <row r="1507" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1507" s="1">
         <f t="shared" si="23"/>
-        <v>1344</v>
+        <v>1351</v>
       </c>
       <c r="B1507" s="29" t="s">
         <v>180</v>
@@ -55993,7 +56021,7 @@
     <row r="1508" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1508" s="1">
         <f t="shared" si="23"/>
-        <v>1345</v>
+        <v>1352</v>
       </c>
       <c r="B1508" s="29" t="s">
         <v>180</v>
@@ -56031,7 +56059,7 @@
     <row r="1509" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1509" s="1">
         <f t="shared" si="23"/>
-        <v>1345</v>
+        <v>1352</v>
       </c>
       <c r="B1509" s="29" t="s">
         <v>180</v>
@@ -56063,7 +56091,7 @@
     <row r="1510" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1510" s="1">
         <f t="shared" si="23"/>
-        <v>1346</v>
+        <v>1353</v>
       </c>
       <c r="B1510" s="29" t="s">
         <v>180</v>
@@ -56097,7 +56125,7 @@
     <row r="1511" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1511" s="1">
         <f t="shared" si="23"/>
-        <v>1347</v>
+        <v>1354</v>
       </c>
       <c r="B1511" s="29" t="s">
         <v>180</v>
@@ -56133,7 +56161,7 @@
     <row r="1512" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1512" s="1">
         <f t="shared" si="23"/>
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="B1512" s="29" t="s">
         <v>180</v>
@@ -56171,7 +56199,7 @@
     <row r="1513" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1513" s="1">
         <f t="shared" si="23"/>
-        <v>1348</v>
+        <v>1355</v>
       </c>
       <c r="B1513" s="29" t="s">
         <v>180</v>
@@ -56203,7 +56231,7 @@
     <row r="1514" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1514" s="1">
         <f t="shared" si="23"/>
-        <v>1349</v>
+        <v>1356</v>
       </c>
       <c r="B1514" s="29" t="s">
         <v>181</v>
@@ -56237,7 +56265,7 @@
     <row r="1515" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1515" s="1">
         <f t="shared" si="23"/>
-        <v>1349</v>
+        <v>1357</v>
       </c>
       <c r="B1515" s="29" t="s">
         <v>181</v>
@@ -56247,7 +56275,9 @@
       <c r="E1515" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="F1515" s="30"/>
+      <c r="F1515" s="35" t="s">
+        <v>187</v>
+      </c>
       <c r="G1515" s="30"/>
       <c r="H1515" s="30"/>
       <c r="I1515" s="30"/>
@@ -56273,7 +56303,7 @@
     <row r="1516" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1516" s="1">
         <f t="shared" si="23"/>
-        <v>1350</v>
+        <v>1358</v>
       </c>
       <c r="B1516" s="29" t="s">
         <v>181</v>
@@ -56303,7 +56333,7 @@
     <row r="1517" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1517" s="1">
         <f t="shared" si="23"/>
-        <v>1351</v>
+        <v>1359</v>
       </c>
       <c r="B1517" s="29" t="s">
         <v>181</v>
@@ -56335,7 +56365,7 @@
     <row r="1518" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1518" s="1">
         <f t="shared" si="23"/>
-        <v>1352</v>
+        <v>1360</v>
       </c>
       <c r="B1518" s="29" t="s">
         <v>182</v>
@@ -56373,7 +56403,7 @@
     <row r="1519" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1519" s="1">
         <f t="shared" si="23"/>
-        <v>1353</v>
+        <v>1361</v>
       </c>
       <c r="B1519" s="29" t="s">
         <v>182</v>
@@ -56405,7 +56435,7 @@
     <row r="1520" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1520" s="1">
         <f t="shared" si="23"/>
-        <v>1354</v>
+        <v>1362</v>
       </c>
       <c r="B1520" s="29" t="s">
         <v>182</v>
@@ -56437,7 +56467,7 @@
     <row r="1521" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1521" s="1">
         <f t="shared" si="23"/>
-        <v>1355</v>
+        <v>1363</v>
       </c>
       <c r="B1521" s="29" t="s">
         <v>182</v>
@@ -56473,7 +56503,7 @@
     <row r="1522" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1522" s="1">
         <f t="shared" si="23"/>
-        <v>1356</v>
+        <v>1364</v>
       </c>
       <c r="B1522" s="29" t="s">
         <v>182</v>
@@ -56505,7 +56535,7 @@
     <row r="1523" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1523" s="1">
         <f t="shared" si="23"/>
-        <v>1357</v>
+        <v>1365</v>
       </c>
       <c r="B1523" s="29" t="s">
         <v>182</v>
@@ -56547,7 +56577,7 @@
     <row r="1524" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1524" s="1">
         <f t="shared" si="23"/>
-        <v>1358</v>
+        <v>1366</v>
       </c>
       <c r="B1524" s="29" t="s">
         <v>182</v>
@@ -56581,7 +56611,7 @@
     <row r="1525" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1525" s="1">
         <f t="shared" si="23"/>
-        <v>1358</v>
+        <v>1366</v>
       </c>
       <c r="B1525" s="29" t="s">
         <v>182</v>
@@ -56611,7 +56641,7 @@
     <row r="1526" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1526" s="1">
         <f t="shared" si="23"/>
-        <v>1359</v>
+        <v>1367</v>
       </c>
       <c r="B1526" s="29" t="s">
         <v>182</v>
@@ -56641,7 +56671,7 @@
     <row r="1527" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1527" s="1">
         <f t="shared" si="23"/>
-        <v>1360</v>
+        <v>1368</v>
       </c>
       <c r="B1527" s="29" t="s">
         <v>182</v>
@@ -56675,7 +56705,7 @@
     <row r="1528" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1528" s="1">
         <f t="shared" si="23"/>
-        <v>1361</v>
+        <v>1369</v>
       </c>
       <c r="B1528" s="29" t="s">
         <v>182</v>
@@ -56713,7 +56743,7 @@
     <row r="1529" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1529" s="1">
         <f t="shared" si="23"/>
-        <v>1362</v>
+        <v>1370</v>
       </c>
       <c r="B1529" s="29" t="s">
         <v>182</v>
@@ -56749,7 +56779,7 @@
     <row r="1530" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1530" s="1">
         <f t="shared" si="23"/>
-        <v>1363</v>
+        <v>1371</v>
       </c>
       <c r="B1530" s="29" t="s">
         <v>183</v>
@@ -56781,7 +56811,7 @@
     <row r="1531" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1531" s="1">
         <f t="shared" si="23"/>
-        <v>1364</v>
+        <v>1372</v>
       </c>
       <c r="B1531" s="29" t="s">
         <v>183</v>
@@ -56819,7 +56849,7 @@
     <row r="1532" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1532" s="1">
         <f t="shared" si="23"/>
-        <v>1365</v>
+        <v>1373</v>
       </c>
       <c r="B1532" s="29" t="s">
         <v>183</v>
@@ -56851,7 +56881,7 @@
     <row r="1533" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1533" s="1">
         <f t="shared" si="23"/>
-        <v>1366</v>
+        <v>1374</v>
       </c>
       <c r="B1533" s="29" t="s">
         <v>183</v>
@@ -56887,7 +56917,7 @@
     <row r="1534" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1534" s="1">
         <f t="shared" si="23"/>
-        <v>1367</v>
+        <v>1375</v>
       </c>
       <c r="B1534" s="29" t="s">
         <v>183</v>
@@ -56919,7 +56949,7 @@
     <row r="1535" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1535" s="1">
         <f t="shared" si="23"/>
-        <v>1368</v>
+        <v>1376</v>
       </c>
       <c r="B1535" s="29" t="s">
         <v>183</v>
@@ -56953,7 +56983,7 @@
     <row r="1536" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1536" s="1">
         <f t="shared" si="23"/>
-        <v>1369</v>
+        <v>1377</v>
       </c>
       <c r="B1536" s="29" t="s">
         <v>183</v>
@@ -56987,7 +57017,7 @@
     <row r="1537" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1537" s="1">
         <f t="shared" si="23"/>
-        <v>1370</v>
+        <v>1378</v>
       </c>
       <c r="B1537" s="29" t="s">
         <v>183</v>
@@ -57023,7 +57053,7 @@
     <row r="1538" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1538" s="1">
         <f t="shared" si="23"/>
-        <v>1371</v>
+        <v>1379</v>
       </c>
       <c r="B1538" s="29" t="s">
         <v>183</v>
@@ -57055,7 +57085,7 @@
     <row r="1539" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1539" s="1">
         <f t="shared" si="23"/>
-        <v>1372</v>
+        <v>1380</v>
       </c>
       <c r="B1539" s="29" t="s">
         <v>183</v>
@@ -57089,7 +57119,7 @@
     <row r="1540" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1540" s="1">
         <f t="shared" si="23"/>
-        <v>1373</v>
+        <v>1381</v>
       </c>
       <c r="B1540" s="29" t="s">
         <v>184</v>
@@ -57123,7 +57153,7 @@
     <row r="1541" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1541" s="1">
         <f t="shared" si="23"/>
-        <v>1374</v>
+        <v>1382</v>
       </c>
       <c r="B1541" s="29" t="s">
         <v>184</v>
@@ -57159,7 +57189,7 @@
     <row r="1542" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1542" s="1">
         <f t="shared" si="23"/>
-        <v>1375</v>
+        <v>1383</v>
       </c>
       <c r="B1542" s="29" t="s">
         <v>184</v>
@@ -57191,7 +57221,7 @@
     <row r="1543" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1543" s="1">
         <f t="shared" si="23"/>
-        <v>1376</v>
+        <v>1384</v>
       </c>
       <c r="B1543" s="29" t="s">
         <v>184</v>
@@ -57223,7 +57253,7 @@
     <row r="1544" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1544" s="1">
         <f t="shared" si="23"/>
-        <v>1377</v>
+        <v>1385</v>
       </c>
       <c r="B1544" s="29" t="s">
         <v>184</v>

</xml_diff>